<commit_message>
Refactor: Optimize Data Handling
Enhanced code readability through refactoring.
Removed HTML generation.
Unified API calls for data consistency.
Implemented robust error handling.
Clarified and documented methods.
Revamped Excel data parsing.
</commit_message>
<xml_diff>
--- a/Leaderboards/CurrentCMRITLeaderboard2025.xlsx
+++ b/Leaderboards/CurrentCMRITLeaderboard2025.xlsx
@@ -6,13 +6,13 @@
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Current CodeRankingLeaderboard" r:id="rId3" sheetId="1"/>
+    <sheet name="Current CMRITLeaderboard2025" r:id="rId3" sheetId="1"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="68">
   <si>
     <t>Rank</t>
   </si>
@@ -47,127 +47,175 @@
     <t>Codechef_Rating</t>
   </si>
   <si>
+    <t>HackerRank_Handle</t>
+  </si>
+  <si>
+    <t>HackerRank_Practice_Score</t>
+  </si>
+  <si>
     <t>Percentile</t>
   </si>
   <si>
-    <t>21r01a0513</t>
-  </si>
-  <si>
-    <t>cmrit_21r01a0513</t>
-  </si>
-  <si>
-    <t>vishwatej4</t>
-  </si>
-  <si>
-    <t>92.61%</t>
-  </si>
-  <si>
-    <t>21r01a67f2</t>
-  </si>
-  <si>
-    <t>cmrit25_21r01a67f2</t>
-  </si>
-  <si>
-    <t>sribro123</t>
-  </si>
-  <si>
-    <t>73.62%</t>
-  </si>
-  <si>
-    <t>21r01a05c0</t>
-  </si>
-  <si>
-    <t>cmrit25_21r01a05c0</t>
-  </si>
-  <si>
-    <t>tanirukavyasri</t>
-  </si>
-  <si>
-    <t>67.87%</t>
-  </si>
-  <si>
-    <t>21r01a7238</t>
-  </si>
-  <si>
-    <t>cmrit25_21r01a7238</t>
-  </si>
-  <si>
-    <t>kjcreddy666</t>
-  </si>
-  <si>
-    <t>jai_21r01a7238</t>
-  </si>
-  <si>
-    <t>63.85%</t>
-  </si>
-  <si>
-    <t>21r01a05h2</t>
-  </si>
-  <si>
-    <t>cmrit25_21r01a05h2</t>
-  </si>
-  <si>
-    <t>21r01aymik</t>
-  </si>
-  <si>
-    <t>cmr_21r01a05h2</t>
-  </si>
-  <si>
-    <t>62.17%</t>
-  </si>
-  <si>
-    <t>21r01a0548</t>
-  </si>
-  <si>
-    <t>cmrit25_21r01a0548</t>
-  </si>
-  <si>
-    <t>varshitha613</t>
-  </si>
-  <si>
-    <t>varshitha_77</t>
-  </si>
-  <si>
-    <t>61.12%</t>
-  </si>
-  <si>
-    <t>21r01a0561</t>
-  </si>
-  <si>
-    <t>pavanvasam577</t>
-  </si>
-  <si>
-    <t>60.79%</t>
-  </si>
-  <si>
-    <t>21r01a6764</t>
-  </si>
-  <si>
-    <t>cmrit25_21r01a6764</t>
-  </si>
-  <si>
-    <t>vyshnavi6764</t>
-  </si>
-  <si>
-    <t>44.47%</t>
-  </si>
-  <si>
-    <t>21r01a6758</t>
-  </si>
-  <si>
-    <t>nandhu2304</t>
-  </si>
-  <si>
-    <t>29.23%</t>
-  </si>
-  <si>
-    <t>22r05a6702</t>
-  </si>
-  <si>
-    <t>praneeth702</t>
-  </si>
-  <si>
-    <t>24.49%</t>
+    <t>21r01a7210</t>
+  </si>
+  <si>
+    <t>cmrit25_21r01a7210</t>
+  </si>
+  <si>
+    <t>pavan_10</t>
+  </si>
+  <si>
+    <t>pavan_7210</t>
+  </si>
+  <si>
+    <t>sololeveler_10</t>
+  </si>
+  <si>
+    <t>21r01a7210_pavan</t>
+  </si>
+  <si>
+    <t>94.09%</t>
+  </si>
+  <si>
+    <t>21r01a7209</t>
+  </si>
+  <si>
+    <t>sindhu_21r01a7209</t>
+  </si>
+  <si>
+    <t>sindhuja_9849</t>
+  </si>
+  <si>
+    <t>74.64%</t>
+  </si>
+  <si>
+    <t>21r01a7207</t>
+  </si>
+  <si>
+    <t>cmrit25_21r01a7207</t>
+  </si>
+  <si>
+    <t>a2101a7207</t>
+  </si>
+  <si>
+    <t>42.85%</t>
+  </si>
+  <si>
+    <t>21r01a7214</t>
+  </si>
+  <si>
+    <t>cmrit25_21r01a7214</t>
+  </si>
+  <si>
+    <t>harshinibachu</t>
+  </si>
+  <si>
+    <t>bachuharshini</t>
+  </si>
+  <si>
+    <t>37.63%</t>
+  </si>
+  <si>
+    <t>21r01a7223</t>
+  </si>
+  <si>
+    <t>cmrit25_21r01a7223</t>
+  </si>
+  <si>
+    <t>21r01aewni</t>
+  </si>
+  <si>
+    <t>charishna</t>
+  </si>
+  <si>
+    <t>23.54%</t>
+  </si>
+  <si>
+    <t>21r01a7203</t>
+  </si>
+  <si>
+    <t>cmr21r01a7203</t>
+  </si>
+  <si>
+    <t>18.93%</t>
+  </si>
+  <si>
+    <t>21r01a7224</t>
+  </si>
+  <si>
+    <t>cmrit25_21r01a7224</t>
+  </si>
+  <si>
+    <t>21r01arg58</t>
+  </si>
+  <si>
+    <t>nikitha7224</t>
+  </si>
+  <si>
+    <t>18.55%</t>
+  </si>
+  <si>
+    <t>21r01a7225</t>
+  </si>
+  <si>
+    <t>anonymou99wv</t>
+  </si>
+  <si>
+    <t>anilgoud</t>
+  </si>
+  <si>
+    <t>anil66</t>
+  </si>
+  <si>
+    <t>13.25%</t>
+  </si>
+  <si>
+    <t>21r01a7201</t>
+  </si>
+  <si>
+    <t>cmrit25_21r01a7201</t>
+  </si>
+  <si>
+    <t>aharshitha_31</t>
+  </si>
+  <si>
+    <t>11.95%</t>
+  </si>
+  <si>
+    <t>21r01a7222</t>
+  </si>
+  <si>
+    <t>cmrit25_21r01a7222</t>
+  </si>
+  <si>
+    <t>mounikad25</t>
+  </si>
+  <si>
+    <t>dmounika_22</t>
+  </si>
+  <si>
+    <t>10.31%</t>
+  </si>
+  <si>
+    <t>21r01a7206</t>
+  </si>
+  <si>
+    <t>p21r01a7206</t>
+  </si>
+  <si>
+    <t>10%</t>
+  </si>
+  <si>
+    <t>21r01a7220</t>
+  </si>
+  <si>
+    <t>cmrit25_21r01a7220</t>
+  </si>
+  <si>
+    <t>cmr_21r01a7220</t>
+  </si>
+  <si>
+    <t>8.7%</t>
   </si>
 </sst>
 </file>
@@ -266,14 +314,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:L11"/>
+  <dimension ref="A1:N13"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
     <col min="1" max="1" width="10.2109375" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="15.15625" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="15.07421875" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="34.24609375" customWidth="true" bestFit="true"/>
     <col min="4" max="4" width="33.09765625" customWidth="true" bestFit="true"/>
     <col min="5" max="5" width="22.62890625" customWidth="true" bestFit="true"/>
@@ -283,7 +331,9 @@
     <col min="9" max="9" width="29.63671875" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="31.22265625" customWidth="true" bestFit="true"/>
     <col min="11" max="11" width="30.07421875" customWidth="true" bestFit="true"/>
-    <col min="12" max="12" width="18.6796875" customWidth="true" bestFit="true"/>
+    <col min="12" max="12" width="35.515625" customWidth="true" bestFit="true"/>
+    <col min="13" max="13" width="48.12890625" customWidth="true" bestFit="true"/>
+    <col min="14" max="14" width="18.6796875" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -323,43 +373,55 @@
       <c r="L1" t="s" s="1">
         <v>11</v>
       </c>
+      <c r="M1" t="s" s="1">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s" s="1">
+        <v>13</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n" s="2">
         <v>1.0</v>
       </c>
       <c r="B2" t="s" s="2">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C2" t="s" s="2">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D2" t="n" s="2">
-        <v>867.0</v>
+        <v>834.0</v>
       </c>
       <c r="E2" t="s" s="2">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="F2" t="n" s="2">
-        <v>433.0</v>
+        <v>63.0</v>
       </c>
       <c r="G2" t="n" s="2">
-        <v>151.0</v>
+        <v>5.0</v>
       </c>
       <c r="H2" t="s" s="2">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="I2" t="n" s="2">
-        <v>1529.0</v>
+        <v>1408.0</v>
       </c>
       <c r="J2" t="s" s="2">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="K2" t="n" s="2">
-        <v>1434.0</v>
+        <v>1302.0</v>
       </c>
       <c r="L2" t="s" s="2">
-        <v>15</v>
+        <v>19</v>
+      </c>
+      <c r="M2" t="n" s="2">
+        <v>188.0</v>
+      </c>
+      <c r="N2" t="s" s="2">
+        <v>20</v>
       </c>
     </row>
     <row r="3">
@@ -367,37 +429,43 @@
         <v>2.0</v>
       </c>
       <c r="B3" t="s" s="2">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="C3" t="s" s="2">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="D3" t="n" s="2">
-        <v>832.0</v>
+        <v>761.0</v>
       </c>
       <c r="E3" t="s" s="2">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="F3" t="n" s="2">
-        <v>311.0</v>
+        <v>20.0</v>
       </c>
       <c r="G3" t="n" s="2">
-        <v>0.0</v>
+        <v>11.0</v>
       </c>
       <c r="H3" t="s" s="2">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="I3" t="n" s="2">
-        <v>1580.0</v>
+        <v>1331.0</v>
       </c>
       <c r="J3" t="s" s="2">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="K3" t="n" s="2">
-        <v>1427.0</v>
+        <v>1079.0</v>
       </c>
       <c r="L3" t="s" s="2">
-        <v>19</v>
+        <v>21</v>
+      </c>
+      <c r="M3" t="n" s="2">
+        <v>197.0</v>
+      </c>
+      <c r="N3" t="s" s="2">
+        <v>24</v>
       </c>
     </row>
     <row r="4">
@@ -405,37 +473,43 @@
         <v>3.0</v>
       </c>
       <c r="B4" t="s" s="2">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="C4" t="s" s="2">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="D4" t="n" s="2">
-        <v>521.0</v>
+        <v>749.0</v>
       </c>
       <c r="E4" t="s" s="2">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="F4" t="n" s="2">
-        <v>319.0</v>
+        <v>0.0</v>
       </c>
       <c r="G4" t="n" s="2">
-        <v>104.0</v>
+        <v>1.0</v>
       </c>
       <c r="H4" t="s" s="2">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="I4" t="n" s="2">
-        <v>1404.0</v>
+        <v>0.0</v>
       </c>
       <c r="J4" t="s" s="2">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="K4" t="n" s="2">
-        <v>1305.0</v>
+        <v>1113.0</v>
       </c>
       <c r="L4" t="s" s="2">
-        <v>23</v>
+        <v>25</v>
+      </c>
+      <c r="M4" t="n" s="2">
+        <v>127.0</v>
+      </c>
+      <c r="N4" t="s" s="2">
+        <v>28</v>
       </c>
     </row>
     <row r="5">
@@ -443,37 +517,43 @@
         <v>4.0</v>
       </c>
       <c r="B5" t="s" s="2">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="C5" t="s" s="2">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="D5" t="n" s="2">
-        <v>1013.0</v>
+        <v>757.0</v>
       </c>
       <c r="E5" t="s" s="2">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="F5" t="n" s="2">
-        <v>62.0</v>
+        <v>0.0</v>
       </c>
       <c r="G5" t="n" s="2">
-        <v>13.0</v>
+        <v>0.0</v>
       </c>
       <c r="H5" t="s" s="2">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="I5" t="n" s="2">
-        <v>1455.0</v>
+        <v>0.0</v>
       </c>
       <c r="J5" t="s" s="2">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="K5" t="n" s="2">
-        <v>1602.0</v>
+        <v>1123.0</v>
       </c>
       <c r="L5" t="s" s="2">
-        <v>28</v>
+        <v>29</v>
+      </c>
+      <c r="M5" t="n" s="2">
+        <v>35.0</v>
+      </c>
+      <c r="N5" t="s" s="2">
+        <v>33</v>
       </c>
     </row>
     <row r="6">
@@ -481,37 +561,43 @@
         <v>5.0</v>
       </c>
       <c r="B6" t="s" s="2">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="C6" t="s" s="2">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="D6" t="n" s="2">
-        <v>821.0</v>
+        <v>355.0</v>
       </c>
       <c r="E6" t="s" s="2">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="F6" t="n" s="2">
-        <v>169.0</v>
+        <v>0.0</v>
       </c>
       <c r="G6" t="n" s="2">
-        <v>2.0</v>
+        <v>0.0</v>
       </c>
       <c r="H6" t="s" s="2">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="I6" t="n" s="2">
-        <v>1423.0</v>
+        <v>0.0</v>
       </c>
       <c r="J6" t="s" s="2">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="K6" t="n" s="2">
-        <v>1405.0</v>
+        <v>1125.0</v>
       </c>
       <c r="L6" t="s" s="2">
-        <v>33</v>
+        <v>34</v>
+      </c>
+      <c r="M6" t="n" s="2">
+        <v>42.0</v>
+      </c>
+      <c r="N6" t="s" s="2">
+        <v>38</v>
       </c>
     </row>
     <row r="7">
@@ -519,37 +605,43 @@
         <v>6.0</v>
       </c>
       <c r="B7" t="s" s="2">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="C7" t="s" s="2">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="D7" t="n" s="2">
-        <v>881.0</v>
+        <v>0.0</v>
       </c>
       <c r="E7" t="s" s="2">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="F7" t="n" s="2">
-        <v>69.0</v>
+        <v>0.0</v>
       </c>
       <c r="G7" t="n" s="2">
-        <v>58.0</v>
+        <v>0.0</v>
       </c>
       <c r="H7" t="s" s="2">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="I7" t="n" s="2">
-        <v>1427.0</v>
+        <v>1408.0</v>
       </c>
       <c r="J7" t="s" s="2">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="K7" t="n" s="2">
-        <v>1385.0</v>
+        <v>1031.0</v>
       </c>
       <c r="L7" t="s" s="2">
-        <v>38</v>
+        <v>39</v>
+      </c>
+      <c r="M7" t="n" s="2">
+        <v>20.0</v>
+      </c>
+      <c r="N7" t="s" s="2">
+        <v>41</v>
       </c>
     </row>
     <row r="8">
@@ -557,35 +649,43 @@
         <v>7.0</v>
       </c>
       <c r="B8" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="C8" s="2"/>
+        <v>42</v>
+      </c>
+      <c r="C8" t="s" s="2">
+        <v>43</v>
+      </c>
       <c r="D8" t="n" s="2">
         <v>0.0</v>
       </c>
       <c r="E8" t="s" s="2">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="F8" t="n" s="2">
-        <v>445.0</v>
+        <v>20.0</v>
       </c>
       <c r="G8" t="n" s="2">
-        <v>113.0</v>
+        <v>0.0</v>
       </c>
       <c r="H8" t="s" s="2">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="I8" t="n" s="2">
-        <v>1521.0</v>
+        <v>0.0</v>
       </c>
       <c r="J8" t="s" s="2">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="K8" t="n" s="2">
-        <v>1421.0</v>
+        <v>1010.0</v>
       </c>
       <c r="L8" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
+      </c>
+      <c r="M8" t="n" s="2">
+        <v>25.0</v>
+      </c>
+      <c r="N8" t="s" s="2">
+        <v>46</v>
       </c>
     </row>
     <row r="9">
@@ -593,37 +693,43 @@
         <v>8.0</v>
       </c>
       <c r="B9" t="s" s="2">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="C9" t="s" s="2">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="D9" t="n" s="2">
-        <v>832.0</v>
+        <v>0.0</v>
       </c>
       <c r="E9" t="s" s="2">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="F9" t="n" s="2">
         <v>0.0</v>
       </c>
       <c r="G9" t="n" s="2">
-        <v>100.0</v>
+        <v>0.0</v>
       </c>
       <c r="H9" t="s" s="2">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="I9" t="n" s="2">
         <v>0.0</v>
       </c>
       <c r="J9" t="s" s="2">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="K9" t="n" s="2">
-        <v>1458.0</v>
+        <v>991.0</v>
       </c>
       <c r="L9" t="s" s="2">
-        <v>45</v>
+        <v>47</v>
+      </c>
+      <c r="M9" t="n" s="2">
+        <v>111.0</v>
+      </c>
+      <c r="N9" t="s" s="2">
+        <v>51</v>
       </c>
     </row>
     <row r="10">
@@ -631,35 +737,43 @@
         <v>9.0</v>
       </c>
       <c r="B10" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="C10" s="2"/>
+        <v>52</v>
+      </c>
+      <c r="C10" t="s" s="2">
+        <v>53</v>
+      </c>
       <c r="D10" t="n" s="2">
         <v>0.0</v>
       </c>
       <c r="E10" t="s" s="2">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="F10" t="n" s="2">
-        <v>135.0</v>
+        <v>0.0</v>
       </c>
       <c r="G10" t="n" s="2">
-        <v>25.0</v>
+        <v>0.0</v>
       </c>
       <c r="H10" t="s" s="2">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="I10" t="n" s="2">
-        <v>1238.0</v>
+        <v>0.0</v>
       </c>
       <c r="J10" t="s" s="2">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="K10" t="n" s="2">
-        <v>1077.0</v>
+        <v>836.0</v>
       </c>
       <c r="L10" t="s" s="2">
-        <v>48</v>
+        <v>52</v>
+      </c>
+      <c r="M10" t="n" s="2">
+        <v>109.0</v>
+      </c>
+      <c r="N10" t="s" s="2">
+        <v>55</v>
       </c>
     </row>
     <row r="11">
@@ -667,35 +781,131 @@
         <v>10.0</v>
       </c>
       <c r="B11" t="s" s="2">
-        <v>49</v>
-      </c>
-      <c r="C11" s="2"/>
+        <v>56</v>
+      </c>
+      <c r="C11" t="s" s="2">
+        <v>57</v>
+      </c>
       <c r="D11" t="n" s="2">
         <v>0.0</v>
       </c>
       <c r="E11" t="s" s="2">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="F11" t="n" s="2">
-        <v>191.0</v>
+        <v>0.0</v>
       </c>
       <c r="G11" t="n" s="2">
-        <v>39.0</v>
+        <v>0.0</v>
       </c>
       <c r="H11" t="s" s="2">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="I11" t="n" s="2">
         <v>0.0</v>
       </c>
       <c r="J11" t="s" s="2">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="K11" t="n" s="2">
-        <v>1446.0</v>
+        <v>933.0</v>
       </c>
       <c r="L11" t="s" s="2">
-        <v>51</v>
+        <v>56</v>
+      </c>
+      <c r="M11" t="n" s="2">
+        <v>62.0</v>
+      </c>
+      <c r="N11" t="s" s="2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n" s="2">
+        <v>11.0</v>
+      </c>
+      <c r="B12" t="s" s="2">
+        <v>61</v>
+      </c>
+      <c r="C12" t="s" s="2">
+        <v>61</v>
+      </c>
+      <c r="D12" t="n" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="E12" t="s" s="2">
+        <v>61</v>
+      </c>
+      <c r="F12" t="n" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="G12" t="n" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="H12" t="s" s="2">
+        <v>61</v>
+      </c>
+      <c r="I12" t="n" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="J12" t="s" s="2">
+        <v>62</v>
+      </c>
+      <c r="K12" t="n" s="2">
+        <v>833.0</v>
+      </c>
+      <c r="L12" t="s" s="2">
+        <v>61</v>
+      </c>
+      <c r="M12" t="n" s="2">
+        <v>71.0</v>
+      </c>
+      <c r="N12" t="s" s="2">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n" s="2">
+        <v>12.0</v>
+      </c>
+      <c r="B13" t="s" s="2">
+        <v>64</v>
+      </c>
+      <c r="C13" t="s" s="2">
+        <v>65</v>
+      </c>
+      <c r="D13" t="n" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="E13" t="s" s="2">
+        <v>64</v>
+      </c>
+      <c r="F13" t="n" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="G13" t="n" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="H13" t="s" s="2">
+        <v>66</v>
+      </c>
+      <c r="I13" t="n" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="J13" t="s" s="2">
+        <v>66</v>
+      </c>
+      <c r="K13" t="n" s="2">
+        <v>1133.0</v>
+      </c>
+      <c r="L13" t="s" s="2">
+        <v>64</v>
+      </c>
+      <c r="M13" t="n" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="N13" t="s" s="2">
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add generated leaderboard data - 17-12-2023 19:43:46
</commit_message>
<xml_diff>
--- a/Leaderboards/CurrentCMRITLeaderboard2025.xlsx
+++ b/Leaderboards/CurrentCMRITLeaderboard2025.xlsx
@@ -332,20 +332,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="10.2109375" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="15.07421875" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="34.24609375" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="33.09765625" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="22.62890625" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="34.78125" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="35.2421875" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="30.78515625" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="29.63671875" customWidth="true" bestFit="true"/>
-    <col min="10" max="10" width="31.22265625" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="30.07421875" customWidth="true" bestFit="true"/>
-    <col min="12" max="12" width="35.515625" customWidth="true" bestFit="true"/>
-    <col min="13" max="13" width="48.12890625" customWidth="true" bestFit="true"/>
-    <col min="14" max="14" width="18.6796875" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="11.5625" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="17.2265625" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="38.01171875" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="37.12109375" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="24.7734375" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="38.3515625" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="39.09375" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="34.17578125" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="33.28515625" customWidth="true" bestFit="true"/>
+    <col min="10" max="10" width="34.46875" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="33.578125" customWidth="true" bestFit="true"/>
+    <col min="12" max="12" width="39.56640625" customWidth="true" bestFit="true"/>
+    <col min="13" max="13" width="53.890625" customWidth="true" bestFit="true"/>
+    <col min="14" max="14" width="21.25390625" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">

</xml_diff>

<commit_message>
Add generated leaderboard data - 12-01-2024 20:40:57
</commit_message>
<xml_diff>
--- a/Leaderboards/CurrentCMRITLeaderboard2025.xlsx
+++ b/Leaderboards/CurrentCMRITLeaderboard2025.xlsx
@@ -2318,6 +2318,21 @@
     <t>33.9%</t>
   </si>
   <si>
+    <t>21r01a7215</t>
+  </si>
+  <si>
+    <t>dhansai</t>
+  </si>
+  <si>
+    <t>dhanswfst</t>
+  </si>
+  <si>
+    <t>dhansaib6</t>
+  </si>
+  <si>
+    <t>33.88%</t>
+  </si>
+  <si>
     <t>21r01a0544</t>
   </si>
   <si>
@@ -2330,21 +2345,6 @@
     <t>33.87%</t>
   </si>
   <si>
-    <t>21r01a7215</t>
-  </si>
-  <si>
-    <t>dhansai</t>
-  </si>
-  <si>
-    <t>dhanswfst</t>
-  </si>
-  <si>
-    <t>dhansaib6</t>
-  </si>
-  <si>
-    <t>33.86%</t>
-  </si>
-  <si>
     <t>21r01a0559</t>
   </si>
   <si>
@@ -2639,7 +2639,7 @@
     <t>vaishnavisingir1</t>
   </si>
   <si>
-    <t>33.21%</t>
+    <t>33.23%</t>
   </si>
   <si>
     <t>21r01a66c3</t>
@@ -19163,37 +19163,37 @@
         <v>769</v>
       </c>
       <c r="D175" t="n" s="2">
-        <v>789.0</v>
+        <v>724.0</v>
       </c>
       <c r="E175" t="s" s="2">
-        <v>768</v>
+        <v>770</v>
       </c>
       <c r="F175" t="n" s="2">
-        <v>20.0</v>
+        <v>10.0</v>
       </c>
       <c r="G175" t="n" s="2">
+        <v>54.0</v>
+      </c>
+      <c r="H175" t="s" s="2">
+        <v>771</v>
+      </c>
+      <c r="I175" t="n" s="2">
+        <v>1468.0</v>
+      </c>
+      <c r="J175" t="s" s="2">
+        <v>771</v>
+      </c>
+      <c r="K175" t="n" s="2">
+        <v>1380.0</v>
+      </c>
+      <c r="L175" t="s" s="2">
+        <v>771</v>
+      </c>
+      <c r="M175" t="n" s="2">
         <v>27.0</v>
       </c>
-      <c r="H175" t="s" s="2">
-        <v>770</v>
-      </c>
-      <c r="I175" t="n" s="2">
-        <v>1375.0</v>
-      </c>
-      <c r="J175" t="s" s="2">
-        <v>770</v>
-      </c>
-      <c r="K175" t="n" s="2">
-        <v>998.0</v>
-      </c>
-      <c r="L175" t="s" s="2">
-        <v>768</v>
-      </c>
-      <c r="M175" t="n" s="2">
-        <v>167.0</v>
-      </c>
       <c r="N175" t="s" s="2">
-        <v>771</v>
+        <v>772</v>
       </c>
     </row>
     <row r="176">
@@ -19201,40 +19201,40 @@
         <v>175.0</v>
       </c>
       <c r="B176" t="s" s="2">
-        <v>772</v>
+        <v>773</v>
       </c>
       <c r="C176" t="s" s="2">
+        <v>774</v>
+      </c>
+      <c r="D176" t="n" s="2">
+        <v>789.0</v>
+      </c>
+      <c r="E176" t="s" s="2">
         <v>773</v>
       </c>
-      <c r="D176" t="n" s="2">
-        <v>724.0</v>
-      </c>
-      <c r="E176" t="s" s="2">
-        <v>774</v>
-      </c>
       <c r="F176" t="n" s="2">
-        <v>10.0</v>
+        <v>20.0</v>
       </c>
       <c r="G176" t="n" s="2">
-        <v>52.0</v>
+        <v>27.0</v>
       </c>
       <c r="H176" t="s" s="2">
         <v>775</v>
       </c>
       <c r="I176" t="n" s="2">
-        <v>1468.0</v>
+        <v>1375.0</v>
       </c>
       <c r="J176" t="s" s="2">
         <v>775</v>
       </c>
       <c r="K176" t="n" s="2">
-        <v>1380.0</v>
+        <v>998.0</v>
       </c>
       <c r="L176" t="s" s="2">
-        <v>775</v>
+        <v>773</v>
       </c>
       <c r="M176" t="n" s="2">
-        <v>27.0</v>
+        <v>167.0</v>
       </c>
       <c r="N176" t="s" s="2">
         <v>776</v>
@@ -20184,7 +20184,7 @@
         <v>10.0</v>
       </c>
       <c r="G198" t="n" s="2">
-        <v>66.0</v>
+        <v>68.0</v>
       </c>
       <c r="H198" t="s" s="2">
         <v>872</v>

</xml_diff>

<commit_message>
Add generated leaderboard data - 13-01-2024 20:22:54
</commit_message>
<xml_diff>
--- a/Leaderboards/CurrentCMRITLeaderboard2025.xlsx
+++ b/Leaderboards/CurrentCMRITLeaderboard2025.xlsx
@@ -188,7 +188,7 @@
     <t>narayansharma</t>
   </si>
   <si>
-    <t>54.7%</t>
+    <t>54.89%</t>
   </si>
   <si>
     <t>21r01a66h1</t>
@@ -1346,6 +1346,15 @@
     <t>37.47%</t>
   </si>
   <si>
+    <t>22r05a0514</t>
+  </si>
+  <si>
+    <t>kodam1</t>
+  </si>
+  <si>
+    <t>37.33%</t>
+  </si>
+  <si>
     <t>22r05a0406</t>
   </si>
   <si>
@@ -1391,15 +1400,6 @@
     <t>37.21%</t>
   </si>
   <si>
-    <t>22r05a0514</t>
-  </si>
-  <si>
-    <t>kodam1</t>
-  </si>
-  <si>
-    <t>37.2%</t>
-  </si>
-  <si>
     <t>21r01a66f9</t>
   </si>
   <si>
@@ -4280,6 +4280,18 @@
     <t>25.57%</t>
   </si>
   <si>
+    <t>21r01a05g9</t>
+  </si>
+  <si>
+    <t>cmrit25_21r01a05g9</t>
+  </si>
+  <si>
+    <t>srivarsha_31</t>
+  </si>
+  <si>
+    <t>25.49%</t>
+  </si>
+  <si>
     <t>21r01a04p0</t>
   </si>
   <si>
@@ -4293,18 +4305,6 @@
   </si>
   <si>
     <t>25.42%</t>
-  </si>
-  <si>
-    <t>21r01a05g9</t>
-  </si>
-  <si>
-    <t>cmrit25_21r01a05g9</t>
-  </si>
-  <si>
-    <t>srivarsha_31</t>
-  </si>
-  <si>
-    <t>25.41%</t>
   </si>
   <si>
     <t>21r01a67j5</t>
@@ -12000,7 +12000,7 @@
         <v>415.0</v>
       </c>
       <c r="G12" t="n" s="2">
-        <v>385.0</v>
+        <v>404.0</v>
       </c>
       <c r="H12" t="s" s="2">
         <v>56</v>
@@ -15863,37 +15863,37 @@
         <v>445</v>
       </c>
       <c r="D100" t="n" s="2">
-        <v>866.0</v>
+        <v>644.0</v>
       </c>
       <c r="E100" t="s" s="2">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="F100" t="n" s="2">
-        <v>20.0</v>
+        <v>115.0</v>
       </c>
       <c r="G100" t="n" s="2">
-        <v>1.0</v>
+        <v>15.0</v>
       </c>
       <c r="H100" t="s" s="2">
         <v>444</v>
       </c>
       <c r="I100" t="n" s="2">
-        <v>1459.0</v>
+        <v>1479.0</v>
       </c>
       <c r="J100" t="s" s="2">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="K100" t="n" s="2">
-        <v>1389.0</v>
+        <v>1333.0</v>
       </c>
       <c r="L100" t="s" s="2">
         <v>444</v>
       </c>
       <c r="M100" t="n" s="2">
-        <v>68.0</v>
+        <v>32.0</v>
       </c>
       <c r="N100" t="s" s="2">
-        <v>448</v>
+        <v>446</v>
       </c>
     </row>
     <row r="101">
@@ -15901,43 +15901,43 @@
         <v>100.0</v>
       </c>
       <c r="B101" t="s" s="2">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="C101" t="s" s="2">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="D101" t="n" s="2">
-        <v>840.0</v>
+        <v>866.0</v>
       </c>
       <c r="E101" t="s" s="2">
         <v>449</v>
       </c>
       <c r="F101" t="n" s="2">
-        <v>19.0</v>
+        <v>20.0</v>
       </c>
       <c r="G101" t="n" s="2">
-        <v>56.0</v>
+        <v>1.0</v>
       </c>
       <c r="H101" t="s" s="2">
+        <v>447</v>
+      </c>
+      <c r="I101" t="n" s="2">
+        <v>1459.0</v>
+      </c>
+      <c r="J101" t="s" s="2">
+        <v>450</v>
+      </c>
+      <c r="K101" t="n" s="2">
+        <v>1389.0</v>
+      </c>
+      <c r="L101" t="s" s="2">
+        <v>447</v>
+      </c>
+      <c r="M101" t="n" s="2">
+        <v>68.0</v>
+      </c>
+      <c r="N101" t="s" s="2">
         <v>451</v>
-      </c>
-      <c r="I101" t="n" s="2">
-        <v>1383.0</v>
-      </c>
-      <c r="J101" t="s" s="2">
-        <v>452</v>
-      </c>
-      <c r="K101" t="n" s="2">
-        <v>928.0</v>
-      </c>
-      <c r="L101" t="s" s="2">
-        <v>449</v>
-      </c>
-      <c r="M101" t="n" s="2">
-        <v>433.0</v>
-      </c>
-      <c r="N101" t="s" s="2">
-        <v>453</v>
       </c>
     </row>
     <row r="102">
@@ -15945,43 +15945,43 @@
         <v>101.0</v>
       </c>
       <c r="B102" t="s" s="2">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="C102" t="s" s="2">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="D102" t="n" s="2">
-        <v>730.0</v>
+        <v>840.0</v>
       </c>
       <c r="E102" t="s" s="2">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="F102" t="n" s="2">
-        <v>60.0</v>
+        <v>19.0</v>
       </c>
       <c r="G102" t="n" s="2">
-        <v>28.0</v>
+        <v>56.0</v>
       </c>
       <c r="H102" t="s" s="2">
         <v>454</v>
       </c>
       <c r="I102" t="n" s="2">
-        <v>1448.0</v>
+        <v>1383.0</v>
       </c>
       <c r="J102" t="s" s="2">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="K102" t="n" s="2">
-        <v>1328.0</v>
+        <v>928.0</v>
       </c>
       <c r="L102" t="s" s="2">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="M102" t="n" s="2">
-        <v>155.0</v>
+        <v>433.0</v>
       </c>
       <c r="N102" t="s" s="2">
-        <v>458</v>
+        <v>456</v>
       </c>
     </row>
     <row r="103">
@@ -15989,40 +15989,40 @@
         <v>102.0</v>
       </c>
       <c r="B103" t="s" s="2">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="C103" t="s" s="2">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="D103" t="n" s="2">
-        <v>644.0</v>
+        <v>730.0</v>
       </c>
       <c r="E103" t="s" s="2">
         <v>459</v>
       </c>
       <c r="F103" t="n" s="2">
-        <v>115.0</v>
+        <v>60.0</v>
       </c>
       <c r="G103" t="n" s="2">
-        <v>4.0</v>
+        <v>28.0</v>
       </c>
       <c r="H103" t="s" s="2">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="I103" t="n" s="2">
-        <v>1479.0</v>
+        <v>1448.0</v>
       </c>
       <c r="J103" t="s" s="2">
         <v>460</v>
       </c>
       <c r="K103" t="n" s="2">
-        <v>1333.0</v>
+        <v>1328.0</v>
       </c>
       <c r="L103" t="s" s="2">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="M103" t="n" s="2">
-        <v>29.0</v>
+        <v>155.0</v>
       </c>
       <c r="N103" t="s" s="2">
         <v>461</v>
@@ -25983,13 +25983,13 @@
         <v>1423</v>
       </c>
       <c r="D330" t="n" s="2">
-        <v>789.0</v>
+        <v>350.0</v>
       </c>
       <c r="E330" t="s" s="2">
-        <v>1424</v>
+        <v>1422</v>
       </c>
       <c r="F330" t="n" s="2">
-        <v>0.0</v>
+        <v>49.0</v>
       </c>
       <c r="G330" t="n" s="2">
         <v>0.0</v>
@@ -25998,22 +25998,22 @@
         <v>1422</v>
       </c>
       <c r="I330" t="n" s="2">
-        <v>1459.0</v>
+        <v>1537.0</v>
       </c>
       <c r="J330" t="s" s="2">
-        <v>1425</v>
+        <v>1424</v>
       </c>
       <c r="K330" t="n" s="2">
-        <v>0.0</v>
+        <v>862.0</v>
       </c>
       <c r="L330" t="s" s="2">
         <v>1422</v>
       </c>
       <c r="M330" t="n" s="2">
-        <v>32.0</v>
+        <v>121.0</v>
       </c>
       <c r="N330" t="s" s="2">
-        <v>1426</v>
+        <v>1425</v>
       </c>
     </row>
     <row r="331">
@@ -26021,40 +26021,40 @@
         <v>330.0</v>
       </c>
       <c r="B331" t="s" s="2">
+        <v>1426</v>
+      </c>
+      <c r="C331" t="s" s="2">
         <v>1427</v>
       </c>
-      <c r="C331" t="s" s="2">
+      <c r="D331" t="n" s="2">
+        <v>789.0</v>
+      </c>
+      <c r="E331" t="s" s="2">
         <v>1428</v>
       </c>
-      <c r="D331" t="n" s="2">
-        <v>350.0</v>
-      </c>
-      <c r="E331" t="s" s="2">
-        <v>1427</v>
-      </c>
       <c r="F331" t="n" s="2">
-        <v>49.0</v>
+        <v>0.0</v>
       </c>
       <c r="G331" t="n" s="2">
         <v>0.0</v>
       </c>
       <c r="H331" t="s" s="2">
-        <v>1427</v>
+        <v>1426</v>
       </c>
       <c r="I331" t="n" s="2">
-        <v>1537.0</v>
+        <v>1459.0</v>
       </c>
       <c r="J331" t="s" s="2">
         <v>1429</v>
       </c>
       <c r="K331" t="n" s="2">
-        <v>862.0</v>
+        <v>0.0</v>
       </c>
       <c r="L331" t="s" s="2">
-        <v>1427</v>
+        <v>1426</v>
       </c>
       <c r="M331" t="n" s="2">
-        <v>112.0</v>
+        <v>32.0</v>
       </c>
       <c r="N331" t="s" s="2">
         <v>1430</v>

</xml_diff>

<commit_message>
Add generated leaderboard data - 24-01-2024 08:08:52
</commit_message>
<xml_diff>
--- a/Leaderboards/CurrentCMRITLeaderboard2025.xlsx
+++ b/Leaderboards/CurrentCMRITLeaderboard2025.xlsx
@@ -332,20 +332,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="10.2109375" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="15.07421875" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="34.24609375" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="33.09765625" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="22.62890625" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="34.78125" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="35.2421875" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="30.78515625" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="29.63671875" customWidth="true" bestFit="true"/>
-    <col min="10" max="10" width="31.22265625" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="30.07421875" customWidth="true" bestFit="true"/>
-    <col min="12" max="12" width="35.515625" customWidth="true" bestFit="true"/>
-    <col min="13" max="13" width="48.12890625" customWidth="true" bestFit="true"/>
-    <col min="14" max="14" width="18.6796875" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="11.5625" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="17.2265625" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="38.01171875" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="37.12109375" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="24.7734375" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="38.3515625" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="39.09375" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="34.17578125" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="33.28515625" customWidth="true" bestFit="true"/>
+    <col min="10" max="10" width="34.46875" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="33.578125" customWidth="true" bestFit="true"/>
+    <col min="12" max="12" width="39.56640625" customWidth="true" bestFit="true"/>
+    <col min="13" max="13" width="53.890625" customWidth="true" bestFit="true"/>
+    <col min="14" max="14" width="21.25390625" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">

</xml_diff>

<commit_message>
Add generated leaderboard data - 2024-03-12T19:19:37
</commit_message>
<xml_diff>
--- a/Leaderboards/CurrentCMRITLeaderboard2025.xlsx
+++ b/Leaderboards/CurrentCMRITLeaderboard2025.xlsx
@@ -173,7 +173,7 @@
     <t>prashanth50</t>
   </si>
   <si>
-    <t>58.14%</t>
+    <t>58.15%</t>
   </si>
   <si>
     <t>21R01A66H1</t>
@@ -254,7 +254,7 @@
     <t>premsai20</t>
   </si>
   <si>
-    <t>56.43%</t>
+    <t>56.44%</t>
   </si>
   <si>
     <t>21R01A05F9</t>
@@ -650,7 +650,7 @@
     <t>cmr_21r01a0557</t>
   </si>
   <si>
-    <t>48.32%</t>
+    <t>48.43%</t>
   </si>
   <si>
     <t>21R01A7309</t>
@@ -15144,7 +15144,7 @@
         <v>425.0</v>
       </c>
       <c r="G9" s="2" t="n">
-        <v>405.0</v>
+        <v>409.0</v>
       </c>
       <c r="H9" s="2" t="s">
         <v>49</v>
@@ -15364,7 +15364,7 @@
         <v>560.0</v>
       </c>
       <c r="G14" s="2" t="n">
-        <v>30.0</v>
+        <v>34.0</v>
       </c>
       <c r="H14" s="2" t="s">
         <v>78</v>
@@ -16464,7 +16464,7 @@
         <v>259.0</v>
       </c>
       <c r="G39" s="2" t="n">
-        <v>365.0</v>
+        <v>401.0</v>
       </c>
       <c r="H39" s="2" t="s">
         <v>208</v>

</xml_diff>

<commit_message>
Add generated leaderboard data - 2024-03-18T20:10:45
</commit_message>
<xml_diff>
--- a/Leaderboards/CurrentCMRITLeaderboard2025.xlsx
+++ b/Leaderboards/CurrentCMRITLeaderboard2025.xlsx
@@ -308,46 +308,46 @@
     <t>54.72%</t>
   </si>
   <si>
+    <t>21R01A66A1</t>
+  </si>
+  <si>
+    <t>CMRIT25_21R01A66A1</t>
+  </si>
+  <si>
+    <t>21r01aspay</t>
+  </si>
+  <si>
+    <t>cmr_21R01A66A1</t>
+  </si>
+  <si>
+    <t>cmr_21r01a66a1</t>
+  </si>
+  <si>
+    <t>54.54%</t>
+  </si>
+  <si>
+    <t>21R01A0504</t>
+  </si>
+  <si>
+    <t>CMRIT25_21R01A0504</t>
+  </si>
+  <si>
+    <t>21r01a0504</t>
+  </si>
+  <si>
+    <t>madhusudhan04</t>
+  </si>
+  <si>
+    <t>53.98%</t>
+  </si>
+  <si>
     <t>21R01A6712</t>
   </si>
   <si>
     <t>rahuldrp</t>
   </si>
   <si>
-    <t>54.67%</t>
-  </si>
-  <si>
-    <t>21R01A66A1</t>
-  </si>
-  <si>
-    <t>CMRIT25_21R01A66A1</t>
-  </si>
-  <si>
-    <t>21r01aspay</t>
-  </si>
-  <si>
-    <t>cmr_21R01A66A1</t>
-  </si>
-  <si>
-    <t>cmr_21r01a66a1</t>
-  </si>
-  <si>
-    <t>54.54%</t>
-  </si>
-  <si>
-    <t>21R01A0504</t>
-  </si>
-  <si>
-    <t>CMRIT25_21R01A0504</t>
-  </si>
-  <si>
-    <t>21r01a0504</t>
-  </si>
-  <si>
-    <t>madhusudhan04</t>
-  </si>
-  <si>
-    <t>53.98%</t>
+    <t>53.88%</t>
   </si>
   <si>
     <t>21R01A05H0</t>
@@ -1736,7 +1736,7 @@
     <t>cmr_21r01a04m7</t>
   </si>
   <si>
-    <t>40.7%</t>
+    <t>40.71%</t>
   </si>
   <si>
     <t>21R01A6627</t>
@@ -14917,7 +14917,7 @@
         <v>435.0</v>
       </c>
       <c r="G8" s="2" t="n">
-        <v>455.0</v>
+        <v>457.0</v>
       </c>
       <c r="H8" s="2" t="s">
         <v>44</v>
@@ -15348,37 +15348,37 @@
         <v>99</v>
       </c>
       <c r="D18" s="2" t="n">
-        <v>817.0</v>
+        <v>1084.0</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="F18" s="2" t="n">
-        <v>387.0</v>
+        <v>318.0</v>
       </c>
       <c r="G18" s="2" t="n">
-        <v>64.0</v>
+        <v>2.0</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="I18" s="2" t="n">
-        <v>1423.0</v>
+        <v>1613.0</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="K18" s="2" t="n">
-        <v>1618.0</v>
+        <v>1494.0</v>
       </c>
       <c r="L18" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="M18" s="2" t="n">
-        <v>526.0</v>
+        <v>139.0</v>
       </c>
       <c r="N18" s="2" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
     </row>
     <row r="19">
@@ -15386,43 +15386,43 @@
         <v>18.0</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="D19" s="2" t="n">
-        <v>1084.0</v>
+        <v>887.0</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="F19" s="2" t="n">
-        <v>318.0</v>
+        <v>463.0</v>
       </c>
       <c r="G19" s="2" t="n">
-        <v>2.0</v>
+        <v>263.0</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="I19" s="2" t="n">
-        <v>1613.0</v>
+        <v>1453.0</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="K19" s="2" t="n">
-        <v>1494.0</v>
+        <v>1280.0</v>
       </c>
       <c r="L19" s="2" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="M19" s="2" t="n">
-        <v>139.0</v>
+        <v>45.0</v>
       </c>
       <c r="N19" s="2" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
     </row>
     <row r="20">
@@ -15430,40 +15430,40 @@
         <v>19.0</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="D20" s="2" t="n">
-        <v>887.0</v>
+        <v>817.0</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="F20" s="2" t="n">
-        <v>463.0</v>
+        <v>367.0</v>
       </c>
       <c r="G20" s="2" t="n">
-        <v>263.0</v>
+        <v>64.0</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="I20" s="2" t="n">
-        <v>1453.0</v>
+        <v>1423.0</v>
       </c>
       <c r="J20" s="2" t="s">
         <v>110</v>
       </c>
       <c r="K20" s="2" t="n">
-        <v>1280.0</v>
+        <v>1618.0</v>
       </c>
       <c r="L20" s="2" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="M20" s="2" t="n">
-        <v>45.0</v>
+        <v>526.0</v>
       </c>
       <c r="N20" s="2" t="s">
         <v>111</v>
@@ -19317,7 +19317,7 @@
         <v>30.0</v>
       </c>
       <c r="G108" s="2" t="n">
-        <v>146.0</v>
+        <v>150.0</v>
       </c>
       <c r="H108" s="2" t="s">
         <v>570</v>

</xml_diff>

<commit_message>
Add generated leaderboard data - 2024-03-30T20:11:14
</commit_message>
<xml_diff>
--- a/Leaderboards/CurrentCMRITLeaderboard2025.xlsx
+++ b/Leaderboards/CurrentCMRITLeaderboard2025.xlsx
@@ -83,7 +83,7 @@
     <t>pavanvasam577</t>
   </si>
   <si>
-    <t>65.09%</t>
+    <t>65.14%</t>
   </si>
   <si>
     <t>21R01A67F2</t>
@@ -173,7 +173,7 @@
     <t>prashanth50</t>
   </si>
   <si>
-    <t>58.33%</t>
+    <t>58.35%</t>
   </si>
   <si>
     <t>21R01A66H1</t>
@@ -479,7 +479,7 @@
     <t>deepikachowdar</t>
   </si>
   <si>
-    <t>50.53%</t>
+    <t>50.54%</t>
   </si>
   <si>
     <t>21R01A0539</t>
@@ -1601,7 +1601,7 @@
     <t>vishnupriya508</t>
   </si>
   <si>
-    <t>41.76%</t>
+    <t>41.78%</t>
   </si>
   <si>
     <t>21R01A05J3</t>
@@ -3878,7 +3878,7 @@
     <t>adithya2210</t>
   </si>
   <si>
-    <t>35.01%</t>
+    <t>35.02%</t>
   </si>
   <si>
     <t>22R05A0502</t>
@@ -5996,24 +5996,24 @@
     <t>ashritha92</t>
   </si>
   <si>
+    <t>21R01A67J7</t>
+  </si>
+  <si>
+    <t>CMRIT25_21R01A67J7</t>
+  </si>
+  <si>
+    <t>manohar7j7</t>
+  </si>
+  <si>
+    <t>21r01a67j7</t>
+  </si>
+  <si>
+    <t>cmr_21r01a67j7</t>
+  </si>
+  <si>
     <t>30.64%</t>
   </si>
   <si>
-    <t>21R01A67J7</t>
-  </si>
-  <si>
-    <t>CMRIT25_21R01A67J7</t>
-  </si>
-  <si>
-    <t>manohar7j7</t>
-  </si>
-  <si>
-    <t>21r01a67j7</t>
-  </si>
-  <si>
-    <t>cmr_21r01a67j7</t>
-  </si>
-  <si>
     <t>21R01A67F4</t>
   </si>
   <si>
@@ -8609,6 +8609,18 @@
     <t>22.12%</t>
   </si>
   <si>
+    <t>21R01A04M0</t>
+  </si>
+  <si>
+    <t>Cmrit25_21r01a04m0</t>
+  </si>
+  <si>
+    <t>vishnu4m0</t>
+  </si>
+  <si>
+    <t>22.07%</t>
+  </si>
+  <si>
     <t>21R01A7222</t>
   </si>
   <si>
@@ -8627,18 +8639,6 @@
     <t>22.06%</t>
   </si>
   <si>
-    <t>21R01A04M0</t>
-  </si>
-  <si>
-    <t>Cmrit25_21r01a04m0</t>
-  </si>
-  <si>
-    <t>vishnu4m0</t>
-  </si>
-  <si>
-    <t>22.05%</t>
-  </si>
-  <si>
     <t>21R01A7324</t>
   </si>
   <si>
@@ -8684,6 +8684,24 @@
     <t>21.95%</t>
   </si>
   <si>
+    <t>21R01A05P8</t>
+  </si>
+  <si>
+    <t>CMRIT25_21R01A05P8</t>
+  </si>
+  <si>
+    <t>rohan_adepu</t>
+  </si>
+  <si>
+    <t>21r01a05p8cmritonline.ac.in</t>
+  </si>
+  <si>
+    <t>21R01A05P8rohan</t>
+  </si>
+  <si>
+    <t>21.89%</t>
+  </si>
+  <si>
     <t>21R01A05E9</t>
   </si>
   <si>
@@ -8697,24 +8715,6 @@
   </si>
   <si>
     <t>21.87%</t>
-  </si>
-  <si>
-    <t>21R01A05P8</t>
-  </si>
-  <si>
-    <t>CMRIT25_21R01A05P8</t>
-  </si>
-  <si>
-    <t>rohan_adepu</t>
-  </si>
-  <si>
-    <t>21r01a05p8cmritonline.ac.in</t>
-  </si>
-  <si>
-    <t>21R01A05P8rohan</t>
-  </si>
-  <si>
-    <t>21.85%</t>
   </si>
   <si>
     <t>21R01A0451</t>
@@ -14733,7 +14733,7 @@
         <v>766.0</v>
       </c>
       <c r="G3" s="2" t="n">
-        <v>200.0</v>
+        <v>215.0</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>21</v>
@@ -14997,7 +14997,7 @@
         <v>435.0</v>
       </c>
       <c r="G9" s="2" t="n">
-        <v>481.0</v>
+        <v>488.0</v>
       </c>
       <c r="H9" s="2" t="s">
         <v>49</v>
@@ -15833,7 +15833,7 @@
         <v>262.0</v>
       </c>
       <c r="G28" s="2" t="n">
-        <v>312.0</v>
+        <v>317.0</v>
       </c>
       <c r="H28" s="2" t="s">
         <v>153</v>
@@ -16141,7 +16141,7 @@
         <v>391.0</v>
       </c>
       <c r="G35" s="2" t="n">
-        <v>576.0</v>
+        <v>578.0</v>
       </c>
       <c r="H35" s="2" t="s">
         <v>192</v>
@@ -16361,7 +16361,7 @@
         <v>397.0</v>
       </c>
       <c r="G40" s="2" t="n">
-        <v>136.0</v>
+        <v>137.0</v>
       </c>
       <c r="H40" s="2" t="s">
         <v>216</v>
@@ -18913,7 +18913,7 @@
         <v>185.0</v>
       </c>
       <c r="G98" s="2" t="n">
-        <v>95.0</v>
+        <v>103.0</v>
       </c>
       <c r="H98" s="2" t="s">
         <v>527</v>
@@ -20453,7 +20453,7 @@
         <v>150.0</v>
       </c>
       <c r="G133" s="2" t="n">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
       <c r="H133" s="2" t="s">
         <v>707</v>
@@ -23489,7 +23489,7 @@
         <v>119.0</v>
       </c>
       <c r="G202" s="2" t="n">
-        <v>11.0</v>
+        <v>13.0</v>
       </c>
       <c r="H202" s="2" t="s">
         <v>1072</v>
@@ -25249,7 +25249,7 @@
         <v>10.0</v>
       </c>
       <c r="G242" s="2" t="n">
-        <v>43.0</v>
+        <v>47.0</v>
       </c>
       <c r="H242" s="2" t="s">
         <v>1287</v>
@@ -26261,7 +26261,7 @@
         <v>28.0</v>
       </c>
       <c r="G265" s="2" t="n">
-        <v>118.0</v>
+        <v>121.0</v>
       </c>
       <c r="H265" s="2" t="s">
         <v>1406</v>
@@ -31277,7 +31277,7 @@
         <v>49.0</v>
       </c>
       <c r="G379" s="2" t="n">
-        <v>94.0</v>
+        <v>98.0</v>
       </c>
       <c r="H379" s="2" t="s">
         <v>1992</v>
@@ -31298,7 +31298,7 @@
         <v>424.0</v>
       </c>
       <c r="N379" s="2" t="s">
-        <v>1994</v>
+        <v>1990</v>
       </c>
     </row>
     <row r="380">
@@ -31306,16 +31306,16 @@
         <v>379.0</v>
       </c>
       <c r="B380" s="2" t="s">
+        <v>1994</v>
+      </c>
+      <c r="C380" s="2" t="s">
         <v>1995</v>
-      </c>
-      <c r="C380" s="2" t="s">
-        <v>1996</v>
       </c>
       <c r="D380" s="2" t="n">
         <v>529.0</v>
       </c>
       <c r="E380" s="2" t="s">
-        <v>1997</v>
+        <v>1996</v>
       </c>
       <c r="F380" s="2" t="n">
         <v>68.0</v>
@@ -31324,25 +31324,25 @@
         <v>51.0</v>
       </c>
       <c r="H380" s="2" t="s">
-        <v>1998</v>
+        <v>1997</v>
       </c>
       <c r="I380" s="2" t="n">
         <v>1338.0</v>
       </c>
       <c r="J380" s="2" t="s">
-        <v>1999</v>
+        <v>1998</v>
       </c>
       <c r="K380" s="2" t="n">
         <v>1123.0</v>
       </c>
       <c r="L380" s="2" t="s">
-        <v>1995</v>
+        <v>1994</v>
       </c>
       <c r="M380" s="2" t="n">
         <v>318.0</v>
       </c>
       <c r="N380" s="2" t="s">
-        <v>1994</v>
+        <v>1999</v>
       </c>
     </row>
     <row r="381">
@@ -38836,37 +38836,37 @@
         <v>2866</v>
       </c>
       <c r="D551" s="2" t="n">
-        <v>738.0</v>
+        <v>364.0</v>
       </c>
       <c r="E551" s="2" t="s">
+        <v>2865</v>
+      </c>
+      <c r="F551" s="2" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="G551" s="2" t="n">
+        <v>25.0</v>
+      </c>
+      <c r="H551" s="2" t="s">
+        <v>2865</v>
+      </c>
+      <c r="I551" s="2" t="n">
+        <v>1545.0</v>
+      </c>
+      <c r="J551" s="2" t="s">
         <v>2867</v>
       </c>
-      <c r="F551" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="G551" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="H551" s="2" t="s">
+      <c r="K551" s="2" t="n">
+        <v>902.0</v>
+      </c>
+      <c r="L551" s="2" t="s">
+        <v>2865</v>
+      </c>
+      <c r="M551" s="2" t="n">
+        <v>14.0</v>
+      </c>
+      <c r="N551" s="2" t="s">
         <v>2868</v>
-      </c>
-      <c r="I551" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="J551" s="2" t="s">
-        <v>2869</v>
-      </c>
-      <c r="K551" s="2" t="n">
-        <v>941.0</v>
-      </c>
-      <c r="L551" s="2" t="s">
-        <v>2867</v>
-      </c>
-      <c r="M551" s="2" t="n">
-        <v>77.0</v>
-      </c>
-      <c r="N551" s="2" t="s">
-        <v>2870</v>
       </c>
     </row>
     <row r="552">
@@ -38874,40 +38874,40 @@
         <v>551.0</v>
       </c>
       <c r="B552" s="2" t="s">
-        <v>2871</v>
+        <v>2869</v>
       </c>
       <c r="C552" s="2" t="s">
-        <v>2872</v>
+        <v>2870</v>
       </c>
       <c r="D552" s="2" t="n">
-        <v>364.0</v>
+        <v>738.0</v>
       </c>
       <c r="E552" s="2" t="s">
         <v>2871</v>
       </c>
       <c r="F552" s="2" t="n">
-        <v>10.0</v>
+        <v>0.0</v>
       </c>
       <c r="G552" s="2" t="n">
-        <v>21.0</v>
+        <v>0.0</v>
       </c>
       <c r="H552" s="2" t="s">
-        <v>2871</v>
+        <v>2872</v>
       </c>
       <c r="I552" s="2" t="n">
-        <v>1545.0</v>
+        <v>0.0</v>
       </c>
       <c r="J552" s="2" t="s">
         <v>2873</v>
       </c>
       <c r="K552" s="2" t="n">
-        <v>902.0</v>
+        <v>941.0</v>
       </c>
       <c r="L552" s="2" t="s">
         <v>2871</v>
       </c>
       <c r="M552" s="2" t="n">
-        <v>14.0</v>
+        <v>77.0</v>
       </c>
       <c r="N552" s="2" t="s">
         <v>2874</v>
@@ -39056,37 +39056,37 @@
         <v>2891</v>
       </c>
       <c r="D556" s="2" t="n">
-        <v>376.0</v>
+        <v>566.0</v>
       </c>
       <c r="E556" s="2" t="s">
         <v>2892</v>
       </c>
       <c r="F556" s="2" t="n">
-        <v>10.0</v>
+        <v>0.0</v>
       </c>
       <c r="G556" s="2" t="n">
-        <v>0.0</v>
+        <v>115.0</v>
       </c>
       <c r="H556" s="2" t="s">
-        <v>2329</v>
+        <v>2893</v>
       </c>
       <c r="I556" s="2" t="n">
-        <v>1560.0</v>
+        <v>0.0</v>
       </c>
       <c r="J556" s="2" t="s">
-        <v>2893</v>
+        <v>2892</v>
       </c>
       <c r="K556" s="2" t="n">
-        <v>846.0</v>
+        <v>950.0</v>
       </c>
       <c r="L556" s="2" t="s">
-        <v>2329</v>
+        <v>2894</v>
       </c>
       <c r="M556" s="2" t="n">
-        <v>0.0</v>
+        <v>456.0</v>
       </c>
       <c r="N556" s="2" t="s">
-        <v>2894</v>
+        <v>2895</v>
       </c>
     </row>
     <row r="557">
@@ -39094,40 +39094,40 @@
         <v>556.0</v>
       </c>
       <c r="B557" s="2" t="s">
-        <v>2895</v>
+        <v>2896</v>
       </c>
       <c r="C557" s="2" t="s">
-        <v>2896</v>
+        <v>2897</v>
       </c>
       <c r="D557" s="2" t="n">
-        <v>566.0</v>
+        <v>376.0</v>
       </c>
       <c r="E557" s="2" t="s">
-        <v>2897</v>
+        <v>2898</v>
       </c>
       <c r="F557" s="2" t="n">
-        <v>0.0</v>
+        <v>10.0</v>
       </c>
       <c r="G557" s="2" t="n">
-        <v>115.0</v>
+        <v>0.0</v>
       </c>
       <c r="H557" s="2" t="s">
-        <v>2898</v>
+        <v>2329</v>
       </c>
       <c r="I557" s="2" t="n">
-        <v>0.0</v>
+        <v>1560.0</v>
       </c>
       <c r="J557" s="2" t="s">
-        <v>2897</v>
+        <v>2899</v>
       </c>
       <c r="K557" s="2" t="n">
-        <v>950.0</v>
+        <v>846.0</v>
       </c>
       <c r="L557" s="2" t="s">
-        <v>2899</v>
+        <v>2329</v>
       </c>
       <c r="M557" s="2" t="n">
-        <v>451.0</v>
+        <v>0.0</v>
       </c>
       <c r="N557" s="2" t="s">
         <v>2900</v>

</xml_diff>

<commit_message>
Add generated leaderboard data - 2024-05-24T20:09:59
</commit_message>
<xml_diff>
--- a/Leaderboards/CurrentCMRITLeaderboard2025.xlsx
+++ b/Leaderboards/CurrentCMRITLeaderboard2025.xlsx
@@ -98,7 +98,7 @@
     <t>pavanvasam577</t>
   </si>
   <si>
-    <t>70.32%</t>
+    <t>70.34%</t>
   </si>
   <si>
     <t>21R01A67F2</t>
@@ -959,7 +959,7 @@
     <t>21r01a0549</t>
   </si>
   <si>
-    <t>46.65%</t>
+    <t>46.67%</t>
   </si>
   <si>
     <t>21R01A66A0</t>
@@ -1409,6 +1409,18 @@
     <t>44.15%</t>
   </si>
   <si>
+    <t>21R01A0563</t>
+  </si>
+  <si>
+    <t>21r01a0563</t>
+  </si>
+  <si>
+    <t>shivathmika63</t>
+  </si>
+  <si>
+    <t>44.14%</t>
+  </si>
+  <si>
     <t>21R01A05P0</t>
   </si>
   <si>
@@ -1424,18 +1436,6 @@
     <t>44.11%</t>
   </si>
   <si>
-    <t>21R01A0563</t>
-  </si>
-  <si>
-    <t>21r01a0563</t>
-  </si>
-  <si>
-    <t>shivathmika63</t>
-  </si>
-  <si>
-    <t>44.07%</t>
-  </si>
-  <si>
     <t>21R01A0437</t>
   </si>
   <si>
@@ -1826,6 +1826,24 @@
     <t>41.17%</t>
   </si>
   <si>
+    <t>21R01A6632</t>
+  </si>
+  <si>
+    <t>CMRIT25_21R01A6632</t>
+  </si>
+  <si>
+    <t>21r016632</t>
+  </si>
+  <si>
+    <t>21r01a6632</t>
+  </si>
+  <si>
+    <t>cmr21r01a6632</t>
+  </si>
+  <si>
+    <t>41.07%</t>
+  </si>
+  <si>
     <t>21R01A67H6</t>
   </si>
   <si>
@@ -1838,24 +1856,6 @@
     <t>21r01a67h6</t>
   </si>
   <si>
-    <t>41.07%</t>
-  </si>
-  <si>
-    <t>21R01A6632</t>
-  </si>
-  <si>
-    <t>CMRIT25_21R01A6632</t>
-  </si>
-  <si>
-    <t>21r016632</t>
-  </si>
-  <si>
-    <t>21r01a6632</t>
-  </si>
-  <si>
-    <t>cmr21r01a6632</t>
-  </si>
-  <si>
     <t>21R01A7258</t>
   </si>
   <si>
@@ -2108,7 +2108,7 @@
     <t>bhavani2003</t>
   </si>
   <si>
-    <t>40.03%</t>
+    <t>40.04%</t>
   </si>
   <si>
     <t>21R01A6739</t>
@@ -4202,7 +4202,7 @@
     <t>21r01a66c41</t>
   </si>
   <si>
-    <t>34.42%</t>
+    <t>34.43%</t>
   </si>
   <si>
     <t>21R01A0421</t>
@@ -7796,6 +7796,18 @@
     <t>24.76%</t>
   </si>
   <si>
+    <t>22R05A0405</t>
+  </si>
+  <si>
+    <t>Cmrit25_22r05a0405</t>
+  </si>
+  <si>
+    <t>22r05a0405</t>
+  </si>
+  <si>
+    <t>cmr_22r05a0405</t>
+  </si>
+  <si>
     <t>21R01A6642</t>
   </si>
   <si>
@@ -7838,31 +7850,19 @@
     <t>24.73%</t>
   </si>
   <si>
-    <t>22R05A0405</t>
-  </si>
-  <si>
-    <t>Cmrit25_22r05a0405</t>
-  </si>
-  <si>
-    <t>22r05a0405</t>
-  </si>
-  <si>
-    <t>cmr_22r05a0405</t>
+    <t>21R01A6734</t>
+  </si>
+  <si>
+    <t>CMRIT25_21R01A6734</t>
+  </si>
+  <si>
+    <t>21r01a6734</t>
+  </si>
+  <si>
+    <t>r01a6734</t>
   </si>
   <si>
     <t>24.71%</t>
-  </si>
-  <si>
-    <t>21R01A6734</t>
-  </si>
-  <si>
-    <t>CMRIT25_21R01A6734</t>
-  </si>
-  <si>
-    <t>21r01a6734</t>
-  </si>
-  <si>
-    <t>r01a6734</t>
   </si>
   <si>
     <t>21R01A67E5</t>
@@ -14828,7 +14828,7 @@
         <v>826.0</v>
       </c>
       <c r="G4" s="2" t="n">
-        <v>425.0</v>
+        <v>442.0</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>26</v>
@@ -15664,7 +15664,7 @@
         <v>204.0</v>
       </c>
       <c r="G23" s="2" t="n">
-        <v>1198.0</v>
+        <v>1200.0</v>
       </c>
       <c r="H23" s="2" t="s">
         <v>128</v>
@@ -17160,7 +17160,7 @@
         <v>256.0</v>
       </c>
       <c r="G57" s="2" t="n">
-        <v>710.0</v>
+        <v>722.0</v>
       </c>
       <c r="H57" s="2" t="s">
         <v>312</v>
@@ -18424,40 +18424,40 @@
         <v>465</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="D86" s="2" t="n">
-        <v>834.0</v>
+        <v>860.0</v>
       </c>
       <c r="E86" s="2" t="s">
         <v>466</v>
       </c>
       <c r="F86" s="2" t="n">
-        <v>159.0</v>
+        <v>250.0</v>
       </c>
       <c r="G86" s="2" t="n">
-        <v>146.0</v>
+        <v>127.0</v>
       </c>
       <c r="H86" s="2" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="I86" s="2" t="n">
-        <v>1470.0</v>
+        <v>1301.0</v>
       </c>
       <c r="J86" s="2" t="s">
         <v>467</v>
       </c>
       <c r="K86" s="2" t="n">
-        <v>1262.0</v>
+        <v>1065.0</v>
       </c>
       <c r="L86" s="2" t="s">
+        <v>465</v>
+      </c>
+      <c r="M86" s="2" t="n">
+        <v>191.0</v>
+      </c>
+      <c r="N86" s="2" t="s">
         <v>468</v>
-      </c>
-      <c r="M86" s="2" t="n">
-        <v>465.0</v>
-      </c>
-      <c r="N86" s="2" t="s">
-        <v>469</v>
       </c>
     </row>
     <row r="87">
@@ -18465,40 +18465,40 @@
         <v>86.0</v>
       </c>
       <c r="B87" s="2" t="s">
+        <v>469</v>
+      </c>
+      <c r="C87" s="2" t="s">
+        <v>469</v>
+      </c>
+      <c r="D87" s="2" t="n">
+        <v>834.0</v>
+      </c>
+      <c r="E87" s="2" t="s">
         <v>470</v>
       </c>
-      <c r="C87" s="2" t="s">
+      <c r="F87" s="2" t="n">
+        <v>159.0</v>
+      </c>
+      <c r="G87" s="2" t="n">
+        <v>146.0</v>
+      </c>
+      <c r="H87" s="2" t="s">
+        <v>469</v>
+      </c>
+      <c r="I87" s="2" t="n">
+        <v>1470.0</v>
+      </c>
+      <c r="J87" s="2" t="s">
         <v>471</v>
       </c>
-      <c r="D87" s="2" t="n">
-        <v>860.0</v>
-      </c>
-      <c r="E87" s="2" t="s">
-        <v>471</v>
-      </c>
-      <c r="F87" s="2" t="n">
-        <v>250.0</v>
-      </c>
-      <c r="G87" s="2" t="n">
-        <v>79.0</v>
-      </c>
-      <c r="H87" s="2" t="s">
-        <v>471</v>
-      </c>
-      <c r="I87" s="2" t="n">
-        <v>1301.0</v>
-      </c>
-      <c r="J87" s="2" t="s">
+      <c r="K87" s="2" t="n">
+        <v>1262.0</v>
+      </c>
+      <c r="L87" s="2" t="s">
         <v>472</v>
       </c>
-      <c r="K87" s="2" t="n">
-        <v>1065.0</v>
-      </c>
-      <c r="L87" s="2" t="s">
-        <v>470</v>
-      </c>
       <c r="M87" s="2" t="n">
-        <v>191.0</v>
+        <v>465.0</v>
       </c>
       <c r="N87" s="2" t="s">
         <v>473</v>
@@ -19659,37 +19659,37 @@
         <v>605</v>
       </c>
       <c r="D114" s="2" t="n">
-        <v>828.0</v>
+        <v>706.0</v>
       </c>
       <c r="E114" s="2" t="s">
         <v>606</v>
       </c>
       <c r="F114" s="2" t="n">
-        <v>79.0</v>
+        <v>172.0</v>
       </c>
       <c r="G114" s="2" t="n">
-        <v>63.0</v>
+        <v>185.0</v>
       </c>
       <c r="H114" s="2" t="s">
-        <v>604</v>
+        <v>607</v>
       </c>
       <c r="I114" s="2" t="n">
-        <v>1602.0</v>
+        <v>1409.0</v>
       </c>
       <c r="J114" s="2" t="s">
-        <v>606</v>
+        <v>608</v>
       </c>
       <c r="K114" s="2" t="n">
-        <v>1375.0</v>
+        <v>1203.0</v>
       </c>
       <c r="L114" s="2" t="s">
         <v>607</v>
       </c>
       <c r="M114" s="2" t="n">
-        <v>367.0</v>
+        <v>436.0</v>
       </c>
       <c r="N114" s="2" t="s">
-        <v>608</v>
+        <v>609</v>
       </c>
     </row>
     <row r="115">
@@ -19697,43 +19697,43 @@
         <v>114.0</v>
       </c>
       <c r="B115" s="2" t="s">
+        <v>610</v>
+      </c>
+      <c r="C115" s="2" t="s">
+        <v>611</v>
+      </c>
+      <c r="D115" s="2" t="n">
+        <v>828.0</v>
+      </c>
+      <c r="E115" s="2" t="s">
+        <v>612</v>
+      </c>
+      <c r="F115" s="2" t="n">
+        <v>79.0</v>
+      </c>
+      <c r="G115" s="2" t="n">
+        <v>63.0</v>
+      </c>
+      <c r="H115" s="2" t="s">
+        <v>610</v>
+      </c>
+      <c r="I115" s="2" t="n">
+        <v>1602.0</v>
+      </c>
+      <c r="J115" s="2" t="s">
+        <v>612</v>
+      </c>
+      <c r="K115" s="2" t="n">
+        <v>1375.0</v>
+      </c>
+      <c r="L115" s="2" t="s">
+        <v>613</v>
+      </c>
+      <c r="M115" s="2" t="n">
+        <v>367.0</v>
+      </c>
+      <c r="N115" s="2" t="s">
         <v>609</v>
-      </c>
-      <c r="C115" s="2" t="s">
-        <v>610</v>
-      </c>
-      <c r="D115" s="2" t="n">
-        <v>706.0</v>
-      </c>
-      <c r="E115" s="2" t="s">
-        <v>611</v>
-      </c>
-      <c r="F115" s="2" t="n">
-        <v>172.0</v>
-      </c>
-      <c r="G115" s="2" t="n">
-        <v>182.0</v>
-      </c>
-      <c r="H115" s="2" t="s">
-        <v>612</v>
-      </c>
-      <c r="I115" s="2" t="n">
-        <v>1409.0</v>
-      </c>
-      <c r="J115" s="2" t="s">
-        <v>613</v>
-      </c>
-      <c r="K115" s="2" t="n">
-        <v>1203.0</v>
-      </c>
-      <c r="L115" s="2" t="s">
-        <v>612</v>
-      </c>
-      <c r="M115" s="2" t="n">
-        <v>436.0</v>
-      </c>
-      <c r="N115" s="2" t="s">
-        <v>608</v>
       </c>
     </row>
     <row r="116">
@@ -20416,7 +20416,7 @@
         <v>179.0</v>
       </c>
       <c r="G131" s="2" t="n">
-        <v>368.0</v>
+        <v>376.0</v>
       </c>
       <c r="H131" s="2" t="s">
         <v>694</v>
@@ -26268,7 +26268,7 @@
         <v>10.0</v>
       </c>
       <c r="G264" s="2" t="n">
-        <v>184.0</v>
+        <v>188.0</v>
       </c>
       <c r="H264" s="2" t="s">
         <v>1393</v>
@@ -31416,7 +31416,7 @@
         <v>10.0</v>
       </c>
       <c r="G381" s="2" t="n">
-        <v>156.0</v>
+        <v>160.0</v>
       </c>
       <c r="H381" s="2" t="s">
         <v>2001</v>
@@ -35860,7 +35860,7 @@
         <v>0.0</v>
       </c>
       <c r="G482" s="2" t="n">
-        <v>288.0</v>
+        <v>290.0</v>
       </c>
       <c r="H482" s="2" t="s">
         <v>2523</v>
@@ -36511,37 +36511,37 @@
         <v>2595</v>
       </c>
       <c r="D497" s="2" t="n">
-        <v>803.0</v>
+        <v>406.0</v>
       </c>
       <c r="E497" s="2" t="s">
-        <v>2595</v>
+        <v>2596</v>
       </c>
       <c r="F497" s="2" t="n">
-        <v>19.0</v>
+        <v>0.0</v>
       </c>
       <c r="G497" s="2" t="n">
-        <v>6.0</v>
+        <v>95.0</v>
       </c>
       <c r="H497" s="2" t="s">
-        <v>2595</v>
+        <v>2596</v>
       </c>
       <c r="I497" s="2" t="n">
-        <v>0.0</v>
+        <v>1514.0</v>
       </c>
       <c r="J497" s="2" t="s">
+        <v>2597</v>
+      </c>
+      <c r="K497" s="2" t="n">
+        <v>1007.0</v>
+      </c>
+      <c r="L497" s="2" t="s">
         <v>2596</v>
       </c>
-      <c r="K497" s="2" t="n">
-        <v>1069.0</v>
-      </c>
-      <c r="L497" s="2" t="s">
-        <v>2595</v>
-      </c>
       <c r="M497" s="2" t="n">
-        <v>30.0</v>
+        <v>207.0</v>
       </c>
       <c r="N497" s="2" t="s">
-        <v>2597</v>
+        <v>2593</v>
       </c>
     </row>
     <row r="498">
@@ -36555,37 +36555,37 @@
         <v>2599</v>
       </c>
       <c r="D498" s="2" t="n">
-        <v>752.0</v>
+        <v>803.0</v>
       </c>
       <c r="E498" s="2" t="s">
+        <v>2599</v>
+      </c>
+      <c r="F498" s="2" t="n">
+        <v>19.0</v>
+      </c>
+      <c r="G498" s="2" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="H498" s="2" t="s">
+        <v>2599</v>
+      </c>
+      <c r="I498" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="J498" s="2" t="s">
         <v>2600</v>
       </c>
-      <c r="F498" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="G498" s="2" t="n">
-        <v>10.0</v>
-      </c>
-      <c r="H498" s="2" t="s">
+      <c r="K498" s="2" t="n">
+        <v>1069.0</v>
+      </c>
+      <c r="L498" s="2" t="s">
+        <v>2599</v>
+      </c>
+      <c r="M498" s="2" t="n">
+        <v>30.0</v>
+      </c>
+      <c r="N498" s="2" t="s">
         <v>2601</v>
-      </c>
-      <c r="I498" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="J498" s="2" t="s">
-        <v>2602</v>
-      </c>
-      <c r="K498" s="2" t="n">
-        <v>1322.0</v>
-      </c>
-      <c r="L498" s="2" t="s">
-        <v>2603</v>
-      </c>
-      <c r="M498" s="2" t="n">
-        <v>69.0</v>
-      </c>
-      <c r="N498" s="2" t="s">
-        <v>2597</v>
       </c>
     </row>
     <row r="499">
@@ -36593,43 +36593,43 @@
         <v>498.0</v>
       </c>
       <c r="B499" s="2" t="s">
+        <v>2602</v>
+      </c>
+      <c r="C499" s="2" t="s">
+        <v>2603</v>
+      </c>
+      <c r="D499" s="2" t="n">
+        <v>752.0</v>
+      </c>
+      <c r="E499" s="2" t="s">
         <v>2604</v>
       </c>
-      <c r="C499" s="2" t="s">
-        <v>2604</v>
-      </c>
-      <c r="D499" s="2" t="n">
-        <v>359.0</v>
-      </c>
-      <c r="E499" s="2" t="s">
-        <v>1708</v>
-      </c>
       <c r="F499" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="G499" s="2" t="n">
-        <v>0.0</v>
+        <v>10.0</v>
       </c>
       <c r="H499" s="2" t="s">
         <v>2605</v>
       </c>
       <c r="I499" s="2" t="n">
-        <v>1551.0</v>
+        <v>0.0</v>
       </c>
       <c r="J499" s="2" t="s">
         <v>2606</v>
       </c>
       <c r="K499" s="2" t="n">
-        <v>1421.0</v>
+        <v>1322.0</v>
       </c>
       <c r="L499" s="2" t="s">
-        <v>2605</v>
+        <v>2607</v>
       </c>
       <c r="M499" s="2" t="n">
-        <v>5.0</v>
+        <v>69.0</v>
       </c>
       <c r="N499" s="2" t="s">
-        <v>2607</v>
+        <v>2601</v>
       </c>
     </row>
     <row r="500">
@@ -36640,40 +36640,40 @@
         <v>2608</v>
       </c>
       <c r="C500" s="2" t="s">
+        <v>2608</v>
+      </c>
+      <c r="D500" s="2" t="n">
+        <v>359.0</v>
+      </c>
+      <c r="E500" s="2" t="s">
+        <v>1708</v>
+      </c>
+      <c r="F500" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G500" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H500" s="2" t="s">
         <v>2609</v>
       </c>
-      <c r="D500" s="2" t="n">
-        <v>406.0</v>
-      </c>
-      <c r="E500" s="2" t="s">
+      <c r="I500" s="2" t="n">
+        <v>1551.0</v>
+      </c>
+      <c r="J500" s="2" t="s">
         <v>2610</v>
       </c>
-      <c r="F500" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="G500" s="2" t="n">
-        <v>63.0</v>
-      </c>
-      <c r="H500" s="2" t="s">
-        <v>2610</v>
-      </c>
-      <c r="I500" s="2" t="n">
-        <v>1514.0</v>
-      </c>
-      <c r="J500" s="2" t="s">
+      <c r="K500" s="2" t="n">
+        <v>1421.0</v>
+      </c>
+      <c r="L500" s="2" t="s">
+        <v>2609</v>
+      </c>
+      <c r="M500" s="2" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="N500" s="2" t="s">
         <v>2611</v>
-      </c>
-      <c r="K500" s="2" t="n">
-        <v>1007.0</v>
-      </c>
-      <c r="L500" s="2" t="s">
-        <v>2610</v>
-      </c>
-      <c r="M500" s="2" t="n">
-        <v>207.0</v>
-      </c>
-      <c r="N500" s="2" t="s">
-        <v>2612</v>
       </c>
     </row>
     <row r="501">
@@ -36681,43 +36681,43 @@
         <v>500.0</v>
       </c>
       <c r="B501" s="2" t="s">
+        <v>2612</v>
+      </c>
+      <c r="C501" s="2" t="s">
         <v>2613</v>
-      </c>
-      <c r="C501" s="2" t="s">
-        <v>2614</v>
       </c>
       <c r="D501" s="2" t="n">
         <v>728.0</v>
       </c>
       <c r="E501" s="2" t="s">
+        <v>2614</v>
+      </c>
+      <c r="F501" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G501" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H501" s="2" t="s">
+        <v>2612</v>
+      </c>
+      <c r="I501" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="J501" s="2" t="s">
         <v>2615</v>
-      </c>
-      <c r="F501" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="G501" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="H501" s="2" t="s">
-        <v>2613</v>
-      </c>
-      <c r="I501" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="J501" s="2" t="s">
-        <v>2616</v>
       </c>
       <c r="K501" s="2" t="n">
         <v>1198.0</v>
       </c>
       <c r="L501" s="2" t="s">
-        <v>2613</v>
+        <v>2612</v>
       </c>
       <c r="M501" s="2" t="n">
         <v>224.0</v>
       </c>
       <c r="N501" s="2" t="s">
-        <v>2612</v>
+        <v>2616</v>
       </c>
     </row>
     <row r="502">

</xml_diff>

<commit_message>
Add generated leaderboard data - 2024-06-01T20:15:00
</commit_message>
<xml_diff>
--- a/Leaderboards/CurrentCMRITLeaderboard2025.xlsx
+++ b/Leaderboards/CurrentCMRITLeaderboard2025.xlsx
@@ -1571,7 +1571,7 @@
     <t>cmr_21r01a04m7</t>
   </si>
   <si>
-    <t>43.36%</t>
+    <t>43.39%</t>
   </si>
   <si>
     <t>21R01A05K5</t>
@@ -5960,6 +5960,21 @@
     <t>30.65%</t>
   </si>
   <si>
+    <t>21R01A66A6</t>
+  </si>
+  <si>
+    <t>CMRIT25_21R01A66A6</t>
+  </si>
+  <si>
+    <t>21r01ac1bc</t>
+  </si>
+  <si>
+    <t>yousufansari</t>
+  </si>
+  <si>
+    <t>21r01a66a6</t>
+  </si>
+  <si>
     <t>21R01A04R4</t>
   </si>
   <si>
@@ -5973,21 +5988,6 @@
   </si>
   <si>
     <t>30.64%</t>
-  </si>
-  <si>
-    <t>21R01A66A6</t>
-  </si>
-  <si>
-    <t>CMRIT25_21R01A66A6</t>
-  </si>
-  <si>
-    <t>21r01ac1bc</t>
-  </si>
-  <si>
-    <t>yousufansari</t>
-  </si>
-  <si>
-    <t>21r01a66a6</t>
   </si>
   <si>
     <t>21R01A0507</t>
@@ -14748,7 +14748,7 @@
         <v>682.0</v>
       </c>
       <c r="G3" s="2" t="n">
-        <v>576.0</v>
+        <v>578.0</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>21</v>
@@ -18884,7 +18884,7 @@
         <v>50.0</v>
       </c>
       <c r="G97" s="2" t="n">
-        <v>450.0</v>
+        <v>468.0</v>
       </c>
       <c r="H97" s="2" t="s">
         <v>515</v>
@@ -31236,40 +31236,40 @@
         <v>1982</v>
       </c>
       <c r="C378" s="2" t="s">
-        <v>1982</v>
+        <v>1983</v>
       </c>
       <c r="D378" s="2" t="n">
-        <v>750.0</v>
+        <v>594.0</v>
       </c>
       <c r="E378" s="2" t="s">
-        <v>1983</v>
+        <v>1984</v>
       </c>
       <c r="F378" s="2" t="n">
-        <v>20.0</v>
+        <v>10.0</v>
       </c>
       <c r="G378" s="2" t="n">
-        <v>90.0</v>
+        <v>189.0</v>
       </c>
       <c r="H378" s="2" t="s">
-        <v>1982</v>
+        <v>1985</v>
       </c>
       <c r="I378" s="2" t="n">
-        <v>1425.0</v>
+        <v>1412.0</v>
       </c>
       <c r="J378" s="2" t="s">
-        <v>1984</v>
+        <v>1985</v>
       </c>
       <c r="K378" s="2" t="n">
-        <v>885.0</v>
+        <v>1173.0</v>
       </c>
       <c r="L378" s="2" t="s">
-        <v>1985</v>
+        <v>1986</v>
       </c>
       <c r="M378" s="2" t="n">
-        <v>81.0</v>
+        <v>313.0</v>
       </c>
       <c r="N378" s="2" t="s">
-        <v>1986</v>
+        <v>1981</v>
       </c>
     </row>
     <row r="379">
@@ -31280,40 +31280,40 @@
         <v>1987</v>
       </c>
       <c r="C379" s="2" t="s">
+        <v>1987</v>
+      </c>
+      <c r="D379" s="2" t="n">
+        <v>750.0</v>
+      </c>
+      <c r="E379" s="2" t="s">
         <v>1988</v>
       </c>
-      <c r="D379" s="2" t="n">
-        <v>594.0</v>
-      </c>
-      <c r="E379" s="2" t="s">
+      <c r="F379" s="2" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="G379" s="2" t="n">
+        <v>90.0</v>
+      </c>
+      <c r="H379" s="2" t="s">
+        <v>1987</v>
+      </c>
+      <c r="I379" s="2" t="n">
+        <v>1425.0</v>
+      </c>
+      <c r="J379" s="2" t="s">
         <v>1989</v>
       </c>
-      <c r="F379" s="2" t="n">
-        <v>10.0</v>
-      </c>
-      <c r="G379" s="2" t="n">
-        <v>187.0</v>
-      </c>
-      <c r="H379" s="2" t="s">
+      <c r="K379" s="2" t="n">
+        <v>885.0</v>
+      </c>
+      <c r="L379" s="2" t="s">
         <v>1990</v>
       </c>
-      <c r="I379" s="2" t="n">
-        <v>1412.0</v>
-      </c>
-      <c r="J379" s="2" t="s">
-        <v>1990</v>
-      </c>
-      <c r="K379" s="2" t="n">
-        <v>1173.0</v>
-      </c>
-      <c r="L379" s="2" t="s">
+      <c r="M379" s="2" t="n">
+        <v>81.0</v>
+      </c>
+      <c r="N379" s="2" t="s">
         <v>1991</v>
-      </c>
-      <c r="M379" s="2" t="n">
-        <v>313.0</v>
-      </c>
-      <c r="N379" s="2" t="s">
-        <v>1986</v>
       </c>
     </row>
     <row r="380">

</xml_diff>

<commit_message>
Add generated leaderboard data - 2024-06-17T20:11:03
</commit_message>
<xml_diff>
--- a/Leaderboards/CurrentCMRITLeaderboard2025.xlsx
+++ b/Leaderboards/CurrentCMRITLeaderboard2025.xlsx
@@ -650,7 +650,7 @@
     <t>21r01a6652</t>
   </si>
   <si>
-    <t>50.26</t>
+    <t>50.27</t>
   </si>
   <si>
     <t>21R01A67F8</t>
@@ -2924,24 +2924,24 @@
     <t>21r01a05g0</t>
   </si>
   <si>
+    <t>21R01A6676</t>
+  </si>
+  <si>
+    <t>CMRIT25_21r01a6676</t>
+  </si>
+  <si>
+    <t>21r01a0lxc</t>
+  </si>
+  <si>
+    <t>navaketanb1910</t>
+  </si>
+  <si>
+    <t>21r01a6676</t>
+  </si>
+  <si>
     <t>36.95</t>
   </si>
   <si>
-    <t>21R01A6676</t>
-  </si>
-  <si>
-    <t>CMRIT25_21r01a6676</t>
-  </si>
-  <si>
-    <t>21r01a0lxc</t>
-  </si>
-  <si>
-    <t>navaketanb1910</t>
-  </si>
-  <si>
-    <t>21r01a6676</t>
-  </si>
-  <si>
     <t>21R01A66A3</t>
   </si>
   <si>
@@ -3587,6 +3587,24 @@
     <t>35.4</t>
   </si>
   <si>
+    <t>21R01A7257</t>
+  </si>
+  <si>
+    <t>Vaishnavi_017</t>
+  </si>
+  <si>
+    <t>21r01ax608</t>
+  </si>
+  <si>
+    <t>vaishnavisingireddy</t>
+  </si>
+  <si>
+    <t>vaishnavisingi</t>
+  </si>
+  <si>
+    <t>vaishnavisingir1</t>
+  </si>
+  <si>
     <t>21R01A66C3</t>
   </si>
   <si>
@@ -3599,27 +3617,6 @@
     <t>sunitha_12</t>
   </si>
   <si>
-    <t>21R01A7257</t>
-  </si>
-  <si>
-    <t>Vaishnavi_017</t>
-  </si>
-  <si>
-    <t>21r01ax608</t>
-  </si>
-  <si>
-    <t>vaishnavisingireddy</t>
-  </si>
-  <si>
-    <t>vaishnavisingi</t>
-  </si>
-  <si>
-    <t>vaishnavisingir1</t>
-  </si>
-  <si>
-    <t>35.39</t>
-  </si>
-  <si>
     <t>21R01A05H8</t>
   </si>
   <si>
@@ -3671,6 +3668,24 @@
     <t>35.19</t>
   </si>
   <si>
+    <t>21R01A66C5</t>
+  </si>
+  <si>
+    <t>CMRIT25_21R01A66C5</t>
+  </si>
+  <si>
+    <t>21r01a66c5</t>
+  </si>
+  <si>
+    <t>T_DEVENDAR</t>
+  </si>
+  <si>
+    <t>devendar7987</t>
+  </si>
+  <si>
+    <t>35.17</t>
+  </si>
+  <si>
     <t>21R01A05A1</t>
   </si>
   <si>
@@ -3686,21 +3701,6 @@
     <t>35.15</t>
   </si>
   <si>
-    <t>21R01A66C5</t>
-  </si>
-  <si>
-    <t>CMRIT25_21R01A66C5</t>
-  </si>
-  <si>
-    <t>21r01a66c5</t>
-  </si>
-  <si>
-    <t>T_DEVENDAR</t>
-  </si>
-  <si>
-    <t>devendar7987</t>
-  </si>
-  <si>
     <t>21R01A04E6</t>
   </si>
   <si>
@@ -5837,6 +5837,24 @@
     <t>30.75</t>
   </si>
   <si>
+    <t>21R01A66A6</t>
+  </si>
+  <si>
+    <t>CMRIT25_21R01A66A6</t>
+  </si>
+  <si>
+    <t>21r01ac1bc</t>
+  </si>
+  <si>
+    <t>yousufansari</t>
+  </si>
+  <si>
+    <t>21r01a66a6</t>
+  </si>
+  <si>
+    <t>30.74</t>
+  </si>
+  <si>
     <t>22R05A6608</t>
   </si>
   <si>
@@ -5846,24 +5864,6 @@
     <t>abhishek4044</t>
   </si>
   <si>
-    <t>30.74</t>
-  </si>
-  <si>
-    <t>21R01A66A6</t>
-  </si>
-  <si>
-    <t>CMRIT25_21R01A66A6</t>
-  </si>
-  <si>
-    <t>21r01ac1bc</t>
-  </si>
-  <si>
-    <t>yousufansari</t>
-  </si>
-  <si>
-    <t>21r01a66a6</t>
-  </si>
-  <si>
     <t>21R01A05G5</t>
   </si>
   <si>
@@ -5969,6 +5969,21 @@
     <t>30.45</t>
   </si>
   <si>
+    <t>21R01A0516</t>
+  </si>
+  <si>
+    <t>CMRIT25_21R01A0516</t>
+  </si>
+  <si>
+    <t>21r01a0516</t>
+  </si>
+  <si>
+    <t>vinuthna_516</t>
+  </si>
+  <si>
+    <t>30.4</t>
+  </si>
+  <si>
     <t>21R01A04R9</t>
   </si>
   <si>
@@ -6068,21 +6083,6 @@
     <t>30.27</t>
   </si>
   <si>
-    <t>21R01A0516</t>
-  </si>
-  <si>
-    <t>CMRIT25_21R01A0516</t>
-  </si>
-  <si>
-    <t>21r01a0516</t>
-  </si>
-  <si>
-    <t>vinuthnagoud</t>
-  </si>
-  <si>
-    <t>30.26</t>
-  </si>
-  <si>
     <t>21R01A04R3</t>
   </si>
   <si>
@@ -7604,6 +7604,24 @@
     <t>24.96</t>
   </si>
   <si>
+    <t>21R01A0541</t>
+  </si>
+  <si>
+    <t>21R01A0541@cmritonline.ac.in</t>
+  </si>
+  <si>
+    <t>vinuthnna_reddy</t>
+  </si>
+  <si>
+    <t>vin_21r01a0541</t>
+  </si>
+  <si>
+    <t>21R01A0541cmritonline.ac.in</t>
+  </si>
+  <si>
+    <t>24.94</t>
+  </si>
+  <si>
     <t>21R01A0532</t>
   </si>
   <si>
@@ -7646,24 +7664,6 @@
     <t>24.87</t>
   </si>
   <si>
-    <t>21R01A0541</t>
-  </si>
-  <si>
-    <t>21R01A0541@cmritonline.ac.in</t>
-  </si>
-  <si>
-    <t>vinuthnna_reddy</t>
-  </si>
-  <si>
-    <t>vin_21r01a0541</t>
-  </si>
-  <si>
-    <t>21R01A0541cmritonline.ac.in</t>
-  </si>
-  <si>
-    <t>24.86</t>
-  </si>
-  <si>
     <t>21R01A04P0</t>
   </si>
   <si>
@@ -10877,7 +10877,7 @@
     <t>bonagiridilipku1</t>
   </si>
   <si>
-    <t>10.42</t>
+    <t>10.47</t>
   </si>
   <si>
     <t>21R01A04G2</t>
@@ -16338,7 +16338,7 @@
         <v>409.0</v>
       </c>
       <c r="G39" s="2" t="n">
-        <v>126.0</v>
+        <v>130.0</v>
       </c>
       <c r="H39" s="2" t="s">
         <v>209</v>
@@ -16602,7 +16602,7 @@
         <v>389.0</v>
       </c>
       <c r="G45" s="2" t="n">
-        <v>414.0</v>
+        <v>418.0</v>
       </c>
       <c r="H45" s="2" t="s">
         <v>241</v>
@@ -22762,7 +22762,7 @@
         <v>79.0</v>
       </c>
       <c r="G185" s="2" t="n">
-        <v>802.0</v>
+        <v>810.0</v>
       </c>
       <c r="H185" s="2" t="s">
         <v>967</v>
@@ -22783,7 +22783,7 @@
         <v>60.0</v>
       </c>
       <c r="N185" s="2" t="s">
-        <v>970</v>
+        <v>963</v>
       </c>
     </row>
     <row r="186">
@@ -22791,16 +22791,16 @@
         <v>185.0</v>
       </c>
       <c r="B186" s="2" t="s">
+        <v>970</v>
+      </c>
+      <c r="C186" s="2" t="s">
         <v>971</v>
-      </c>
-      <c r="C186" s="2" t="s">
-        <v>972</v>
       </c>
       <c r="D186" s="2" t="n">
         <v>730.0</v>
       </c>
       <c r="E186" s="2" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="F186" s="2" t="n">
         <v>40.0</v>
@@ -22809,25 +22809,25 @@
         <v>118.0</v>
       </c>
       <c r="H186" s="2" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
       <c r="I186" s="2" t="n">
         <v>1367.0</v>
       </c>
       <c r="J186" s="2" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
       <c r="K186" s="2" t="n">
         <v>1423.0</v>
       </c>
       <c r="L186" s="2" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
       <c r="M186" s="2" t="n">
         <v>443.0</v>
       </c>
       <c r="N186" s="2" t="s">
-        <v>970</v>
+        <v>975</v>
       </c>
     </row>
     <row r="187">
@@ -24645,34 +24645,34 @@
         <v>1192</v>
       </c>
       <c r="D228" s="2" t="n">
-        <v>767.0</v>
+        <v>692.0</v>
       </c>
       <c r="E228" s="2" t="s">
         <v>1193</v>
       </c>
       <c r="F228" s="2" t="n">
-        <v>30.0</v>
+        <v>10.0</v>
       </c>
       <c r="G228" s="2" t="n">
         <v>138.0</v>
       </c>
       <c r="H228" s="2" t="s">
-        <v>1191</v>
+        <v>1194</v>
       </c>
       <c r="I228" s="2" t="n">
-        <v>1432.0</v>
+        <v>1472.0</v>
       </c>
       <c r="J228" s="2" t="s">
-        <v>1194</v>
+        <v>1195</v>
       </c>
       <c r="K228" s="2" t="n">
-        <v>954.0</v>
+        <v>1409.0</v>
       </c>
       <c r="L228" s="2" t="s">
-        <v>1193</v>
+        <v>1196</v>
       </c>
       <c r="M228" s="2" t="n">
-        <v>514.0</v>
+        <v>434.0</v>
       </c>
       <c r="N228" s="2" t="s">
         <v>1190</v>
@@ -24683,43 +24683,43 @@
         <v>228.0</v>
       </c>
       <c r="B229" s="2" t="s">
-        <v>1195</v>
+        <v>1197</v>
       </c>
       <c r="C229" s="2" t="s">
-        <v>1196</v>
+        <v>1198</v>
       </c>
       <c r="D229" s="2" t="n">
-        <v>692.0</v>
+        <v>767.0</v>
       </c>
       <c r="E229" s="2" t="s">
+        <v>1199</v>
+      </c>
+      <c r="F229" s="2" t="n">
+        <v>30.0</v>
+      </c>
+      <c r="G229" s="2" t="n">
+        <v>138.0</v>
+      </c>
+      <c r="H229" s="2" t="s">
         <v>1197</v>
       </c>
-      <c r="F229" s="2" t="n">
-        <v>10.0</v>
-      </c>
-      <c r="G229" s="2" t="n">
-        <v>136.0</v>
-      </c>
-      <c r="H229" s="2" t="s">
-        <v>1198</v>
-      </c>
       <c r="I229" s="2" t="n">
-        <v>1472.0</v>
+        <v>1432.0</v>
       </c>
       <c r="J229" s="2" t="s">
+        <v>1200</v>
+      </c>
+      <c r="K229" s="2" t="n">
+        <v>954.0</v>
+      </c>
+      <c r="L229" s="2" t="s">
         <v>1199</v>
       </c>
-      <c r="K229" s="2" t="n">
-        <v>1409.0</v>
-      </c>
-      <c r="L229" s="2" t="s">
-        <v>1200</v>
-      </c>
       <c r="M229" s="2" t="n">
-        <v>434.0</v>
+        <v>514.0</v>
       </c>
       <c r="N229" s="2" t="s">
-        <v>1201</v>
+        <v>1190</v>
       </c>
     </row>
     <row r="230">
@@ -24727,16 +24727,16 @@
         <v>229.0</v>
       </c>
       <c r="B230" s="2" t="s">
+        <v>1201</v>
+      </c>
+      <c r="C230" s="2" t="s">
         <v>1202</v>
-      </c>
-      <c r="C230" s="2" t="s">
-        <v>1203</v>
       </c>
       <c r="D230" s="2" t="n">
         <v>798.0</v>
       </c>
       <c r="E230" s="2" t="s">
-        <v>1204</v>
+        <v>1203</v>
       </c>
       <c r="F230" s="2" t="n">
         <v>69.0</v>
@@ -24745,25 +24745,25 @@
         <v>66.0</v>
       </c>
       <c r="H230" s="2" t="s">
-        <v>1204</v>
+        <v>1203</v>
       </c>
       <c r="I230" s="2" t="n">
         <v>1536.0</v>
       </c>
       <c r="J230" s="2" t="s">
-        <v>1205</v>
+        <v>1204</v>
       </c>
       <c r="K230" s="2" t="n">
         <v>1083.0</v>
       </c>
       <c r="L230" s="2" t="s">
-        <v>1204</v>
+        <v>1203</v>
       </c>
       <c r="M230" s="2" t="n">
         <v>83.0</v>
       </c>
       <c r="N230" s="2" t="s">
-        <v>1206</v>
+        <v>1205</v>
       </c>
     </row>
     <row r="231">
@@ -24771,16 +24771,16 @@
         <v>230.0</v>
       </c>
       <c r="B231" s="2" t="s">
+        <v>1206</v>
+      </c>
+      <c r="C231" s="2" t="s">
         <v>1207</v>
-      </c>
-      <c r="C231" s="2" t="s">
-        <v>1208</v>
       </c>
       <c r="D231" s="2" t="n">
         <v>893.0</v>
       </c>
       <c r="E231" s="2" t="s">
-        <v>1209</v>
+        <v>1208</v>
       </c>
       <c r="F231" s="2" t="n">
         <v>30.0</v>
@@ -24789,25 +24789,25 @@
         <v>68.0</v>
       </c>
       <c r="H231" s="2" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
       <c r="I231" s="2" t="n">
         <v>1329.0</v>
       </c>
       <c r="J231" s="2" t="s">
-        <v>1211</v>
+        <v>1210</v>
       </c>
       <c r="K231" s="2" t="n">
         <v>1188.0</v>
       </c>
       <c r="L231" s="2" t="s">
-        <v>1208</v>
+        <v>1207</v>
       </c>
       <c r="M231" s="2" t="n">
         <v>73.0</v>
       </c>
       <c r="N231" s="2" t="s">
-        <v>1212</v>
+        <v>1211</v>
       </c>
     </row>
     <row r="232">
@@ -24815,16 +24815,16 @@
         <v>231.0</v>
       </c>
       <c r="B232" s="2" t="s">
+        <v>1212</v>
+      </c>
+      <c r="C232" s="2" t="s">
         <v>1213</v>
-      </c>
-      <c r="C232" s="2" t="s">
-        <v>1214</v>
       </c>
       <c r="D232" s="2" t="n">
         <v>742.0</v>
       </c>
       <c r="E232" s="2" t="s">
-        <v>1215</v>
+        <v>1214</v>
       </c>
       <c r="F232" s="2" t="n">
         <v>60.0</v>
@@ -24833,25 +24833,25 @@
         <v>21.0</v>
       </c>
       <c r="H232" s="2" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
       <c r="I232" s="2" t="n">
         <v>1552.0</v>
       </c>
       <c r="J232" s="2" t="s">
-        <v>1217</v>
+        <v>1216</v>
       </c>
       <c r="K232" s="2" t="n">
         <v>1361.0</v>
       </c>
       <c r="L232" s="2" t="s">
-        <v>1214</v>
+        <v>1213</v>
       </c>
       <c r="M232" s="2" t="n">
         <v>43.0</v>
       </c>
       <c r="N232" s="2" t="s">
-        <v>1218</v>
+        <v>1217</v>
       </c>
     </row>
     <row r="233">
@@ -24859,40 +24859,40 @@
         <v>232.0</v>
       </c>
       <c r="B233" s="2" t="s">
+        <v>1218</v>
+      </c>
+      <c r="C233" s="2" t="s">
         <v>1219</v>
       </c>
-      <c r="C233" s="2" t="s">
+      <c r="D233" s="2" t="n">
+        <v>745.0</v>
+      </c>
+      <c r="E233" s="2" t="s">
         <v>1220</v>
       </c>
-      <c r="D233" s="2" t="n">
-        <v>617.0</v>
-      </c>
-      <c r="E233" s="2" t="s">
+      <c r="F233" s="2" t="n">
+        <v>79.0</v>
+      </c>
+      <c r="G233" s="2" t="n">
+        <v>446.0</v>
+      </c>
+      <c r="H233" s="2" t="s">
         <v>1221</v>
       </c>
-      <c r="F233" s="2" t="n">
-        <v>105.0</v>
-      </c>
-      <c r="G233" s="2" t="n">
-        <v>105.0</v>
-      </c>
-      <c r="H233" s="2" t="s">
-        <v>1219</v>
-      </c>
       <c r="I233" s="2" t="n">
-        <v>1477.0</v>
+        <v>1420.0</v>
       </c>
       <c r="J233" s="2" t="s">
         <v>1222</v>
       </c>
       <c r="K233" s="2" t="n">
-        <v>1167.0</v>
+        <v>895.0</v>
       </c>
       <c r="L233" s="2" t="s">
-        <v>1219</v>
+        <v>1218</v>
       </c>
       <c r="M233" s="2" t="n">
-        <v>330.0</v>
+        <v>303.0</v>
       </c>
       <c r="N233" s="2" t="s">
         <v>1223</v>
@@ -24909,37 +24909,37 @@
         <v>1225</v>
       </c>
       <c r="D234" s="2" t="n">
-        <v>745.0</v>
+        <v>617.0</v>
       </c>
       <c r="E234" s="2" t="s">
         <v>1226</v>
       </c>
       <c r="F234" s="2" t="n">
-        <v>79.0</v>
+        <v>105.0</v>
       </c>
       <c r="G234" s="2" t="n">
-        <v>430.0</v>
+        <v>105.0</v>
       </c>
       <c r="H234" s="2" t="s">
+        <v>1224</v>
+      </c>
+      <c r="I234" s="2" t="n">
+        <v>1477.0</v>
+      </c>
+      <c r="J234" s="2" t="s">
         <v>1227</v>
       </c>
-      <c r="I234" s="2" t="n">
-        <v>1420.0</v>
-      </c>
-      <c r="J234" s="2" t="s">
-        <v>1228</v>
-      </c>
       <c r="K234" s="2" t="n">
-        <v>895.0</v>
+        <v>1167.0</v>
       </c>
       <c r="L234" s="2" t="s">
         <v>1224</v>
       </c>
       <c r="M234" s="2" t="n">
-        <v>303.0</v>
+        <v>330.0</v>
       </c>
       <c r="N234" s="2" t="s">
-        <v>1223</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="235">
@@ -30981,37 +30981,37 @@
         <v>1942</v>
       </c>
       <c r="D372" s="2" t="n">
-        <v>739.0</v>
+        <v>594.0</v>
       </c>
       <c r="E372" s="2" t="s">
-        <v>1942</v>
+        <v>1943</v>
       </c>
       <c r="F372" s="2" t="n">
-        <v>0.0</v>
+        <v>10.0</v>
       </c>
       <c r="G372" s="2" t="n">
-        <v>8.0</v>
+        <v>239.0</v>
       </c>
       <c r="H372" s="2" t="s">
-        <v>1942</v>
+        <v>1944</v>
       </c>
       <c r="I372" s="2" t="n">
-        <v>1432.0</v>
+        <v>1412.0</v>
       </c>
       <c r="J372" s="2" t="s">
-        <v>1943</v>
+        <v>1944</v>
       </c>
       <c r="K372" s="2" t="n">
-        <v>1119.0</v>
+        <v>1179.0</v>
       </c>
       <c r="L372" s="2" t="s">
-        <v>1942</v>
+        <v>1945</v>
       </c>
       <c r="M372" s="2" t="n">
-        <v>57.0</v>
+        <v>313.0</v>
       </c>
       <c r="N372" s="2" t="s">
-        <v>1944</v>
+        <v>1946</v>
       </c>
     </row>
     <row r="373">
@@ -31019,43 +31019,43 @@
         <v>372.0</v>
       </c>
       <c r="B373" s="2" t="s">
-        <v>1945</v>
+        <v>1947</v>
       </c>
       <c r="C373" s="2" t="s">
-        <v>1946</v>
+        <v>1948</v>
       </c>
       <c r="D373" s="2" t="n">
-        <v>594.0</v>
+        <v>739.0</v>
       </c>
       <c r="E373" s="2" t="s">
-        <v>1947</v>
+        <v>1948</v>
       </c>
       <c r="F373" s="2" t="n">
-        <v>10.0</v>
+        <v>0.0</v>
       </c>
       <c r="G373" s="2" t="n">
-        <v>235.0</v>
+        <v>8.0</v>
       </c>
       <c r="H373" s="2" t="s">
         <v>1948</v>
       </c>
       <c r="I373" s="2" t="n">
-        <v>1412.0</v>
+        <v>1432.0</v>
       </c>
       <c r="J373" s="2" t="s">
+        <v>1949</v>
+      </c>
+      <c r="K373" s="2" t="n">
+        <v>1119.0</v>
+      </c>
+      <c r="L373" s="2" t="s">
         <v>1948</v>
       </c>
-      <c r="K373" s="2" t="n">
-        <v>1179.0</v>
-      </c>
-      <c r="L373" s="2" t="s">
-        <v>1949</v>
-      </c>
       <c r="M373" s="2" t="n">
-        <v>313.0</v>
+        <v>57.0</v>
       </c>
       <c r="N373" s="2" t="s">
-        <v>1944</v>
+        <v>1946</v>
       </c>
     </row>
     <row r="374">
@@ -31099,7 +31099,7 @@
         <v>80.0</v>
       </c>
       <c r="N374" s="2" t="s">
-        <v>1944</v>
+        <v>1946</v>
       </c>
     </row>
     <row r="375">
@@ -31377,37 +31377,37 @@
         <v>1986</v>
       </c>
       <c r="D381" s="2" t="n">
-        <v>621.0</v>
+        <v>604.0</v>
       </c>
       <c r="E381" s="2" t="s">
         <v>1987</v>
       </c>
       <c r="F381" s="2" t="n">
-        <v>20.0</v>
+        <v>245.0</v>
       </c>
       <c r="G381" s="2" t="n">
-        <v>98.0</v>
+        <v>207.0</v>
       </c>
       <c r="H381" s="2" t="s">
+        <v>1987</v>
+      </c>
+      <c r="I381" s="2" t="n">
+        <v>1416.0</v>
+      </c>
+      <c r="J381" s="2" t="s">
         <v>1988</v>
       </c>
-      <c r="I381" s="2" t="n">
-        <v>1628.0</v>
-      </c>
-      <c r="J381" s="2" t="s">
+      <c r="K381" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L381" s="2" t="s">
+        <v>1987</v>
+      </c>
+      <c r="M381" s="2" t="n">
+        <v>15.0</v>
+      </c>
+      <c r="N381" s="2" t="s">
         <v>1989</v>
-      </c>
-      <c r="K381" s="2" t="n">
-        <v>1123.0</v>
-      </c>
-      <c r="L381" s="2" t="s">
-        <v>1988</v>
-      </c>
-      <c r="M381" s="2" t="n">
-        <v>72.0</v>
-      </c>
-      <c r="N381" s="2" t="s">
-        <v>1990</v>
       </c>
     </row>
     <row r="382">
@@ -31415,43 +31415,43 @@
         <v>381.0</v>
       </c>
       <c r="B382" s="2" t="s">
+        <v>1990</v>
+      </c>
+      <c r="C382" s="2" t="s">
         <v>1991</v>
       </c>
-      <c r="C382" s="2" t="s">
+      <c r="D382" s="2" t="n">
+        <v>621.0</v>
+      </c>
+      <c r="E382" s="2" t="s">
         <v>1992</v>
       </c>
-      <c r="D382" s="2" t="n">
-        <v>585.0</v>
-      </c>
-      <c r="E382" s="2" t="s">
+      <c r="F382" s="2" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="G382" s="2" t="n">
+        <v>98.0</v>
+      </c>
+      <c r="H382" s="2" t="s">
         <v>1993</v>
       </c>
-      <c r="F382" s="2" t="n">
-        <v>69.0</v>
-      </c>
-      <c r="G382" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="H382" s="2" t="s">
+      <c r="I382" s="2" t="n">
+        <v>1628.0</v>
+      </c>
+      <c r="J382" s="2" t="s">
         <v>1994</v>
       </c>
-      <c r="I382" s="2" t="n">
-        <v>1380.0</v>
-      </c>
-      <c r="J382" s="2" t="s">
-        <v>1995</v>
-      </c>
       <c r="K382" s="2" t="n">
-        <v>954.0</v>
+        <v>1123.0</v>
       </c>
       <c r="L382" s="2" t="s">
         <v>1993</v>
       </c>
       <c r="M382" s="2" t="n">
-        <v>238.0</v>
+        <v>72.0</v>
       </c>
       <c r="N382" s="2" t="s">
-        <v>1996</v>
+        <v>1995</v>
       </c>
     </row>
     <row r="383">
@@ -31459,40 +31459,40 @@
         <v>382.0</v>
       </c>
       <c r="B383" s="2" t="s">
+        <v>1996</v>
+      </c>
+      <c r="C383" s="2" t="s">
         <v>1997</v>
       </c>
-      <c r="C383" s="2" t="s">
+      <c r="D383" s="2" t="n">
+        <v>585.0</v>
+      </c>
+      <c r="E383" s="2" t="s">
         <v>1998</v>
       </c>
-      <c r="D383" s="2" t="n">
-        <v>768.0</v>
-      </c>
-      <c r="E383" s="2" t="s">
-        <v>1999</v>
-      </c>
       <c r="F383" s="2" t="n">
-        <v>25.0</v>
+        <v>69.0</v>
       </c>
       <c r="G383" s="2" t="n">
-        <v>8.0</v>
+        <v>0.0</v>
       </c>
       <c r="H383" s="2" t="s">
         <v>1999</v>
       </c>
       <c r="I383" s="2" t="n">
-        <v>1268.0</v>
+        <v>1380.0</v>
       </c>
       <c r="J383" s="2" t="s">
         <v>2000</v>
       </c>
       <c r="K383" s="2" t="n">
-        <v>920.0</v>
+        <v>954.0</v>
       </c>
       <c r="L383" s="2" t="s">
-        <v>1999</v>
+        <v>1998</v>
       </c>
       <c r="M383" s="2" t="n">
-        <v>65.0</v>
+        <v>238.0</v>
       </c>
       <c r="N383" s="2" t="s">
         <v>2001</v>
@@ -31509,37 +31509,37 @@
         <v>2003</v>
       </c>
       <c r="D384" s="2" t="n">
-        <v>734.0</v>
+        <v>768.0</v>
       </c>
       <c r="E384" s="2" t="s">
         <v>2004</v>
       </c>
       <c r="F384" s="2" t="n">
-        <v>10.0</v>
+        <v>25.0</v>
       </c>
       <c r="G384" s="2" t="n">
-        <v>7.0</v>
+        <v>8.0</v>
       </c>
       <c r="H384" s="2" t="s">
+        <v>2004</v>
+      </c>
+      <c r="I384" s="2" t="n">
+        <v>1268.0</v>
+      </c>
+      <c r="J384" s="2" t="s">
         <v>2005</v>
       </c>
-      <c r="I384" s="2" t="n">
-        <v>1331.0</v>
-      </c>
-      <c r="J384" s="2" t="s">
+      <c r="K384" s="2" t="n">
+        <v>920.0</v>
+      </c>
+      <c r="L384" s="2" t="s">
+        <v>2004</v>
+      </c>
+      <c r="M384" s="2" t="n">
+        <v>65.0</v>
+      </c>
+      <c r="N384" s="2" t="s">
         <v>2006</v>
-      </c>
-      <c r="K384" s="2" t="n">
-        <v>1071.0</v>
-      </c>
-      <c r="L384" s="2" t="s">
-        <v>2005</v>
-      </c>
-      <c r="M384" s="2" t="n">
-        <v>70.0</v>
-      </c>
-      <c r="N384" s="2" t="s">
-        <v>2001</v>
       </c>
     </row>
     <row r="385">
@@ -31553,37 +31553,37 @@
         <v>2008</v>
       </c>
       <c r="D385" s="2" t="n">
-        <v>703.0</v>
+        <v>734.0</v>
       </c>
       <c r="E385" s="2" t="s">
-        <v>2007</v>
+        <v>2009</v>
       </c>
       <c r="F385" s="2" t="n">
-        <v>0.0</v>
+        <v>10.0</v>
       </c>
       <c r="G385" s="2" t="n">
-        <v>0.0</v>
+        <v>7.0</v>
       </c>
       <c r="H385" s="2" t="s">
-        <v>2009</v>
+        <v>2010</v>
       </c>
       <c r="I385" s="2" t="n">
-        <v>1367.0</v>
+        <v>1331.0</v>
       </c>
       <c r="J385" s="2" t="s">
+        <v>2011</v>
+      </c>
+      <c r="K385" s="2" t="n">
+        <v>1071.0</v>
+      </c>
+      <c r="L385" s="2" t="s">
         <v>2010</v>
       </c>
-      <c r="K385" s="2" t="n">
-        <v>1243.0</v>
-      </c>
-      <c r="L385" s="2" t="s">
-        <v>2011</v>
-      </c>
       <c r="M385" s="2" t="n">
-        <v>45.0</v>
+        <v>70.0</v>
       </c>
       <c r="N385" s="2" t="s">
-        <v>2001</v>
+        <v>2006</v>
       </c>
     </row>
     <row r="386">
@@ -31597,37 +31597,37 @@
         <v>2013</v>
       </c>
       <c r="D386" s="2" t="n">
-        <v>657.0</v>
+        <v>703.0</v>
       </c>
       <c r="E386" s="2" t="s">
+        <v>2012</v>
+      </c>
+      <c r="F386" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G386" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H386" s="2" t="s">
         <v>2014</v>
       </c>
-      <c r="F386" s="2" t="n">
-        <v>10.0</v>
-      </c>
-      <c r="G386" s="2" t="n">
-        <v>133.0</v>
-      </c>
-      <c r="H386" s="2" t="s">
+      <c r="I386" s="2" t="n">
+        <v>1367.0</v>
+      </c>
+      <c r="J386" s="2" t="s">
         <v>2015</v>
       </c>
-      <c r="I386" s="2" t="n">
-        <v>1385.0</v>
-      </c>
-      <c r="J386" s="2" t="s">
+      <c r="K386" s="2" t="n">
+        <v>1243.0</v>
+      </c>
+      <c r="L386" s="2" t="s">
         <v>2016</v>
       </c>
-      <c r="K386" s="2" t="n">
-        <v>1261.0</v>
-      </c>
-      <c r="L386" s="2" t="s">
-        <v>2015</v>
-      </c>
       <c r="M386" s="2" t="n">
-        <v>65.0</v>
+        <v>45.0</v>
       </c>
       <c r="N386" s="2" t="s">
-        <v>2017</v>
+        <v>2006</v>
       </c>
     </row>
     <row r="387">
@@ -31635,40 +31635,40 @@
         <v>386.0</v>
       </c>
       <c r="B387" s="2" t="s">
+        <v>2017</v>
+      </c>
+      <c r="C387" s="2" t="s">
         <v>2018</v>
       </c>
-      <c r="C387" s="2" t="s">
+      <c r="D387" s="2" t="n">
+        <v>657.0</v>
+      </c>
+      <c r="E387" s="2" t="s">
         <v>2019</v>
       </c>
-      <c r="D387" s="2" t="n">
-        <v>604.0</v>
-      </c>
-      <c r="E387" s="2" t="s">
-        <v>2020</v>
-      </c>
       <c r="F387" s="2" t="n">
-        <v>245.0</v>
+        <v>10.0</v>
       </c>
       <c r="G387" s="2" t="n">
-        <v>115.0</v>
+        <v>133.0</v>
       </c>
       <c r="H387" s="2" t="s">
         <v>2020</v>
       </c>
       <c r="I387" s="2" t="n">
-        <v>1416.0</v>
+        <v>1385.0</v>
       </c>
       <c r="J387" s="2" t="s">
         <v>2021</v>
       </c>
       <c r="K387" s="2" t="n">
-        <v>0.0</v>
+        <v>1261.0</v>
       </c>
       <c r="L387" s="2" t="s">
         <v>2020</v>
       </c>
       <c r="M387" s="2" t="n">
-        <v>15.0</v>
+        <v>65.0</v>
       </c>
       <c r="N387" s="2" t="s">
         <v>2022</v>
@@ -36041,37 +36041,37 @@
         <v>2531</v>
       </c>
       <c r="D487" s="2" t="n">
-        <v>371.0</v>
+        <v>0.0</v>
       </c>
       <c r="E487" s="2" t="s">
-        <v>2532</v>
+        <v>2530</v>
       </c>
       <c r="F487" s="2" t="n">
-        <v>20.0</v>
+        <v>309.0</v>
       </c>
       <c r="G487" s="2" t="n">
-        <v>281.0</v>
+        <v>102.0</v>
       </c>
       <c r="H487" s="2" t="s">
         <v>2532</v>
       </c>
       <c r="I487" s="2" t="n">
-        <v>1373.0</v>
+        <v>1353.0</v>
       </c>
       <c r="J487" s="2" t="s">
         <v>2533</v>
       </c>
       <c r="K487" s="2" t="n">
-        <v>1090.0</v>
+        <v>890.0</v>
       </c>
       <c r="L487" s="2" t="s">
-        <v>2532</v>
+        <v>2534</v>
       </c>
       <c r="M487" s="2" t="n">
-        <v>216.0</v>
+        <v>0.0</v>
       </c>
       <c r="N487" s="2" t="s">
-        <v>2534</v>
+        <v>2535</v>
       </c>
     </row>
     <row r="488">
@@ -36079,43 +36079,43 @@
         <v>487.0</v>
       </c>
       <c r="B488" s="2" t="s">
-        <v>2535</v>
+        <v>2536</v>
       </c>
       <c r="C488" s="2" t="s">
-        <v>2536</v>
+        <v>2537</v>
       </c>
       <c r="D488" s="2" t="n">
-        <v>720.0</v>
+        <v>371.0</v>
       </c>
       <c r="E488" s="2" t="s">
-        <v>2535</v>
+        <v>2538</v>
       </c>
       <c r="F488" s="2" t="n">
-        <v>0.0</v>
+        <v>20.0</v>
       </c>
       <c r="G488" s="2" t="n">
-        <v>80.0</v>
+        <v>281.0</v>
       </c>
       <c r="H488" s="2" t="s">
-        <v>2537</v>
+        <v>2538</v>
       </c>
       <c r="I488" s="2" t="n">
-        <v>0.0</v>
+        <v>1373.0</v>
       </c>
       <c r="J488" s="2" t="s">
+        <v>2539</v>
+      </c>
+      <c r="K488" s="2" t="n">
+        <v>1090.0</v>
+      </c>
+      <c r="L488" s="2" t="s">
         <v>2538</v>
       </c>
-      <c r="K488" s="2" t="n">
-        <v>1200.0</v>
-      </c>
-      <c r="L488" s="2" t="s">
-        <v>2535</v>
-      </c>
       <c r="M488" s="2" t="n">
-        <v>252.0</v>
+        <v>216.0</v>
       </c>
       <c r="N488" s="2" t="s">
-        <v>2539</v>
+        <v>2540</v>
       </c>
     </row>
     <row r="489">
@@ -36123,43 +36123,43 @@
         <v>488.0</v>
       </c>
       <c r="B489" s="2" t="s">
-        <v>2540</v>
+        <v>2541</v>
       </c>
       <c r="C489" s="2" t="s">
+        <v>2542</v>
+      </c>
+      <c r="D489" s="2" t="n">
+        <v>720.0</v>
+      </c>
+      <c r="E489" s="2" t="s">
         <v>2541</v>
       </c>
-      <c r="D489" s="2" t="n">
-        <v>730.0</v>
-      </c>
-      <c r="E489" s="2" t="s">
-        <v>2540</v>
-      </c>
       <c r="F489" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="G489" s="2" t="n">
-        <v>125.0</v>
+        <v>80.0</v>
       </c>
       <c r="H489" s="2" t="s">
-        <v>2542</v>
+        <v>2543</v>
       </c>
       <c r="I489" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="J489" s="2" t="s">
-        <v>2542</v>
+        <v>2544</v>
       </c>
       <c r="K489" s="2" t="n">
-        <v>1081.0</v>
+        <v>1200.0</v>
       </c>
       <c r="L489" s="2" t="s">
-        <v>2540</v>
+        <v>2541</v>
       </c>
       <c r="M489" s="2" t="n">
-        <v>304.0</v>
+        <v>252.0</v>
       </c>
       <c r="N489" s="2" t="s">
-        <v>2543</v>
+        <v>2545</v>
       </c>
     </row>
     <row r="490">
@@ -36167,40 +36167,40 @@
         <v>489.0</v>
       </c>
       <c r="B490" s="2" t="s">
-        <v>2544</v>
+        <v>2546</v>
       </c>
       <c r="C490" s="2" t="s">
-        <v>2545</v>
+        <v>2547</v>
       </c>
       <c r="D490" s="2" t="n">
-        <v>0.0</v>
+        <v>730.0</v>
       </c>
       <c r="E490" s="2" t="s">
-        <v>2544</v>
+        <v>2546</v>
       </c>
       <c r="F490" s="2" t="n">
-        <v>309.0</v>
+        <v>0.0</v>
       </c>
       <c r="G490" s="2" t="n">
-        <v>46.0</v>
+        <v>125.0</v>
       </c>
       <c r="H490" s="2" t="s">
+        <v>2548</v>
+      </c>
+      <c r="I490" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="J490" s="2" t="s">
+        <v>2548</v>
+      </c>
+      <c r="K490" s="2" t="n">
+        <v>1081.0</v>
+      </c>
+      <c r="L490" s="2" t="s">
         <v>2546</v>
       </c>
-      <c r="I490" s="2" t="n">
-        <v>1353.0</v>
-      </c>
-      <c r="J490" s="2" t="s">
-        <v>2547</v>
-      </c>
-      <c r="K490" s="2" t="n">
-        <v>890.0</v>
-      </c>
-      <c r="L490" s="2" t="s">
-        <v>2548</v>
-      </c>
       <c r="M490" s="2" t="n">
-        <v>0.0</v>
+        <v>304.0</v>
       </c>
       <c r="N490" s="2" t="s">
         <v>2549</v>
@@ -45422,7 +45422,7 @@
         <v>70.0</v>
       </c>
       <c r="G700" s="2" t="n">
-        <v>0.0</v>
+        <v>30.0</v>
       </c>
       <c r="H700" s="2" t="s">
         <v>3619</v>

</xml_diff>

<commit_message>
Add generated leaderboard data - 2024-06-18T20:10:55
</commit_message>
<xml_diff>
--- a/Leaderboards/CurrentCMRITLeaderboard2025.xlsx
+++ b/Leaderboards/CurrentCMRITLeaderboard2025.xlsx
@@ -3443,7 +3443,7 @@
     <t>21r01a67e3</t>
   </si>
   <si>
-    <t>35.84</t>
+    <t>35.86</t>
   </si>
   <si>
     <t>21R01A0553</t>
@@ -3683,7 +3683,7 @@
     <t>devendar7987</t>
   </si>
   <si>
-    <t>35.17</t>
+    <t>35.18</t>
   </si>
   <si>
     <t>21R01A05A1</t>
@@ -5822,6 +5822,24 @@
     <t>21r01a04r4</t>
   </si>
   <si>
+    <t>21R01A66A6</t>
+  </si>
+  <si>
+    <t>CMRIT25_21R01A66A6</t>
+  </si>
+  <si>
+    <t>21r01ac1bc</t>
+  </si>
+  <si>
+    <t>yousufansari</t>
+  </si>
+  <si>
+    <t>21r01a66a6</t>
+  </si>
+  <si>
+    <t>30.75</t>
+  </si>
+  <si>
     <t>21R01A7360</t>
   </si>
   <si>
@@ -5834,36 +5852,18 @@
     <t>tumusanjay</t>
   </si>
   <si>
-    <t>30.75</t>
-  </si>
-  <si>
-    <t>21R01A66A6</t>
-  </si>
-  <si>
-    <t>CMRIT25_21R01A66A6</t>
-  </si>
-  <si>
-    <t>21r01ac1bc</t>
-  </si>
-  <si>
-    <t>yousufansari</t>
-  </si>
-  <si>
-    <t>21r01a66a6</t>
+    <t>22R05A6608</t>
+  </si>
+  <si>
+    <t>22r05a6608</t>
+  </si>
+  <si>
+    <t>abhishek4044</t>
   </si>
   <si>
     <t>30.74</t>
   </si>
   <si>
-    <t>22R05A6608</t>
-  </si>
-  <si>
-    <t>22r05a6608</t>
-  </si>
-  <si>
-    <t>abhishek4044</t>
-  </si>
-  <si>
     <t>21R01A05G5</t>
   </si>
   <si>
@@ -7571,6 +7571,24 @@
     <t>25.06</t>
   </si>
   <si>
+    <t>21R01A0541</t>
+  </si>
+  <si>
+    <t>21R01A0541@cmritonline.ac.in</t>
+  </si>
+  <si>
+    <t>vinuthnna_reddy</t>
+  </si>
+  <si>
+    <t>vin_21r01a0541</t>
+  </si>
+  <si>
+    <t>21R01A0541cmritonline.ac.in</t>
+  </si>
+  <si>
+    <t>25.04</t>
+  </si>
+  <si>
     <t>21R01A0540</t>
   </si>
   <si>
@@ -7604,24 +7622,6 @@
     <t>24.96</t>
   </si>
   <si>
-    <t>21R01A0541</t>
-  </si>
-  <si>
-    <t>21R01A0541@cmritonline.ac.in</t>
-  </si>
-  <si>
-    <t>vinuthnna_reddy</t>
-  </si>
-  <si>
-    <t>vin_21r01a0541</t>
-  </si>
-  <si>
-    <t>21R01A0541cmritonline.ac.in</t>
-  </si>
-  <si>
-    <t>24.94</t>
-  </si>
-  <si>
     <t>21R01A0532</t>
   </si>
   <si>
@@ -10877,7 +10877,7 @@
     <t>bonagiridilipku1</t>
   </si>
   <si>
-    <t>10.47</t>
+    <t>10.5</t>
   </si>
   <si>
     <t>21R01A04G2</t>
@@ -24214,7 +24214,7 @@
         <v>19.0</v>
       </c>
       <c r="G218" s="2" t="n">
-        <v>14.0</v>
+        <v>28.0</v>
       </c>
       <c r="H218" s="2" t="s">
         <v>1138</v>
@@ -24874,7 +24874,7 @@
         <v>79.0</v>
       </c>
       <c r="G233" s="2" t="n">
-        <v>446.0</v>
+        <v>448.0</v>
       </c>
       <c r="H233" s="2" t="s">
         <v>1221</v>
@@ -30937,37 +30937,37 @@
         <v>1937</v>
       </c>
       <c r="D371" s="2" t="n">
-        <v>831.0</v>
+        <v>594.0</v>
       </c>
       <c r="E371" s="2" t="s">
-        <v>1937</v>
+        <v>1938</v>
       </c>
       <c r="F371" s="2" t="n">
-        <v>0.0</v>
+        <v>10.0</v>
       </c>
       <c r="G371" s="2" t="n">
-        <v>0.0</v>
+        <v>243.0</v>
       </c>
       <c r="H371" s="2" t="s">
-        <v>1938</v>
+        <v>1939</v>
       </c>
       <c r="I371" s="2" t="n">
-        <v>1550.0</v>
+        <v>1412.0</v>
       </c>
       <c r="J371" s="2" t="s">
         <v>1939</v>
       </c>
       <c r="K371" s="2" t="n">
-        <v>779.0</v>
+        <v>1179.0</v>
       </c>
       <c r="L371" s="2" t="s">
-        <v>1937</v>
+        <v>1940</v>
       </c>
       <c r="M371" s="2" t="n">
-        <v>0.0</v>
+        <v>313.0</v>
       </c>
       <c r="N371" s="2" t="s">
-        <v>1940</v>
+        <v>1941</v>
       </c>
     </row>
     <row r="372">
@@ -30975,43 +30975,43 @@
         <v>371.0</v>
       </c>
       <c r="B372" s="2" t="s">
-        <v>1941</v>
+        <v>1942</v>
       </c>
       <c r="C372" s="2" t="s">
-        <v>1942</v>
+        <v>1943</v>
       </c>
       <c r="D372" s="2" t="n">
-        <v>594.0</v>
+        <v>831.0</v>
       </c>
       <c r="E372" s="2" t="s">
         <v>1943</v>
       </c>
       <c r="F372" s="2" t="n">
-        <v>10.0</v>
+        <v>0.0</v>
       </c>
       <c r="G372" s="2" t="n">
-        <v>239.0</v>
+        <v>0.0</v>
       </c>
       <c r="H372" s="2" t="s">
         <v>1944</v>
       </c>
       <c r="I372" s="2" t="n">
-        <v>1412.0</v>
+        <v>1550.0</v>
       </c>
       <c r="J372" s="2" t="s">
-        <v>1944</v>
+        <v>1945</v>
       </c>
       <c r="K372" s="2" t="n">
-        <v>1179.0</v>
+        <v>779.0</v>
       </c>
       <c r="L372" s="2" t="s">
-        <v>1945</v>
+        <v>1943</v>
       </c>
       <c r="M372" s="2" t="n">
-        <v>313.0</v>
+        <v>0.0</v>
       </c>
       <c r="N372" s="2" t="s">
-        <v>1946</v>
+        <v>1941</v>
       </c>
     </row>
     <row r="373">
@@ -31019,16 +31019,16 @@
         <v>372.0</v>
       </c>
       <c r="B373" s="2" t="s">
+        <v>1946</v>
+      </c>
+      <c r="C373" s="2" t="s">
         <v>1947</v>
-      </c>
-      <c r="C373" s="2" t="s">
-        <v>1948</v>
       </c>
       <c r="D373" s="2" t="n">
         <v>739.0</v>
       </c>
       <c r="E373" s="2" t="s">
-        <v>1948</v>
+        <v>1947</v>
       </c>
       <c r="F373" s="2" t="n">
         <v>0.0</v>
@@ -31037,25 +31037,25 @@
         <v>8.0</v>
       </c>
       <c r="H373" s="2" t="s">
-        <v>1948</v>
+        <v>1947</v>
       </c>
       <c r="I373" s="2" t="n">
         <v>1432.0</v>
       </c>
       <c r="J373" s="2" t="s">
-        <v>1949</v>
+        <v>1948</v>
       </c>
       <c r="K373" s="2" t="n">
         <v>1119.0</v>
       </c>
       <c r="L373" s="2" t="s">
-        <v>1948</v>
+        <v>1947</v>
       </c>
       <c r="M373" s="2" t="n">
         <v>57.0</v>
       </c>
       <c r="N373" s="2" t="s">
-        <v>1946</v>
+        <v>1949</v>
       </c>
     </row>
     <row r="374">
@@ -31099,7 +31099,7 @@
         <v>80.0</v>
       </c>
       <c r="N374" s="2" t="s">
-        <v>1946</v>
+        <v>1949</v>
       </c>
     </row>
     <row r="375">
@@ -35953,37 +35953,37 @@
         <v>2520</v>
       </c>
       <c r="D485" s="2" t="n">
-        <v>371.0</v>
+        <v>0.0</v>
       </c>
       <c r="E485" s="2" t="s">
-        <v>2521</v>
+        <v>2519</v>
       </c>
       <c r="F485" s="2" t="n">
-        <v>120.0</v>
+        <v>309.0</v>
       </c>
       <c r="G485" s="2" t="n">
-        <v>427.0</v>
+        <v>166.0</v>
       </c>
       <c r="H485" s="2" t="s">
         <v>2521</v>
       </c>
       <c r="I485" s="2" t="n">
-        <v>1500.0</v>
+        <v>1353.0</v>
       </c>
       <c r="J485" s="2" t="s">
         <v>2522</v>
       </c>
       <c r="K485" s="2" t="n">
-        <v>580.0</v>
+        <v>890.0</v>
       </c>
       <c r="L485" s="2" t="s">
-        <v>2521</v>
+        <v>2523</v>
       </c>
       <c r="M485" s="2" t="n">
-        <v>26.0</v>
+        <v>0.0</v>
       </c>
       <c r="N485" s="2" t="s">
-        <v>2523</v>
+        <v>2524</v>
       </c>
     </row>
     <row r="486">
@@ -35991,40 +35991,40 @@
         <v>485.0</v>
       </c>
       <c r="B486" s="2" t="s">
-        <v>2524</v>
+        <v>2525</v>
       </c>
       <c r="C486" s="2" t="s">
-        <v>2525</v>
+        <v>2526</v>
       </c>
       <c r="D486" s="2" t="n">
-        <v>748.0</v>
+        <v>371.0</v>
       </c>
       <c r="E486" s="2" t="s">
-        <v>2526</v>
+        <v>2527</v>
       </c>
       <c r="F486" s="2" t="n">
-        <v>0.0</v>
+        <v>120.0</v>
       </c>
       <c r="G486" s="2" t="n">
-        <v>60.0</v>
+        <v>427.0</v>
       </c>
       <c r="H486" s="2" t="s">
-        <v>2524</v>
+        <v>2527</v>
       </c>
       <c r="I486" s="2" t="n">
-        <v>0.0</v>
+        <v>1500.0</v>
       </c>
       <c r="J486" s="2" t="s">
+        <v>2528</v>
+      </c>
+      <c r="K486" s="2" t="n">
+        <v>580.0</v>
+      </c>
+      <c r="L486" s="2" t="s">
         <v>2527</v>
       </c>
-      <c r="K486" s="2" t="n">
-        <v>1014.0</v>
-      </c>
-      <c r="L486" s="2" t="s">
-        <v>2528</v>
-      </c>
       <c r="M486" s="2" t="n">
-        <v>332.0</v>
+        <v>26.0</v>
       </c>
       <c r="N486" s="2" t="s">
         <v>2529</v>
@@ -36041,34 +36041,34 @@
         <v>2531</v>
       </c>
       <c r="D487" s="2" t="n">
-        <v>0.0</v>
+        <v>748.0</v>
       </c>
       <c r="E487" s="2" t="s">
+        <v>2532</v>
+      </c>
+      <c r="F487" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G487" s="2" t="n">
+        <v>60.0</v>
+      </c>
+      <c r="H487" s="2" t="s">
         <v>2530</v>
       </c>
-      <c r="F487" s="2" t="n">
-        <v>309.0</v>
-      </c>
-      <c r="G487" s="2" t="n">
-        <v>102.0</v>
-      </c>
-      <c r="H487" s="2" t="s">
-        <v>2532</v>
-      </c>
       <c r="I487" s="2" t="n">
-        <v>1353.0</v>
+        <v>0.0</v>
       </c>
       <c r="J487" s="2" t="s">
         <v>2533</v>
       </c>
       <c r="K487" s="2" t="n">
-        <v>890.0</v>
+        <v>1014.0</v>
       </c>
       <c r="L487" s="2" t="s">
         <v>2534</v>
       </c>
       <c r="M487" s="2" t="n">
-        <v>0.0</v>
+        <v>332.0</v>
       </c>
       <c r="N487" s="2" t="s">
         <v>2535</v>
@@ -45422,7 +45422,7 @@
         <v>70.0</v>
       </c>
       <c r="G700" s="2" t="n">
-        <v>30.0</v>
+        <v>50.0</v>
       </c>
       <c r="H700" s="2" t="s">
         <v>3619</v>

</xml_diff>

<commit_message>
Add generated leaderboard data - 2024-06-29T20:11:49
</commit_message>
<xml_diff>
--- a/Leaderboards/CurrentCMRITLeaderboard2025.xlsx
+++ b/Leaderboards/CurrentCMRITLeaderboard2025.xlsx
@@ -704,6 +704,21 @@
     <t>49.19</t>
   </si>
   <si>
+    <t>21R01A05N8</t>
+  </si>
+  <si>
+    <t>CMRIT25-21r01a05n8</t>
+  </si>
+  <si>
+    <t>karthik_51</t>
+  </si>
+  <si>
+    <t>21r01a05n8</t>
+  </si>
+  <si>
+    <t>49.17</t>
+  </si>
+  <si>
     <t>22R05A0501</t>
   </si>
   <si>
@@ -2022,21 +2037,6 @@
   </si>
   <si>
     <t>40.18</t>
-  </si>
-  <si>
-    <t>21R01A05N8</t>
-  </si>
-  <si>
-    <t>CMRIT25-21r01a05n8</t>
-  </si>
-  <si>
-    <t>karthik_51</t>
-  </si>
-  <si>
-    <t>21r01a05n8</t>
-  </si>
-  <si>
-    <t>40.07</t>
   </si>
   <si>
     <t>22R05A0508</t>
@@ -16520,34 +16520,34 @@
         <v>231</v>
       </c>
       <c r="D43" s="2" t="n">
-        <v>727.0</v>
+        <v>935.0</v>
       </c>
       <c r="E43" s="2" t="s">
         <v>232</v>
       </c>
       <c r="F43" s="2" t="n">
-        <v>419.0</v>
+        <v>249.0</v>
       </c>
       <c r="G43" s="2" t="n">
-        <v>418.0</v>
+        <v>141.0</v>
       </c>
       <c r="H43" s="2" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="I43" s="2" t="n">
         <v>1490.0</v>
       </c>
       <c r="J43" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="K43" s="2" t="n">
+        <v>1471.0</v>
+      </c>
+      <c r="L43" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="K43" s="2" t="n">
-        <v>1036.0</v>
-      </c>
-      <c r="L43" s="2" t="s">
-        <v>230</v>
-      </c>
       <c r="M43" s="2" t="n">
-        <v>287.0</v>
+        <v>284.0</v>
       </c>
       <c r="N43" s="2" t="s">
         <v>234</v>
@@ -16564,37 +16564,37 @@
         <v>236</v>
       </c>
       <c r="D44" s="2" t="n">
-        <v>700.0</v>
+        <v>727.0</v>
       </c>
       <c r="E44" s="2" t="s">
         <v>237</v>
       </c>
       <c r="F44" s="2" t="n">
-        <v>436.0</v>
+        <v>419.0</v>
       </c>
       <c r="G44" s="2" t="n">
-        <v>0.0</v>
+        <v>418.0</v>
       </c>
       <c r="H44" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="I44" s="2" t="n">
+        <v>1490.0</v>
+      </c>
+      <c r="J44" s="2" t="s">
         <v>238</v>
       </c>
-      <c r="I44" s="2" t="n">
-        <v>1559.0</v>
-      </c>
-      <c r="J44" s="2" t="s">
+      <c r="K44" s="2" t="n">
+        <v>1036.0</v>
+      </c>
+      <c r="L44" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="M44" s="2" t="n">
+        <v>287.0</v>
+      </c>
+      <c r="N44" s="2" t="s">
         <v>239</v>
-      </c>
-      <c r="K44" s="2" t="n">
-        <v>1164.0</v>
-      </c>
-      <c r="L44" s="2" t="s">
-        <v>238</v>
-      </c>
-      <c r="M44" s="2" t="n">
-        <v>180.0</v>
-      </c>
-      <c r="N44" s="2" t="s">
-        <v>240</v>
       </c>
     </row>
     <row r="45">
@@ -16602,40 +16602,40 @@
         <v>44.0</v>
       </c>
       <c r="B45" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="C45" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="C45" s="2" t="s">
+      <c r="D45" s="2" t="n">
+        <v>700.0</v>
+      </c>
+      <c r="E45" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="D45" s="2" t="n">
-        <v>795.0</v>
-      </c>
-      <c r="E45" s="2" t="s">
-        <v>243</v>
-      </c>
       <c r="F45" s="2" t="n">
-        <v>391.0</v>
+        <v>436.0</v>
       </c>
       <c r="G45" s="2" t="n">
-        <v>778.0</v>
+        <v>0.0</v>
       </c>
       <c r="H45" s="2" t="s">
         <v>243</v>
       </c>
       <c r="I45" s="2" t="n">
-        <v>1422.0</v>
+        <v>1559.0</v>
       </c>
       <c r="J45" s="2" t="s">
         <v>244</v>
       </c>
       <c r="K45" s="2" t="n">
-        <v>1184.0</v>
+        <v>1164.0</v>
       </c>
       <c r="L45" s="2" t="s">
         <v>243</v>
       </c>
       <c r="M45" s="2" t="n">
-        <v>59.0</v>
+        <v>180.0</v>
       </c>
       <c r="N45" s="2" t="s">
         <v>245</v>
@@ -16652,37 +16652,37 @@
         <v>247</v>
       </c>
       <c r="D46" s="2" t="n">
-        <v>759.0</v>
+        <v>795.0</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="F46" s="2" t="n">
-        <v>449.0</v>
+        <v>391.0</v>
       </c>
       <c r="G46" s="2" t="n">
-        <v>147.0</v>
+        <v>778.0</v>
       </c>
       <c r="H46" s="2" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="I46" s="2" t="n">
-        <v>1336.0</v>
+        <v>1422.0</v>
       </c>
       <c r="J46" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="K46" s="2" t="n">
+        <v>1184.0</v>
+      </c>
+      <c r="L46" s="2" t="s">
         <v>248</v>
       </c>
-      <c r="K46" s="2" t="n">
-        <v>791.0</v>
-      </c>
-      <c r="L46" s="2" t="s">
-        <v>246</v>
-      </c>
       <c r="M46" s="2" t="n">
-        <v>256.0</v>
+        <v>59.0</v>
       </c>
       <c r="N46" s="2" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
     </row>
     <row r="47">
@@ -16690,40 +16690,40 @@
         <v>46.0</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="D47" s="2" t="n">
-        <v>612.0</v>
+        <v>759.0</v>
       </c>
       <c r="E47" s="2" t="s">
         <v>252</v>
       </c>
       <c r="F47" s="2" t="n">
-        <v>460.0</v>
+        <v>449.0</v>
       </c>
       <c r="G47" s="2" t="n">
-        <v>12.0</v>
+        <v>147.0</v>
       </c>
       <c r="H47" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="I47" s="2" t="n">
-        <v>1667.0</v>
+        <v>1336.0</v>
       </c>
       <c r="J47" s="2" t="s">
         <v>253</v>
       </c>
       <c r="K47" s="2" t="n">
-        <v>1077.0</v>
+        <v>791.0</v>
       </c>
       <c r="L47" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="M47" s="2" t="n">
-        <v>150.0</v>
+        <v>256.0</v>
       </c>
       <c r="N47" s="2" t="s">
         <v>254</v>
@@ -16740,37 +16740,37 @@
         <v>256</v>
       </c>
       <c r="D48" s="2" t="n">
-        <v>753.0</v>
+        <v>612.0</v>
       </c>
       <c r="E48" s="2" t="s">
         <v>257</v>
       </c>
       <c r="F48" s="2" t="n">
-        <v>349.0</v>
+        <v>460.0</v>
       </c>
       <c r="G48" s="2" t="n">
-        <v>340.0</v>
+        <v>12.0</v>
       </c>
       <c r="H48" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="I48" s="2" t="n">
+        <v>1667.0</v>
+      </c>
+      <c r="J48" s="2" t="s">
         <v>258</v>
       </c>
-      <c r="I48" s="2" t="n">
-        <v>1438.0</v>
-      </c>
-      <c r="J48" s="2" t="s">
+      <c r="K48" s="2" t="n">
+        <v>1077.0</v>
+      </c>
+      <c r="L48" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="M48" s="2" t="n">
+        <v>150.0</v>
+      </c>
+      <c r="N48" s="2" t="s">
         <v>259</v>
-      </c>
-      <c r="K48" s="2" t="n">
-        <v>1417.0</v>
-      </c>
-      <c r="L48" s="2" t="s">
-        <v>260</v>
-      </c>
-      <c r="M48" s="2" t="n">
-        <v>137.0</v>
-      </c>
-      <c r="N48" s="2" t="s">
-        <v>261</v>
       </c>
     </row>
     <row r="49">
@@ -16778,40 +16778,40 @@
         <v>48.0</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="D49" s="2" t="n">
-        <v>836.0</v>
+        <v>753.0</v>
       </c>
       <c r="E49" s="2" t="s">
         <v>262</v>
       </c>
       <c r="F49" s="2" t="n">
-        <v>278.0</v>
+        <v>349.0</v>
       </c>
       <c r="G49" s="2" t="n">
-        <v>520.0</v>
+        <v>340.0</v>
       </c>
       <c r="H49" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="I49" s="2" t="n">
+        <v>1438.0</v>
+      </c>
+      <c r="J49" s="2" t="s">
         <v>264</v>
       </c>
-      <c r="I49" s="2" t="n">
-        <v>1432.0</v>
-      </c>
-      <c r="J49" s="2" t="s">
+      <c r="K49" s="2" t="n">
+        <v>1417.0</v>
+      </c>
+      <c r="L49" s="2" t="s">
         <v>265</v>
       </c>
-      <c r="K49" s="2" t="n">
-        <v>1193.0</v>
-      </c>
-      <c r="L49" s="2" t="s">
-        <v>262</v>
-      </c>
       <c r="M49" s="2" t="n">
-        <v>390.0</v>
+        <v>137.0</v>
       </c>
       <c r="N49" s="2" t="s">
         <v>266</v>
@@ -16825,37 +16825,37 @@
         <v>267</v>
       </c>
       <c r="C50" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="D50" s="2" t="n">
+        <v>836.0</v>
+      </c>
+      <c r="E50" s="2" t="s">
         <v>267</v>
       </c>
-      <c r="D50" s="2" t="n">
-        <v>883.0</v>
-      </c>
-      <c r="E50" s="2" t="s">
-        <v>268</v>
-      </c>
       <c r="F50" s="2" t="n">
-        <v>296.0</v>
+        <v>278.0</v>
       </c>
       <c r="G50" s="2" t="n">
-        <v>0.0</v>
+        <v>520.0</v>
       </c>
       <c r="H50" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="I50" s="2" t="n">
+        <v>1432.0</v>
+      </c>
+      <c r="J50" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="K50" s="2" t="n">
+        <v>1193.0</v>
+      </c>
+      <c r="L50" s="2" t="s">
         <v>267</v>
       </c>
-      <c r="I50" s="2" t="n">
-        <v>1512.0</v>
-      </c>
-      <c r="J50" s="2" t="s">
-        <v>269</v>
-      </c>
-      <c r="K50" s="2" t="n">
-        <v>1470.0</v>
-      </c>
-      <c r="L50" s="2" t="s">
-        <v>270</v>
-      </c>
       <c r="M50" s="2" t="n">
-        <v>10.0</v>
+        <v>390.0</v>
       </c>
       <c r="N50" s="2" t="s">
         <v>271</v>
@@ -16869,40 +16869,40 @@
         <v>272</v>
       </c>
       <c r="C51" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="D51" s="2" t="n">
+        <v>883.0</v>
+      </c>
+      <c r="E51" s="2" t="s">
         <v>273</v>
       </c>
-      <c r="D51" s="2" t="n">
-        <v>968.0</v>
-      </c>
-      <c r="E51" s="2" t="s">
+      <c r="F51" s="2" t="n">
+        <v>296.0</v>
+      </c>
+      <c r="G51" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H51" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="I51" s="2" t="n">
+        <v>1512.0</v>
+      </c>
+      <c r="J51" s="2" t="s">
         <v>274</v>
       </c>
-      <c r="F51" s="2" t="n">
-        <v>179.0</v>
-      </c>
-      <c r="G51" s="2" t="n">
-        <v>803.0</v>
-      </c>
-      <c r="H51" s="2" t="s">
-        <v>275</v>
-      </c>
-      <c r="I51" s="2" t="n">
-        <v>1494.0</v>
-      </c>
-      <c r="J51" s="2" t="s">
-        <v>276</v>
-      </c>
       <c r="K51" s="2" t="n">
-        <v>1210.0</v>
+        <v>1470.0</v>
       </c>
       <c r="L51" s="2" t="s">
         <v>275</v>
       </c>
       <c r="M51" s="2" t="n">
-        <v>402.0</v>
+        <v>10.0</v>
       </c>
       <c r="N51" s="2" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="52">
@@ -16910,40 +16910,40 @@
         <v>51.0</v>
       </c>
       <c r="B52" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="C52" s="2" t="s">
         <v>278</v>
       </c>
-      <c r="C52" s="2" t="s">
+      <c r="D52" s="2" t="n">
+        <v>968.0</v>
+      </c>
+      <c r="E52" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="D52" s="2" t="n">
-        <v>581.0</v>
-      </c>
-      <c r="E52" s="2" t="s">
+      <c r="F52" s="2" t="n">
+        <v>179.0</v>
+      </c>
+      <c r="G52" s="2" t="n">
+        <v>803.0</v>
+      </c>
+      <c r="H52" s="2" t="s">
         <v>280</v>
       </c>
-      <c r="F52" s="2" t="n">
-        <v>298.0</v>
-      </c>
-      <c r="G52" s="2" t="n">
-        <v>488.0</v>
-      </c>
-      <c r="H52" s="2" t="s">
-        <v>281</v>
-      </c>
       <c r="I52" s="2" t="n">
-        <v>1396.0</v>
+        <v>1494.0</v>
       </c>
       <c r="J52" s="2" t="s">
         <v>281</v>
       </c>
       <c r="K52" s="2" t="n">
-        <v>1339.0</v>
+        <v>1210.0</v>
       </c>
       <c r="L52" s="2" t="s">
         <v>280</v>
       </c>
       <c r="M52" s="2" t="n">
-        <v>852.0</v>
+        <v>402.0</v>
       </c>
       <c r="N52" s="2" t="s">
         <v>282</v>
@@ -16960,34 +16960,34 @@
         <v>284</v>
       </c>
       <c r="D53" s="2" t="n">
-        <v>747.0</v>
+        <v>581.0</v>
       </c>
       <c r="E53" s="2" t="s">
         <v>285</v>
       </c>
       <c r="F53" s="2" t="n">
-        <v>422.0</v>
+        <v>298.0</v>
       </c>
       <c r="G53" s="2" t="n">
-        <v>74.0</v>
+        <v>488.0</v>
       </c>
       <c r="H53" s="2" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="I53" s="2" t="n">
-        <v>1274.0</v>
+        <v>1396.0</v>
       </c>
       <c r="J53" s="2" t="s">
         <v>286</v>
       </c>
       <c r="K53" s="2" t="n">
-        <v>1153.0</v>
+        <v>1339.0</v>
       </c>
       <c r="L53" s="2" t="s">
         <v>285</v>
       </c>
       <c r="M53" s="2" t="n">
-        <v>63.0</v>
+        <v>852.0</v>
       </c>
       <c r="N53" s="2" t="s">
         <v>287</v>
@@ -17004,37 +17004,37 @@
         <v>289</v>
       </c>
       <c r="D54" s="2" t="n">
-        <v>860.0</v>
+        <v>747.0</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="F54" s="2" t="n">
-        <v>340.0</v>
+        <v>422.0</v>
       </c>
       <c r="G54" s="2" t="n">
-        <v>127.0</v>
+        <v>74.0</v>
       </c>
       <c r="H54" s="2" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="I54" s="2" t="n">
-        <v>1334.0</v>
+        <v>1274.0</v>
       </c>
       <c r="J54" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="K54" s="2" t="n">
+        <v>1153.0</v>
+      </c>
+      <c r="L54" s="2" t="s">
         <v>290</v>
       </c>
-      <c r="K54" s="2" t="n">
-        <v>1034.0</v>
-      </c>
-      <c r="L54" s="2" t="s">
-        <v>288</v>
-      </c>
       <c r="M54" s="2" t="n">
-        <v>191.0</v>
+        <v>63.0</v>
       </c>
       <c r="N54" s="2" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
     </row>
     <row r="55">
@@ -17042,40 +17042,40 @@
         <v>54.0</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="D55" s="2" t="n">
-        <v>880.0</v>
+        <v>860.0</v>
       </c>
       <c r="E55" s="2" t="s">
         <v>294</v>
       </c>
       <c r="F55" s="2" t="n">
-        <v>188.0</v>
+        <v>340.0</v>
       </c>
       <c r="G55" s="2" t="n">
-        <v>190.0</v>
+        <v>127.0</v>
       </c>
       <c r="H55" s="2" t="s">
         <v>294</v>
       </c>
       <c r="I55" s="2" t="n">
-        <v>1501.0</v>
+        <v>1334.0</v>
       </c>
       <c r="J55" s="2" t="s">
         <v>295</v>
       </c>
       <c r="K55" s="2" t="n">
-        <v>1471.0</v>
+        <v>1034.0</v>
       </c>
       <c r="L55" s="2" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="M55" s="2" t="n">
-        <v>382.0</v>
+        <v>191.0</v>
       </c>
       <c r="N55" s="2" t="s">
         <v>296</v>
@@ -17092,34 +17092,34 @@
         <v>298</v>
       </c>
       <c r="D56" s="2" t="n">
-        <v>805.0</v>
+        <v>880.0</v>
       </c>
       <c r="E56" s="2" t="s">
         <v>299</v>
       </c>
       <c r="F56" s="2" t="n">
-        <v>319.0</v>
+        <v>188.0</v>
       </c>
       <c r="G56" s="2" t="n">
-        <v>105.0</v>
+        <v>190.0</v>
       </c>
       <c r="H56" s="2" t="s">
         <v>299</v>
       </c>
       <c r="I56" s="2" t="n">
-        <v>1411.0</v>
+        <v>1501.0</v>
       </c>
       <c r="J56" s="2" t="s">
         <v>300</v>
       </c>
       <c r="K56" s="2" t="n">
-        <v>1091.0</v>
+        <v>1471.0</v>
       </c>
       <c r="L56" s="2" t="s">
         <v>299</v>
       </c>
       <c r="M56" s="2" t="n">
-        <v>300.0</v>
+        <v>382.0</v>
       </c>
       <c r="N56" s="2" t="s">
         <v>301</v>
@@ -17136,37 +17136,37 @@
         <v>303</v>
       </c>
       <c r="D57" s="2" t="n">
-        <v>776.0</v>
+        <v>805.0</v>
       </c>
       <c r="E57" s="2" t="s">
         <v>304</v>
       </c>
       <c r="F57" s="2" t="n">
-        <v>344.0</v>
+        <v>319.0</v>
       </c>
       <c r="G57" s="2" t="n">
-        <v>35.0</v>
+        <v>105.0</v>
       </c>
       <c r="H57" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="I57" s="2" t="n">
+        <v>1411.0</v>
+      </c>
+      <c r="J57" s="2" t="s">
         <v>305</v>
       </c>
-      <c r="I57" s="2" t="n">
-        <v>1214.0</v>
-      </c>
-      <c r="J57" s="2" t="s">
+      <c r="K57" s="2" t="n">
+        <v>1091.0</v>
+      </c>
+      <c r="L57" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="M57" s="2" t="n">
+        <v>300.0</v>
+      </c>
+      <c r="N57" s="2" t="s">
         <v>306</v>
-      </c>
-      <c r="K57" s="2" t="n">
-        <v>1356.0</v>
-      </c>
-      <c r="L57" s="2" t="s">
-        <v>305</v>
-      </c>
-      <c r="M57" s="2" t="n">
-        <v>182.0</v>
-      </c>
-      <c r="N57" s="2" t="s">
-        <v>307</v>
       </c>
     </row>
     <row r="58">
@@ -17174,43 +17174,43 @@
         <v>57.0</v>
       </c>
       <c r="B58" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="C58" s="2" t="s">
         <v>308</v>
       </c>
-      <c r="C58" s="2" t="s">
+      <c r="D58" s="2" t="n">
+        <v>776.0</v>
+      </c>
+      <c r="E58" s="2" t="s">
         <v>309</v>
       </c>
-      <c r="D58" s="2" t="n">
-        <v>905.0</v>
-      </c>
-      <c r="E58" s="2" t="s">
+      <c r="F58" s="2" t="n">
+        <v>344.0</v>
+      </c>
+      <c r="G58" s="2" t="n">
+        <v>35.0</v>
+      </c>
+      <c r="H58" s="2" t="s">
         <v>310</v>
       </c>
-      <c r="F58" s="2" t="n">
-        <v>253.0</v>
-      </c>
-      <c r="G58" s="2" t="n">
-        <v>54.0</v>
-      </c>
-      <c r="H58" s="2" t="s">
+      <c r="I58" s="2" t="n">
+        <v>1214.0</v>
+      </c>
+      <c r="J58" s="2" t="s">
         <v>311</v>
       </c>
-      <c r="I58" s="2" t="n">
-        <v>1422.0</v>
-      </c>
-      <c r="J58" s="2" t="s">
+      <c r="K58" s="2" t="n">
+        <v>1356.0</v>
+      </c>
+      <c r="L58" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="M58" s="2" t="n">
+        <v>182.0</v>
+      </c>
+      <c r="N58" s="2" t="s">
         <v>312</v>
-      </c>
-      <c r="K58" s="2" t="n">
-        <v>1413.0</v>
-      </c>
-      <c r="L58" s="2" t="s">
-        <v>311</v>
-      </c>
-      <c r="M58" s="2" t="n">
-        <v>97.0</v>
-      </c>
-      <c r="N58" s="2" t="s">
-        <v>313</v>
       </c>
     </row>
     <row r="59">
@@ -17218,40 +17218,40 @@
         <v>58.0</v>
       </c>
       <c r="B59" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="C59" s="2" t="s">
         <v>314</v>
       </c>
-      <c r="C59" s="2" t="s">
+      <c r="D59" s="2" t="n">
+        <v>905.0</v>
+      </c>
+      <c r="E59" s="2" t="s">
         <v>315</v>
       </c>
-      <c r="D59" s="2" t="n">
-        <v>732.0</v>
-      </c>
-      <c r="E59" s="2" t="s">
-        <v>316</v>
-      </c>
       <c r="F59" s="2" t="n">
-        <v>328.0</v>
+        <v>253.0</v>
       </c>
       <c r="G59" s="2" t="n">
-        <v>213.0</v>
+        <v>54.0</v>
       </c>
       <c r="H59" s="2" t="s">
         <v>316</v>
       </c>
       <c r="I59" s="2" t="n">
-        <v>1491.0</v>
+        <v>1422.0</v>
       </c>
       <c r="J59" s="2" t="s">
         <v>317</v>
       </c>
       <c r="K59" s="2" t="n">
-        <v>1183.0</v>
+        <v>1413.0</v>
       </c>
       <c r="L59" s="2" t="s">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="M59" s="2" t="n">
-        <v>255.0</v>
+        <v>97.0</v>
       </c>
       <c r="N59" s="2" t="s">
         <v>318</v>
@@ -17268,34 +17268,34 @@
         <v>320</v>
       </c>
       <c r="D60" s="2" t="n">
-        <v>863.0</v>
+        <v>732.0</v>
       </c>
       <c r="E60" s="2" t="s">
         <v>321</v>
       </c>
       <c r="F60" s="2" t="n">
-        <v>266.0</v>
+        <v>328.0</v>
       </c>
       <c r="G60" s="2" t="n">
-        <v>0.0</v>
+        <v>213.0</v>
       </c>
       <c r="H60" s="2" t="s">
         <v>321</v>
       </c>
       <c r="I60" s="2" t="n">
-        <v>1527.0</v>
+        <v>1491.0</v>
       </c>
       <c r="J60" s="2" t="s">
         <v>322</v>
       </c>
       <c r="K60" s="2" t="n">
-        <v>1360.0</v>
+        <v>1183.0</v>
       </c>
       <c r="L60" s="2" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="M60" s="2" t="n">
-        <v>90.0</v>
+        <v>255.0</v>
       </c>
       <c r="N60" s="2" t="s">
         <v>323</v>
@@ -17312,37 +17312,37 @@
         <v>325</v>
       </c>
       <c r="D61" s="2" t="n">
-        <v>763.0</v>
+        <v>863.0</v>
       </c>
       <c r="E61" s="2" t="s">
         <v>326</v>
       </c>
       <c r="F61" s="2" t="n">
-        <v>256.0</v>
+        <v>266.0</v>
       </c>
       <c r="G61" s="2" t="n">
-        <v>811.0</v>
+        <v>0.0</v>
       </c>
       <c r="H61" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="I61" s="2" t="n">
+        <v>1527.0</v>
+      </c>
+      <c r="J61" s="2" t="s">
         <v>327</v>
       </c>
-      <c r="I61" s="2" t="n">
-        <v>1480.0</v>
-      </c>
-      <c r="J61" s="2" t="s">
+      <c r="K61" s="2" t="n">
+        <v>1360.0</v>
+      </c>
+      <c r="L61" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="M61" s="2" t="n">
+        <v>90.0</v>
+      </c>
+      <c r="N61" s="2" t="s">
         <v>328</v>
-      </c>
-      <c r="K61" s="2" t="n">
-        <v>1207.0</v>
-      </c>
-      <c r="L61" s="2" t="s">
-        <v>329</v>
-      </c>
-      <c r="M61" s="2" t="n">
-        <v>380.0</v>
-      </c>
-      <c r="N61" s="2" t="s">
-        <v>330</v>
       </c>
     </row>
     <row r="62">
@@ -17350,40 +17350,40 @@
         <v>61.0</v>
       </c>
       <c r="B62" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="D62" s="2" t="n">
+        <v>763.0</v>
+      </c>
+      <c r="E62" s="2" t="s">
         <v>331</v>
       </c>
-      <c r="C62" s="2" t="s">
+      <c r="F62" s="2" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="G62" s="2" t="n">
+        <v>811.0</v>
+      </c>
+      <c r="H62" s="2" t="s">
         <v>332</v>
       </c>
-      <c r="D62" s="2" t="n">
-        <v>1007.0</v>
-      </c>
-      <c r="E62" s="2" t="s">
+      <c r="I62" s="2" t="n">
+        <v>1480.0</v>
+      </c>
+      <c r="J62" s="2" t="s">
         <v>333</v>
       </c>
-      <c r="F62" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="G62" s="2" t="n">
-        <v>22.0</v>
-      </c>
-      <c r="H62" s="2" t="s">
-        <v>333</v>
-      </c>
-      <c r="I62" s="2" t="n">
-        <v>1558.0</v>
-      </c>
-      <c r="J62" s="2" t="s">
+      <c r="K62" s="2" t="n">
+        <v>1207.0</v>
+      </c>
+      <c r="L62" s="2" t="s">
         <v>334</v>
       </c>
-      <c r="K62" s="2" t="n">
-        <v>1501.0</v>
-      </c>
-      <c r="L62" s="2" t="s">
-        <v>331</v>
-      </c>
       <c r="M62" s="2" t="n">
-        <v>845.0</v>
+        <v>380.0</v>
       </c>
       <c r="N62" s="2" t="s">
         <v>335</v>
@@ -17400,34 +17400,34 @@
         <v>337</v>
       </c>
       <c r="D63" s="2" t="n">
-        <v>592.0</v>
+        <v>1007.0</v>
       </c>
       <c r="E63" s="2" t="s">
         <v>338</v>
       </c>
       <c r="F63" s="2" t="n">
-        <v>436.0</v>
+        <v>0.0</v>
       </c>
       <c r="G63" s="2" t="n">
-        <v>65.0</v>
+        <v>22.0</v>
       </c>
       <c r="H63" s="2" t="s">
         <v>338</v>
       </c>
       <c r="I63" s="2" t="n">
-        <v>1379.0</v>
+        <v>1558.0</v>
       </c>
       <c r="J63" s="2" t="s">
         <v>339</v>
       </c>
       <c r="K63" s="2" t="n">
-        <v>1404.0</v>
+        <v>1501.0</v>
       </c>
       <c r="L63" s="2" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="M63" s="2" t="n">
-        <v>13.0</v>
+        <v>845.0</v>
       </c>
       <c r="N63" s="2" t="s">
         <v>340</v>
@@ -17444,37 +17444,37 @@
         <v>342</v>
       </c>
       <c r="D64" s="2" t="n">
-        <v>805.0</v>
+        <v>592.0</v>
       </c>
       <c r="E64" s="2" t="s">
         <v>343</v>
       </c>
       <c r="F64" s="2" t="n">
-        <v>320.0</v>
+        <v>436.0</v>
       </c>
       <c r="G64" s="2" t="n">
-        <v>55.0</v>
+        <v>65.0</v>
       </c>
       <c r="H64" s="2" t="s">
+        <v>343</v>
+      </c>
+      <c r="I64" s="2" t="n">
+        <v>1379.0</v>
+      </c>
+      <c r="J64" s="2" t="s">
         <v>344</v>
       </c>
-      <c r="I64" s="2" t="n">
-        <v>1421.0</v>
-      </c>
-      <c r="J64" s="2" t="s">
+      <c r="K64" s="2" t="n">
+        <v>1404.0</v>
+      </c>
+      <c r="L64" s="2" t="s">
+        <v>343</v>
+      </c>
+      <c r="M64" s="2" t="n">
+        <v>13.0</v>
+      </c>
+      <c r="N64" s="2" t="s">
         <v>345</v>
-      </c>
-      <c r="K64" s="2" t="n">
-        <v>1260.0</v>
-      </c>
-      <c r="L64" s="2" t="s">
-        <v>346</v>
-      </c>
-      <c r="M64" s="2" t="n">
-        <v>80.0</v>
-      </c>
-      <c r="N64" s="2" t="s">
-        <v>347</v>
       </c>
     </row>
     <row r="65">
@@ -17482,43 +17482,43 @@
         <v>64.0</v>
       </c>
       <c r="B65" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="C65" s="2" t="s">
+        <v>347</v>
+      </c>
+      <c r="D65" s="2" t="n">
+        <v>805.0</v>
+      </c>
+      <c r="E65" s="2" t="s">
         <v>348</v>
       </c>
-      <c r="C65" s="2" t="s">
+      <c r="F65" s="2" t="n">
+        <v>320.0</v>
+      </c>
+      <c r="G65" s="2" t="n">
+        <v>55.0</v>
+      </c>
+      <c r="H65" s="2" t="s">
         <v>349</v>
       </c>
-      <c r="D65" s="2" t="n">
-        <v>779.0</v>
-      </c>
-      <c r="E65" s="2" t="s">
+      <c r="I65" s="2" t="n">
+        <v>1421.0</v>
+      </c>
+      <c r="J65" s="2" t="s">
         <v>350</v>
       </c>
-      <c r="F65" s="2" t="n">
-        <v>139.0</v>
-      </c>
-      <c r="G65" s="2" t="n">
-        <v>619.0</v>
-      </c>
-      <c r="H65" s="2" t="s">
-        <v>351</v>
-      </c>
-      <c r="I65" s="2" t="n">
-        <v>1316.0</v>
-      </c>
-      <c r="J65" s="2" t="s">
-        <v>352</v>
-      </c>
       <c r="K65" s="2" t="n">
-        <v>1119.0</v>
+        <v>1260.0</v>
       </c>
       <c r="L65" s="2" t="s">
         <v>351</v>
       </c>
       <c r="M65" s="2" t="n">
-        <v>1089.0</v>
+        <v>80.0</v>
       </c>
       <c r="N65" s="2" t="s">
-        <v>347</v>
+        <v>352</v>
       </c>
     </row>
     <row r="66">
@@ -17532,37 +17532,37 @@
         <v>354</v>
       </c>
       <c r="D66" s="2" t="n">
-        <v>833.0</v>
+        <v>779.0</v>
       </c>
       <c r="E66" s="2" t="s">
         <v>355</v>
       </c>
       <c r="F66" s="2" t="n">
-        <v>277.0</v>
+        <v>139.0</v>
       </c>
       <c r="G66" s="2" t="n">
-        <v>88.0</v>
+        <v>619.0</v>
       </c>
       <c r="H66" s="2" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="I66" s="2" t="n">
-        <v>1410.0</v>
+        <v>1316.0</v>
       </c>
       <c r="J66" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="K66" s="2" t="n">
+        <v>1119.0</v>
+      </c>
+      <c r="L66" s="2" t="s">
         <v>356</v>
       </c>
-      <c r="K66" s="2" t="n">
-        <v>1180.0</v>
-      </c>
-      <c r="L66" s="2" t="s">
-        <v>355</v>
-      </c>
       <c r="M66" s="2" t="n">
-        <v>271.0</v>
+        <v>1089.0</v>
       </c>
       <c r="N66" s="2" t="s">
-        <v>357</v>
+        <v>352</v>
       </c>
     </row>
     <row r="67">
@@ -17576,34 +17576,34 @@
         <v>359</v>
       </c>
       <c r="D67" s="2" t="n">
-        <v>844.0</v>
+        <v>833.0</v>
       </c>
       <c r="E67" s="2" t="s">
         <v>360</v>
       </c>
       <c r="F67" s="2" t="n">
-        <v>267.0</v>
+        <v>277.0</v>
       </c>
       <c r="G67" s="2" t="n">
-        <v>118.0</v>
+        <v>88.0</v>
       </c>
       <c r="H67" s="2" t="s">
-        <v>358</v>
+        <v>360</v>
       </c>
       <c r="I67" s="2" t="n">
-        <v>1177.0</v>
+        <v>1410.0</v>
       </c>
       <c r="J67" s="2" t="s">
         <v>361</v>
       </c>
       <c r="K67" s="2" t="n">
-        <v>1303.0</v>
+        <v>1180.0</v>
       </c>
       <c r="L67" s="2" t="s">
         <v>360</v>
       </c>
       <c r="M67" s="2" t="n">
-        <v>333.0</v>
+        <v>271.0</v>
       </c>
       <c r="N67" s="2" t="s">
         <v>362</v>
@@ -17620,37 +17620,37 @@
         <v>364</v>
       </c>
       <c r="D68" s="2" t="n">
-        <v>883.0</v>
+        <v>844.0</v>
       </c>
       <c r="E68" s="2" t="s">
         <v>365</v>
       </c>
       <c r="F68" s="2" t="n">
-        <v>224.0</v>
+        <v>267.0</v>
       </c>
       <c r="G68" s="2" t="n">
-        <v>21.0</v>
+        <v>118.0</v>
       </c>
       <c r="H68" s="2" t="s">
+        <v>363</v>
+      </c>
+      <c r="I68" s="2" t="n">
+        <v>1177.0</v>
+      </c>
+      <c r="J68" s="2" t="s">
         <v>366</v>
       </c>
-      <c r="I68" s="2" t="n">
-        <v>1456.0</v>
-      </c>
-      <c r="J68" s="2" t="s">
+      <c r="K68" s="2" t="n">
+        <v>1303.0</v>
+      </c>
+      <c r="L68" s="2" t="s">
         <v>365</v>
       </c>
-      <c r="K68" s="2" t="n">
-        <v>1420.0</v>
-      </c>
-      <c r="L68" s="2" t="s">
+      <c r="M68" s="2" t="n">
+        <v>333.0</v>
+      </c>
+      <c r="N68" s="2" t="s">
         <v>367</v>
-      </c>
-      <c r="M68" s="2" t="n">
-        <v>169.0</v>
-      </c>
-      <c r="N68" s="2" t="s">
-        <v>368</v>
       </c>
     </row>
     <row r="69">
@@ -17658,40 +17658,40 @@
         <v>68.0</v>
       </c>
       <c r="B69" s="2" t="s">
+        <v>368</v>
+      </c>
+      <c r="C69" s="2" t="s">
         <v>369</v>
       </c>
-      <c r="C69" s="2" t="s">
+      <c r="D69" s="2" t="n">
+        <v>883.0</v>
+      </c>
+      <c r="E69" s="2" t="s">
         <v>370</v>
       </c>
-      <c r="D69" s="2" t="n">
-        <v>979.0</v>
-      </c>
-      <c r="E69" s="2" t="s">
-        <v>371</v>
-      </c>
       <c r="F69" s="2" t="n">
-        <v>247.0</v>
+        <v>224.0</v>
       </c>
       <c r="G69" s="2" t="n">
-        <v>117.0</v>
+        <v>21.0</v>
       </c>
       <c r="H69" s="2" t="s">
         <v>371</v>
       </c>
       <c r="I69" s="2" t="n">
-        <v>1429.0</v>
+        <v>1456.0</v>
       </c>
       <c r="J69" s="2" t="s">
+        <v>370</v>
+      </c>
+      <c r="K69" s="2" t="n">
+        <v>1420.0</v>
+      </c>
+      <c r="L69" s="2" t="s">
         <v>372</v>
       </c>
-      <c r="K69" s="2" t="n">
-        <v>788.0</v>
-      </c>
-      <c r="L69" s="2" t="s">
-        <v>371</v>
-      </c>
       <c r="M69" s="2" t="n">
-        <v>273.0</v>
+        <v>169.0</v>
       </c>
       <c r="N69" s="2" t="s">
         <v>373</v>
@@ -17708,34 +17708,34 @@
         <v>375</v>
       </c>
       <c r="D70" s="2" t="n">
-        <v>816.0</v>
+        <v>979.0</v>
       </c>
       <c r="E70" s="2" t="s">
         <v>376</v>
       </c>
       <c r="F70" s="2" t="n">
-        <v>189.0</v>
+        <v>247.0</v>
       </c>
       <c r="G70" s="2" t="n">
-        <v>16.0</v>
+        <v>117.0</v>
       </c>
       <c r="H70" s="2" t="s">
         <v>376</v>
       </c>
       <c r="I70" s="2" t="n">
-        <v>1770.0</v>
+        <v>1429.0</v>
       </c>
       <c r="J70" s="2" t="s">
         <v>377</v>
       </c>
       <c r="K70" s="2" t="n">
-        <v>1358.0</v>
+        <v>788.0</v>
       </c>
       <c r="L70" s="2" t="s">
         <v>376</v>
       </c>
       <c r="M70" s="2" t="n">
-        <v>338.0</v>
+        <v>273.0</v>
       </c>
       <c r="N70" s="2" t="s">
         <v>378</v>
@@ -17752,37 +17752,37 @@
         <v>380</v>
       </c>
       <c r="D71" s="2" t="n">
-        <v>957.0</v>
+        <v>816.0</v>
       </c>
       <c r="E71" s="2" t="s">
         <v>381</v>
       </c>
       <c r="F71" s="2" t="n">
-        <v>140.0</v>
+        <v>189.0</v>
       </c>
       <c r="G71" s="2" t="n">
-        <v>480.0</v>
+        <v>16.0</v>
       </c>
       <c r="H71" s="2" t="s">
-        <v>379</v>
+        <v>381</v>
       </c>
       <c r="I71" s="2" t="n">
-        <v>1549.0</v>
+        <v>1770.0</v>
       </c>
       <c r="J71" s="2" t="s">
         <v>382</v>
       </c>
       <c r="K71" s="2" t="n">
-        <v>1415.0</v>
+        <v>1358.0</v>
       </c>
       <c r="L71" s="2" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="M71" s="2" t="n">
-        <v>218.0</v>
+        <v>338.0</v>
       </c>
       <c r="N71" s="2" t="s">
-        <v>378</v>
+        <v>383</v>
       </c>
     </row>
     <row r="72">
@@ -17790,43 +17790,43 @@
         <v>71.0</v>
       </c>
       <c r="B72" s="2" t="s">
+        <v>384</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="D72" s="2" t="n">
+        <v>957.0</v>
+      </c>
+      <c r="E72" s="2" t="s">
+        <v>386</v>
+      </c>
+      <c r="F72" s="2" t="n">
+        <v>140.0</v>
+      </c>
+      <c r="G72" s="2" t="n">
+        <v>480.0</v>
+      </c>
+      <c r="H72" s="2" t="s">
+        <v>384</v>
+      </c>
+      <c r="I72" s="2" t="n">
+        <v>1549.0</v>
+      </c>
+      <c r="J72" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="K72" s="2" t="n">
+        <v>1415.0</v>
+      </c>
+      <c r="L72" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="M72" s="2" t="n">
+        <v>218.0</v>
+      </c>
+      <c r="N72" s="2" t="s">
         <v>383</v>
-      </c>
-      <c r="C72" s="2" t="s">
-        <v>384</v>
-      </c>
-      <c r="D72" s="2" t="n">
-        <v>874.0</v>
-      </c>
-      <c r="E72" s="2" t="s">
-        <v>385</v>
-      </c>
-      <c r="F72" s="2" t="n">
-        <v>307.0</v>
-      </c>
-      <c r="G72" s="2" t="n">
-        <v>49.0</v>
-      </c>
-      <c r="H72" s="2" t="s">
-        <v>386</v>
-      </c>
-      <c r="I72" s="2" t="n">
-        <v>1597.0</v>
-      </c>
-      <c r="J72" s="2" t="s">
-        <v>384</v>
-      </c>
-      <c r="K72" s="2" t="n">
-        <v>962.0</v>
-      </c>
-      <c r="L72" s="2" t="s">
-        <v>386</v>
-      </c>
-      <c r="M72" s="2" t="n">
-        <v>7.0</v>
-      </c>
-      <c r="N72" s="2" t="s">
-        <v>387</v>
       </c>
     </row>
     <row r="73">
@@ -17840,37 +17840,37 @@
         <v>389</v>
       </c>
       <c r="D73" s="2" t="n">
-        <v>967.0</v>
+        <v>874.0</v>
       </c>
       <c r="E73" s="2" t="s">
         <v>390</v>
       </c>
       <c r="F73" s="2" t="n">
-        <v>218.0</v>
+        <v>307.0</v>
       </c>
       <c r="G73" s="2" t="n">
-        <v>20.0</v>
+        <v>49.0</v>
       </c>
       <c r="H73" s="2" t="s">
         <v>391</v>
       </c>
       <c r="I73" s="2" t="n">
-        <v>1457.0</v>
+        <v>1597.0</v>
       </c>
       <c r="J73" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="K73" s="2" t="n">
+        <v>962.0</v>
+      </c>
+      <c r="L73" s="2" t="s">
+        <v>391</v>
+      </c>
+      <c r="M73" s="2" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="N73" s="2" t="s">
         <v>392</v>
-      </c>
-      <c r="K73" s="2" t="n">
-        <v>1239.0</v>
-      </c>
-      <c r="L73" s="2" t="s">
-        <v>390</v>
-      </c>
-      <c r="M73" s="2" t="n">
-        <v>58.0</v>
-      </c>
-      <c r="N73" s="2" t="s">
-        <v>393</v>
       </c>
     </row>
     <row r="74">
@@ -17878,43 +17878,43 @@
         <v>73.0</v>
       </c>
       <c r="B74" s="2" t="s">
+        <v>393</v>
+      </c>
+      <c r="C74" s="2" t="s">
         <v>394</v>
       </c>
-      <c r="C74" s="2" t="s">
+      <c r="D74" s="2" t="n">
+        <v>967.0</v>
+      </c>
+      <c r="E74" s="2" t="s">
         <v>395</v>
       </c>
-      <c r="D74" s="2" t="n">
-        <v>676.0</v>
-      </c>
-      <c r="E74" s="2" t="s">
+      <c r="F74" s="2" t="n">
+        <v>218.0</v>
+      </c>
+      <c r="G74" s="2" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="H74" s="2" t="s">
         <v>396</v>
       </c>
-      <c r="F74" s="2" t="n">
-        <v>346.0</v>
-      </c>
-      <c r="G74" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="H74" s="2" t="s">
+      <c r="I74" s="2" t="n">
+        <v>1457.0</v>
+      </c>
+      <c r="J74" s="2" t="s">
         <v>397</v>
       </c>
-      <c r="I74" s="2" t="n">
-        <v>1576.0</v>
-      </c>
-      <c r="J74" s="2" t="s">
+      <c r="K74" s="2" t="n">
+        <v>1239.0</v>
+      </c>
+      <c r="L74" s="2" t="s">
+        <v>395</v>
+      </c>
+      <c r="M74" s="2" t="n">
+        <v>58.0</v>
+      </c>
+      <c r="N74" s="2" t="s">
         <v>398</v>
-      </c>
-      <c r="K74" s="2" t="n">
-        <v>1283.0</v>
-      </c>
-      <c r="L74" s="2" t="s">
-        <v>394</v>
-      </c>
-      <c r="M74" s="2" t="n">
-        <v>85.0</v>
-      </c>
-      <c r="N74" s="2" t="s">
-        <v>399</v>
       </c>
     </row>
     <row r="75">
@@ -17922,40 +17922,40 @@
         <v>74.0</v>
       </c>
       <c r="B75" s="2" t="s">
+        <v>399</v>
+      </c>
+      <c r="C75" s="2" t="s">
         <v>400</v>
       </c>
-      <c r="C75" s="2" t="s">
+      <c r="D75" s="2" t="n">
+        <v>676.0</v>
+      </c>
+      <c r="E75" s="2" t="s">
         <v>401</v>
       </c>
-      <c r="D75" s="2" t="n">
-        <v>957.0</v>
-      </c>
-      <c r="E75" s="2" t="s">
+      <c r="F75" s="2" t="n">
+        <v>346.0</v>
+      </c>
+      <c r="G75" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H75" s="2" t="s">
         <v>402</v>
-      </c>
-      <c r="F75" s="2" t="n">
-        <v>86.0</v>
-      </c>
-      <c r="G75" s="2" t="n">
-        <v>102.0</v>
-      </c>
-      <c r="H75" s="2" t="s">
-        <v>403</v>
       </c>
       <c r="I75" s="2" t="n">
         <v>1576.0</v>
       </c>
       <c r="J75" s="2" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="K75" s="2" t="n">
-        <v>1387.0</v>
+        <v>1283.0</v>
       </c>
       <c r="L75" s="2" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
       <c r="M75" s="2" t="n">
-        <v>469.0</v>
+        <v>85.0</v>
       </c>
       <c r="N75" s="2" t="s">
         <v>404</v>
@@ -17972,34 +17972,34 @@
         <v>406</v>
       </c>
       <c r="D76" s="2" t="n">
-        <v>690.0</v>
+        <v>957.0</v>
       </c>
       <c r="E76" s="2" t="s">
         <v>407</v>
       </c>
       <c r="F76" s="2" t="n">
-        <v>134.0</v>
+        <v>86.0</v>
       </c>
       <c r="G76" s="2" t="n">
-        <v>544.0</v>
+        <v>102.0</v>
       </c>
       <c r="H76" s="2" t="s">
-        <v>405</v>
+        <v>408</v>
       </c>
       <c r="I76" s="2" t="n">
-        <v>1421.0</v>
+        <v>1576.0</v>
       </c>
       <c r="J76" s="2" t="s">
+        <v>407</v>
+      </c>
+      <c r="K76" s="2" t="n">
+        <v>1387.0</v>
+      </c>
+      <c r="L76" s="2" t="s">
         <v>408</v>
       </c>
-      <c r="K76" s="2" t="n">
-        <v>1321.0</v>
-      </c>
-      <c r="L76" s="2" t="s">
-        <v>405</v>
-      </c>
       <c r="M76" s="2" t="n">
-        <v>997.0</v>
+        <v>469.0</v>
       </c>
       <c r="N76" s="2" t="s">
         <v>409</v>
@@ -18016,37 +18016,37 @@
         <v>411</v>
       </c>
       <c r="D77" s="2" t="n">
-        <v>908.0</v>
+        <v>690.0</v>
       </c>
       <c r="E77" s="2" t="s">
         <v>412</v>
       </c>
       <c r="F77" s="2" t="n">
-        <v>141.0</v>
+        <v>134.0</v>
       </c>
       <c r="G77" s="2" t="n">
-        <v>54.0</v>
+        <v>544.0</v>
       </c>
       <c r="H77" s="2" t="s">
+        <v>410</v>
+      </c>
+      <c r="I77" s="2" t="n">
+        <v>1421.0</v>
+      </c>
+      <c r="J77" s="2" t="s">
         <v>413</v>
       </c>
-      <c r="I77" s="2" t="n">
-        <v>1393.0</v>
-      </c>
-      <c r="J77" s="2" t="s">
+      <c r="K77" s="2" t="n">
+        <v>1321.0</v>
+      </c>
+      <c r="L77" s="2" t="s">
+        <v>410</v>
+      </c>
+      <c r="M77" s="2" t="n">
+        <v>997.0</v>
+      </c>
+      <c r="N77" s="2" t="s">
         <v>414</v>
-      </c>
-      <c r="K77" s="2" t="n">
-        <v>1386.0</v>
-      </c>
-      <c r="L77" s="2" t="s">
-        <v>415</v>
-      </c>
-      <c r="M77" s="2" t="n">
-        <v>442.0</v>
-      </c>
-      <c r="N77" s="2" t="s">
-        <v>416</v>
       </c>
     </row>
     <row r="78">
@@ -18054,43 +18054,43 @@
         <v>77.0</v>
       </c>
       <c r="B78" s="2" t="s">
+        <v>415</v>
+      </c>
+      <c r="C78" s="2" t="s">
+        <v>416</v>
+      </c>
+      <c r="D78" s="2" t="n">
+        <v>908.0</v>
+      </c>
+      <c r="E78" s="2" t="s">
         <v>417</v>
       </c>
-      <c r="C78" s="2" t="s">
+      <c r="F78" s="2" t="n">
+        <v>141.0</v>
+      </c>
+      <c r="G78" s="2" t="n">
+        <v>54.0</v>
+      </c>
+      <c r="H78" s="2" t="s">
         <v>418</v>
       </c>
-      <c r="D78" s="2" t="n">
-        <v>897.0</v>
-      </c>
-      <c r="E78" s="2" t="s">
+      <c r="I78" s="2" t="n">
+        <v>1393.0</v>
+      </c>
+      <c r="J78" s="2" t="s">
         <v>419</v>
       </c>
-      <c r="F78" s="2" t="n">
-        <v>139.0</v>
-      </c>
-      <c r="G78" s="2" t="n">
-        <v>158.0</v>
-      </c>
-      <c r="H78" s="2" t="s">
-        <v>419</v>
-      </c>
-      <c r="I78" s="2" t="n">
-        <v>1448.0</v>
-      </c>
-      <c r="J78" s="2" t="s">
+      <c r="K78" s="2" t="n">
+        <v>1386.0</v>
+      </c>
+      <c r="L78" s="2" t="s">
         <v>420</v>
       </c>
-      <c r="K78" s="2" t="n">
-        <v>1456.0</v>
-      </c>
-      <c r="L78" s="2" t="s">
-        <v>419</v>
-      </c>
       <c r="M78" s="2" t="n">
-        <v>371.0</v>
+        <v>442.0</v>
       </c>
       <c r="N78" s="2" t="s">
-        <v>416</v>
+        <v>421</v>
       </c>
     </row>
     <row r="79">
@@ -18098,43 +18098,43 @@
         <v>78.0</v>
       </c>
       <c r="B79" s="2" t="s">
+        <v>422</v>
+      </c>
+      <c r="C79" s="2" t="s">
+        <v>423</v>
+      </c>
+      <c r="D79" s="2" t="n">
+        <v>897.0</v>
+      </c>
+      <c r="E79" s="2" t="s">
+        <v>424</v>
+      </c>
+      <c r="F79" s="2" t="n">
+        <v>139.0</v>
+      </c>
+      <c r="G79" s="2" t="n">
+        <v>158.0</v>
+      </c>
+      <c r="H79" s="2" t="s">
+        <v>424</v>
+      </c>
+      <c r="I79" s="2" t="n">
+        <v>1448.0</v>
+      </c>
+      <c r="J79" s="2" t="s">
+        <v>425</v>
+      </c>
+      <c r="K79" s="2" t="n">
+        <v>1456.0</v>
+      </c>
+      <c r="L79" s="2" t="s">
+        <v>424</v>
+      </c>
+      <c r="M79" s="2" t="n">
+        <v>371.0</v>
+      </c>
+      <c r="N79" s="2" t="s">
         <v>421</v>
-      </c>
-      <c r="C79" s="2" t="s">
-        <v>422</v>
-      </c>
-      <c r="D79" s="2" t="n">
-        <v>760.0</v>
-      </c>
-      <c r="E79" s="2" t="s">
-        <v>423</v>
-      </c>
-      <c r="F79" s="2" t="n">
-        <v>319.0</v>
-      </c>
-      <c r="G79" s="2" t="n">
-        <v>65.0</v>
-      </c>
-      <c r="H79" s="2" t="s">
-        <v>423</v>
-      </c>
-      <c r="I79" s="2" t="n">
-        <v>1275.0</v>
-      </c>
-      <c r="J79" s="2" t="s">
-        <v>424</v>
-      </c>
-      <c r="K79" s="2" t="n">
-        <v>1226.0</v>
-      </c>
-      <c r="L79" s="2" t="s">
-        <v>421</v>
-      </c>
-      <c r="M79" s="2" t="n">
-        <v>158.0</v>
-      </c>
-      <c r="N79" s="2" t="s">
-        <v>425</v>
       </c>
     </row>
     <row r="80">
@@ -18148,34 +18148,34 @@
         <v>427</v>
       </c>
       <c r="D80" s="2" t="n">
-        <v>575.0</v>
+        <v>760.0</v>
       </c>
       <c r="E80" s="2" t="s">
         <v>428</v>
       </c>
       <c r="F80" s="2" t="n">
-        <v>340.0</v>
+        <v>319.0</v>
       </c>
       <c r="G80" s="2" t="n">
-        <v>0.0</v>
+        <v>65.0</v>
       </c>
       <c r="H80" s="2" t="s">
-        <v>426</v>
+        <v>428</v>
       </c>
       <c r="I80" s="2" t="n">
-        <v>1421.0</v>
+        <v>1275.0</v>
       </c>
       <c r="J80" s="2" t="s">
         <v>429</v>
       </c>
       <c r="K80" s="2" t="n">
-        <v>1080.0</v>
+        <v>1226.0</v>
       </c>
       <c r="L80" s="2" t="s">
         <v>426</v>
       </c>
       <c r="M80" s="2" t="n">
-        <v>567.0</v>
+        <v>158.0</v>
       </c>
       <c r="N80" s="2" t="s">
         <v>430</v>
@@ -18192,37 +18192,37 @@
         <v>432</v>
       </c>
       <c r="D81" s="2" t="n">
-        <v>887.0</v>
+        <v>575.0</v>
       </c>
       <c r="E81" s="2" t="s">
         <v>433</v>
       </c>
       <c r="F81" s="2" t="n">
-        <v>208.0</v>
+        <v>340.0</v>
       </c>
       <c r="G81" s="2" t="n">
-        <v>52.0</v>
+        <v>0.0</v>
       </c>
       <c r="H81" s="2" t="s">
+        <v>431</v>
+      </c>
+      <c r="I81" s="2" t="n">
+        <v>1421.0</v>
+      </c>
+      <c r="J81" s="2" t="s">
         <v>434</v>
       </c>
-      <c r="I81" s="2" t="n">
-        <v>1358.0</v>
-      </c>
-      <c r="J81" s="2" t="s">
+      <c r="K81" s="2" t="n">
+        <v>1080.0</v>
+      </c>
+      <c r="L81" s="2" t="s">
+        <v>431</v>
+      </c>
+      <c r="M81" s="2" t="n">
+        <v>567.0</v>
+      </c>
+      <c r="N81" s="2" t="s">
         <v>435</v>
-      </c>
-      <c r="K81" s="2" t="n">
-        <v>1431.0</v>
-      </c>
-      <c r="L81" s="2" t="s">
-        <v>436</v>
-      </c>
-      <c r="M81" s="2" t="n">
-        <v>142.0</v>
-      </c>
-      <c r="N81" s="2" t="s">
-        <v>437</v>
       </c>
     </row>
     <row r="82">
@@ -18230,40 +18230,40 @@
         <v>81.0</v>
       </c>
       <c r="B82" s="2" t="s">
+        <v>436</v>
+      </c>
+      <c r="C82" s="2" t="s">
+        <v>437</v>
+      </c>
+      <c r="D82" s="2" t="n">
+        <v>887.0</v>
+      </c>
+      <c r="E82" s="2" t="s">
         <v>438</v>
       </c>
-      <c r="C82" s="2" t="s">
+      <c r="F82" s="2" t="n">
+        <v>208.0</v>
+      </c>
+      <c r="G82" s="2" t="n">
+        <v>52.0</v>
+      </c>
+      <c r="H82" s="2" t="s">
         <v>439</v>
       </c>
-      <c r="D82" s="2" t="n">
-        <v>1040.0</v>
-      </c>
-      <c r="E82" s="2" t="s">
+      <c r="I82" s="2" t="n">
+        <v>1358.0</v>
+      </c>
+      <c r="J82" s="2" t="s">
         <v>440</v>
       </c>
-      <c r="F82" s="2" t="n">
-        <v>119.0</v>
-      </c>
-      <c r="G82" s="2" t="n">
-        <v>28.0</v>
-      </c>
-      <c r="H82" s="2" t="s">
-        <v>440</v>
-      </c>
-      <c r="I82" s="2" t="n">
-        <v>1538.0</v>
-      </c>
-      <c r="J82" s="2" t="s">
+      <c r="K82" s="2" t="n">
+        <v>1431.0</v>
+      </c>
+      <c r="L82" s="2" t="s">
         <v>441</v>
       </c>
-      <c r="K82" s="2" t="n">
-        <v>1335.0</v>
-      </c>
-      <c r="L82" s="2" t="s">
-        <v>440</v>
-      </c>
       <c r="M82" s="2" t="n">
-        <v>125.0</v>
+        <v>142.0</v>
       </c>
       <c r="N82" s="2" t="s">
         <v>442</v>
@@ -18280,34 +18280,34 @@
         <v>444</v>
       </c>
       <c r="D83" s="2" t="n">
-        <v>880.0</v>
+        <v>1040.0</v>
       </c>
       <c r="E83" s="2" t="s">
         <v>445</v>
       </c>
       <c r="F83" s="2" t="n">
-        <v>214.0</v>
+        <v>119.0</v>
       </c>
       <c r="G83" s="2" t="n">
-        <v>14.0</v>
+        <v>28.0</v>
       </c>
       <c r="H83" s="2" t="s">
-        <v>443</v>
+        <v>445</v>
       </c>
       <c r="I83" s="2" t="n">
-        <v>1414.0</v>
+        <v>1538.0</v>
       </c>
       <c r="J83" s="2" t="s">
+        <v>446</v>
+      </c>
+      <c r="K83" s="2" t="n">
+        <v>1335.0</v>
+      </c>
+      <c r="L83" s="2" t="s">
         <v>445</v>
       </c>
-      <c r="K83" s="2" t="n">
-        <v>1531.0</v>
-      </c>
-      <c r="L83" s="2" t="s">
-        <v>446</v>
-      </c>
       <c r="M83" s="2" t="n">
-        <v>8.0</v>
+        <v>125.0</v>
       </c>
       <c r="N83" s="2" t="s">
         <v>447</v>
@@ -18324,37 +18324,37 @@
         <v>449</v>
       </c>
       <c r="D84" s="2" t="n">
-        <v>670.0</v>
+        <v>880.0</v>
       </c>
       <c r="E84" s="2" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="F84" s="2" t="n">
-        <v>281.0</v>
+        <v>214.0</v>
       </c>
       <c r="G84" s="2" t="n">
-        <v>454.0</v>
+        <v>14.0</v>
       </c>
       <c r="H84" s="2" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="I84" s="2" t="n">
-        <v>1427.0</v>
+        <v>1414.0</v>
       </c>
       <c r="J84" s="2" t="s">
         <v>450</v>
       </c>
       <c r="K84" s="2" t="n">
-        <v>1314.0</v>
+        <v>1531.0</v>
       </c>
       <c r="L84" s="2" t="s">
-        <v>449</v>
+        <v>451</v>
       </c>
       <c r="M84" s="2" t="n">
-        <v>308.0</v>
+        <v>8.0</v>
       </c>
       <c r="N84" s="2" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
     </row>
     <row r="85">
@@ -18362,43 +18362,43 @@
         <v>84.0</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="D85" s="2" t="n">
-        <v>636.0</v>
+        <v>670.0</v>
       </c>
       <c r="E85" s="2" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="F85" s="2" t="n">
-        <v>368.0</v>
+        <v>281.0</v>
       </c>
       <c r="G85" s="2" t="n">
-        <v>490.0</v>
+        <v>454.0</v>
       </c>
       <c r="H85" s="2" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="I85" s="2" t="n">
-        <v>1506.0</v>
+        <v>1427.0</v>
       </c>
       <c r="J85" s="2" t="s">
+        <v>455</v>
+      </c>
+      <c r="K85" s="2" t="n">
+        <v>1314.0</v>
+      </c>
+      <c r="L85" s="2" t="s">
         <v>454</v>
       </c>
-      <c r="K85" s="2" t="n">
-        <v>1107.0</v>
-      </c>
-      <c r="L85" s="2" t="s">
-        <v>453</v>
-      </c>
       <c r="M85" s="2" t="n">
-        <v>51.0</v>
+        <v>308.0</v>
       </c>
       <c r="N85" s="2" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
     </row>
     <row r="86">
@@ -18406,43 +18406,43 @@
         <v>85.0</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="D86" s="2" t="n">
-        <v>733.0</v>
+        <v>636.0</v>
       </c>
       <c r="E86" s="2" t="s">
         <v>458</v>
       </c>
       <c r="F86" s="2" t="n">
-        <v>334.0</v>
+        <v>368.0</v>
       </c>
       <c r="G86" s="2" t="n">
-        <v>0.0</v>
+        <v>490.0</v>
       </c>
       <c r="H86" s="2" t="s">
+        <v>458</v>
+      </c>
+      <c r="I86" s="2" t="n">
+        <v>1506.0</v>
+      </c>
+      <c r="J86" s="2" t="s">
         <v>459</v>
       </c>
-      <c r="I86" s="2" t="n">
-        <v>1324.0</v>
-      </c>
-      <c r="J86" s="2" t="s">
+      <c r="K86" s="2" t="n">
+        <v>1107.0</v>
+      </c>
+      <c r="L86" s="2" t="s">
+        <v>458</v>
+      </c>
+      <c r="M86" s="2" t="n">
+        <v>51.0</v>
+      </c>
+      <c r="N86" s="2" t="s">
         <v>460</v>
-      </c>
-      <c r="K86" s="2" t="n">
-        <v>1325.0</v>
-      </c>
-      <c r="L86" s="2" t="s">
-        <v>461</v>
-      </c>
-      <c r="M86" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="N86" s="2" t="s">
-        <v>462</v>
       </c>
     </row>
     <row r="87">
@@ -18450,43 +18450,43 @@
         <v>86.0</v>
       </c>
       <c r="B87" s="2" t="s">
+        <v>461</v>
+      </c>
+      <c r="C87" s="2" t="s">
+        <v>462</v>
+      </c>
+      <c r="D87" s="2" t="n">
+        <v>733.0</v>
+      </c>
+      <c r="E87" s="2" t="s">
         <v>463</v>
       </c>
-      <c r="C87" s="2" t="s">
+      <c r="F87" s="2" t="n">
+        <v>334.0</v>
+      </c>
+      <c r="G87" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H87" s="2" t="s">
         <v>464</v>
       </c>
-      <c r="D87" s="2" t="n">
-        <v>790.0</v>
-      </c>
-      <c r="E87" s="2" t="s">
+      <c r="I87" s="2" t="n">
+        <v>1324.0</v>
+      </c>
+      <c r="J87" s="2" t="s">
         <v>465</v>
       </c>
-      <c r="F87" s="2" t="n">
-        <v>232.0</v>
-      </c>
-      <c r="G87" s="2" t="n">
-        <v>572.0</v>
-      </c>
-      <c r="H87" s="2" t="s">
+      <c r="K87" s="2" t="n">
+        <v>1325.0</v>
+      </c>
+      <c r="L87" s="2" t="s">
         <v>466</v>
       </c>
-      <c r="I87" s="2" t="n">
-        <v>1338.0</v>
-      </c>
-      <c r="J87" s="2" t="s">
+      <c r="M87" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="N87" s="2" t="s">
         <v>467</v>
-      </c>
-      <c r="K87" s="2" t="n">
-        <v>910.0</v>
-      </c>
-      <c r="L87" s="2" t="s">
-        <v>465</v>
-      </c>
-      <c r="M87" s="2" t="n">
-        <v>525.0</v>
-      </c>
-      <c r="N87" s="2" t="s">
-        <v>468</v>
       </c>
     </row>
     <row r="88">
@@ -18494,40 +18494,40 @@
         <v>87.0</v>
       </c>
       <c r="B88" s="2" t="s">
+        <v>468</v>
+      </c>
+      <c r="C88" s="2" t="s">
         <v>469</v>
       </c>
-      <c r="C88" s="2" t="s">
+      <c r="D88" s="2" t="n">
+        <v>790.0</v>
+      </c>
+      <c r="E88" s="2" t="s">
         <v>470</v>
       </c>
-      <c r="D88" s="2" t="n">
-        <v>725.0</v>
-      </c>
-      <c r="E88" s="2" t="s">
-        <v>471</v>
-      </c>
       <c r="F88" s="2" t="n">
-        <v>327.0</v>
+        <v>232.0</v>
       </c>
       <c r="G88" s="2" t="n">
-        <v>695.0</v>
+        <v>572.0</v>
       </c>
       <c r="H88" s="2" t="s">
         <v>471</v>
       </c>
       <c r="I88" s="2" t="n">
-        <v>1280.0</v>
+        <v>1338.0</v>
       </c>
       <c r="J88" s="2" t="s">
         <v>472</v>
       </c>
       <c r="K88" s="2" t="n">
-        <v>1174.0</v>
+        <v>910.0</v>
       </c>
       <c r="L88" s="2" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="M88" s="2" t="n">
-        <v>45.0</v>
+        <v>525.0</v>
       </c>
       <c r="N88" s="2" t="s">
         <v>473</v>
@@ -18544,34 +18544,34 @@
         <v>475</v>
       </c>
       <c r="D89" s="2" t="n">
-        <v>712.0</v>
+        <v>725.0</v>
       </c>
       <c r="E89" s="2" t="s">
         <v>476</v>
       </c>
       <c r="F89" s="2" t="n">
-        <v>259.0</v>
+        <v>327.0</v>
       </c>
       <c r="G89" s="2" t="n">
-        <v>173.0</v>
+        <v>695.0</v>
       </c>
       <c r="H89" s="2" t="s">
-        <v>474</v>
+        <v>476</v>
       </c>
       <c r="I89" s="2" t="n">
-        <v>1242.0</v>
+        <v>1280.0</v>
       </c>
       <c r="J89" s="2" t="s">
         <v>477</v>
       </c>
       <c r="K89" s="2" t="n">
-        <v>1094.0</v>
+        <v>1174.0</v>
       </c>
       <c r="L89" s="2" t="s">
         <v>476</v>
       </c>
       <c r="M89" s="2" t="n">
-        <v>587.0</v>
+        <v>45.0</v>
       </c>
       <c r="N89" s="2" t="s">
         <v>478</v>
@@ -18588,37 +18588,37 @@
         <v>480</v>
       </c>
       <c r="D90" s="2" t="n">
-        <v>795.0</v>
+        <v>712.0</v>
       </c>
       <c r="E90" s="2" t="s">
         <v>481</v>
       </c>
       <c r="F90" s="2" t="n">
-        <v>280.0</v>
+        <v>259.0</v>
       </c>
       <c r="G90" s="2" t="n">
-        <v>0.0</v>
+        <v>173.0</v>
       </c>
       <c r="H90" s="2" t="s">
+        <v>479</v>
+      </c>
+      <c r="I90" s="2" t="n">
+        <v>1242.0</v>
+      </c>
+      <c r="J90" s="2" t="s">
         <v>482</v>
       </c>
-      <c r="I90" s="2" t="n">
-        <v>1465.0</v>
-      </c>
-      <c r="J90" s="2" t="s">
+      <c r="K90" s="2" t="n">
+        <v>1094.0</v>
+      </c>
+      <c r="L90" s="2" t="s">
+        <v>481</v>
+      </c>
+      <c r="M90" s="2" t="n">
+        <v>587.0</v>
+      </c>
+      <c r="N90" s="2" t="s">
         <v>483</v>
-      </c>
-      <c r="K90" s="2" t="n">
-        <v>1273.0</v>
-      </c>
-      <c r="L90" s="2" t="s">
-        <v>484</v>
-      </c>
-      <c r="M90" s="2" t="n">
-        <v>18.0</v>
-      </c>
-      <c r="N90" s="2" t="s">
-        <v>478</v>
       </c>
     </row>
     <row r="91">
@@ -18626,43 +18626,43 @@
         <v>90.0</v>
       </c>
       <c r="B91" s="2" t="s">
+        <v>484</v>
+      </c>
+      <c r="C91" s="2" t="s">
         <v>485</v>
       </c>
-      <c r="C91" s="2" t="s">
+      <c r="D91" s="2" t="n">
+        <v>795.0</v>
+      </c>
+      <c r="E91" s="2" t="s">
         <v>486</v>
       </c>
-      <c r="D91" s="2" t="n">
-        <v>915.0</v>
-      </c>
-      <c r="E91" s="2" t="s">
+      <c r="F91" s="2" t="n">
+        <v>280.0</v>
+      </c>
+      <c r="G91" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H91" s="2" t="s">
         <v>487</v>
       </c>
-      <c r="F91" s="2" t="n">
-        <v>256.0</v>
-      </c>
-      <c r="G91" s="2" t="n">
-        <v>62.0</v>
-      </c>
-      <c r="H91" s="2" t="s">
+      <c r="I91" s="2" t="n">
+        <v>1465.0</v>
+      </c>
+      <c r="J91" s="2" t="s">
         <v>488</v>
       </c>
-      <c r="I91" s="2" t="n">
-        <v>1377.0</v>
-      </c>
-      <c r="J91" s="2" t="s">
+      <c r="K91" s="2" t="n">
+        <v>1273.0</v>
+      </c>
+      <c r="L91" s="2" t="s">
         <v>489</v>
       </c>
-      <c r="K91" s="2" t="n">
-        <v>1062.0</v>
-      </c>
-      <c r="L91" s="2" t="s">
-        <v>487</v>
-      </c>
       <c r="M91" s="2" t="n">
-        <v>26.0</v>
+        <v>18.0</v>
       </c>
       <c r="N91" s="2" t="s">
-        <v>478</v>
+        <v>483</v>
       </c>
     </row>
     <row r="92">
@@ -18676,37 +18676,37 @@
         <v>491</v>
       </c>
       <c r="D92" s="2" t="n">
-        <v>839.0</v>
+        <v>915.0</v>
       </c>
       <c r="E92" s="2" t="s">
         <v>492</v>
       </c>
       <c r="F92" s="2" t="n">
-        <v>238.0</v>
+        <v>256.0</v>
       </c>
       <c r="G92" s="2" t="n">
-        <v>4.0</v>
+        <v>62.0</v>
       </c>
       <c r="H92" s="2" t="s">
         <v>493</v>
       </c>
       <c r="I92" s="2" t="n">
-        <v>1445.0</v>
+        <v>1377.0</v>
       </c>
       <c r="J92" s="2" t="s">
-        <v>491</v>
+        <v>494</v>
       </c>
       <c r="K92" s="2" t="n">
-        <v>1422.0</v>
+        <v>1062.0</v>
       </c>
       <c r="L92" s="2" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="M92" s="2" t="n">
-        <v>0.0</v>
+        <v>26.0</v>
       </c>
       <c r="N92" s="2" t="s">
-        <v>495</v>
+        <v>483</v>
       </c>
     </row>
     <row r="93">
@@ -18714,40 +18714,40 @@
         <v>92.0</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="C93" s="2" t="s">
         <v>496</v>
       </c>
       <c r="D93" s="2" t="n">
-        <v>834.0</v>
+        <v>839.0</v>
       </c>
       <c r="E93" s="2" t="s">
         <v>497</v>
       </c>
       <c r="F93" s="2" t="n">
-        <v>159.0</v>
+        <v>238.0</v>
       </c>
       <c r="G93" s="2" t="n">
-        <v>146.0</v>
+        <v>4.0</v>
       </c>
       <c r="H93" s="2" t="s">
+        <v>498</v>
+      </c>
+      <c r="I93" s="2" t="n">
+        <v>1445.0</v>
+      </c>
+      <c r="J93" s="2" t="s">
         <v>496</v>
       </c>
-      <c r="I93" s="2" t="n">
-        <v>1470.0</v>
-      </c>
-      <c r="J93" s="2" t="s">
-        <v>498</v>
-      </c>
       <c r="K93" s="2" t="n">
-        <v>1262.0</v>
+        <v>1422.0</v>
       </c>
       <c r="L93" s="2" t="s">
         <v>499</v>
       </c>
       <c r="M93" s="2" t="n">
-        <v>465.0</v>
+        <v>0.0</v>
       </c>
       <c r="N93" s="2" t="s">
         <v>500</v>
@@ -18761,37 +18761,37 @@
         <v>501</v>
       </c>
       <c r="C94" s="2" t="s">
+        <v>501</v>
+      </c>
+      <c r="D94" s="2" t="n">
+        <v>834.0</v>
+      </c>
+      <c r="E94" s="2" t="s">
         <v>502</v>
       </c>
-      <c r="D94" s="2" t="n">
-        <v>1147.0</v>
-      </c>
-      <c r="E94" s="2" t="s">
+      <c r="F94" s="2" t="n">
+        <v>159.0</v>
+      </c>
+      <c r="G94" s="2" t="n">
+        <v>146.0</v>
+      </c>
+      <c r="H94" s="2" t="s">
+        <v>501</v>
+      </c>
+      <c r="I94" s="2" t="n">
+        <v>1470.0</v>
+      </c>
+      <c r="J94" s="2" t="s">
         <v>503</v>
       </c>
-      <c r="F94" s="2" t="n">
-        <v>48.0</v>
-      </c>
-      <c r="G94" s="2" t="n">
-        <v>38.0</v>
-      </c>
-      <c r="H94" s="2" t="s">
-        <v>503</v>
-      </c>
-      <c r="I94" s="2" t="n">
-        <v>1434.0</v>
-      </c>
-      <c r="J94" s="2" t="s">
+      <c r="K94" s="2" t="n">
+        <v>1262.0</v>
+      </c>
+      <c r="L94" s="2" t="s">
         <v>504</v>
       </c>
-      <c r="K94" s="2" t="n">
-        <v>1478.0</v>
-      </c>
-      <c r="L94" s="2" t="s">
-        <v>503</v>
-      </c>
       <c r="M94" s="2" t="n">
-        <v>46.0</v>
+        <v>465.0</v>
       </c>
       <c r="N94" s="2" t="s">
         <v>505</v>
@@ -18808,34 +18808,34 @@
         <v>507</v>
       </c>
       <c r="D95" s="2" t="n">
-        <v>848.0</v>
+        <v>1147.0</v>
       </c>
       <c r="E95" s="2" t="s">
         <v>508</v>
       </c>
       <c r="F95" s="2" t="n">
-        <v>213.0</v>
+        <v>48.0</v>
       </c>
       <c r="G95" s="2" t="n">
-        <v>4.0</v>
+        <v>38.0</v>
       </c>
       <c r="H95" s="2" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="I95" s="2" t="n">
-        <v>1337.0</v>
+        <v>1434.0</v>
       </c>
       <c r="J95" s="2" t="s">
         <v>509</v>
       </c>
       <c r="K95" s="2" t="n">
-        <v>1341.0</v>
+        <v>1478.0</v>
       </c>
       <c r="L95" s="2" t="s">
         <v>508</v>
       </c>
       <c r="M95" s="2" t="n">
-        <v>205.0</v>
+        <v>46.0</v>
       </c>
       <c r="N95" s="2" t="s">
         <v>510</v>
@@ -18852,34 +18852,34 @@
         <v>512</v>
       </c>
       <c r="D96" s="2" t="n">
-        <v>779.0</v>
+        <v>848.0</v>
       </c>
       <c r="E96" s="2" t="s">
         <v>513</v>
       </c>
       <c r="F96" s="2" t="n">
-        <v>225.0</v>
+        <v>213.0</v>
       </c>
       <c r="G96" s="2" t="n">
-        <v>133.0</v>
+        <v>4.0</v>
       </c>
       <c r="H96" s="2" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="I96" s="2" t="n">
-        <v>1550.0</v>
+        <v>1337.0</v>
       </c>
       <c r="J96" s="2" t="s">
         <v>514</v>
       </c>
       <c r="K96" s="2" t="n">
-        <v>1386.0</v>
+        <v>1341.0</v>
       </c>
       <c r="L96" s="2" t="s">
         <v>513</v>
       </c>
       <c r="M96" s="2" t="n">
-        <v>120.0</v>
+        <v>205.0</v>
       </c>
       <c r="N96" s="2" t="s">
         <v>515</v>
@@ -18896,37 +18896,37 @@
         <v>517</v>
       </c>
       <c r="D97" s="2" t="n">
-        <v>966.0</v>
+        <v>779.0</v>
       </c>
       <c r="E97" s="2" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
       <c r="F97" s="2" t="n">
-        <v>167.0</v>
+        <v>225.0</v>
       </c>
       <c r="G97" s="2" t="n">
-        <v>30.0</v>
+        <v>133.0</v>
       </c>
       <c r="H97" s="2" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
       <c r="I97" s="2" t="n">
-        <v>1450.0</v>
+        <v>1550.0</v>
       </c>
       <c r="J97" s="2" t="s">
+        <v>519</v>
+      </c>
+      <c r="K97" s="2" t="n">
+        <v>1386.0</v>
+      </c>
+      <c r="L97" s="2" t="s">
         <v>518</v>
       </c>
-      <c r="K97" s="2" t="n">
-        <v>1235.0</v>
-      </c>
-      <c r="L97" s="2" t="s">
-        <v>517</v>
-      </c>
       <c r="M97" s="2" t="n">
-        <v>107.0</v>
+        <v>120.0</v>
       </c>
       <c r="N97" s="2" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
     </row>
     <row r="98">
@@ -18934,40 +18934,40 @@
         <v>97.0</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
       <c r="D98" s="2" t="n">
-        <v>920.0</v>
+        <v>966.0</v>
       </c>
       <c r="E98" s="2" t="s">
         <v>522</v>
       </c>
       <c r="F98" s="2" t="n">
-        <v>179.0</v>
+        <v>167.0</v>
       </c>
       <c r="G98" s="2" t="n">
-        <v>19.0</v>
+        <v>30.0</v>
       </c>
       <c r="H98" s="2" t="s">
         <v>522</v>
       </c>
       <c r="I98" s="2" t="n">
-        <v>1536.0</v>
+        <v>1450.0</v>
       </c>
       <c r="J98" s="2" t="s">
         <v>523</v>
       </c>
       <c r="K98" s="2" t="n">
-        <v>1107.0</v>
+        <v>1235.0</v>
       </c>
       <c r="L98" s="2" t="s">
         <v>522</v>
       </c>
       <c r="M98" s="2" t="n">
-        <v>190.0</v>
+        <v>107.0</v>
       </c>
       <c r="N98" s="2" t="s">
         <v>524</v>
@@ -18984,37 +18984,37 @@
         <v>526</v>
       </c>
       <c r="D99" s="2" t="n">
-        <v>837.0</v>
+        <v>920.0</v>
       </c>
       <c r="E99" s="2" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
       <c r="F99" s="2" t="n">
-        <v>240.0</v>
+        <v>179.0</v>
       </c>
       <c r="G99" s="2" t="n">
-        <v>56.0</v>
+        <v>19.0</v>
       </c>
       <c r="H99" s="2" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
       <c r="I99" s="2" t="n">
-        <v>1453.0</v>
+        <v>1536.0</v>
       </c>
       <c r="J99" s="2" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
       <c r="K99" s="2" t="n">
-        <v>1312.0</v>
+        <v>1107.0</v>
       </c>
       <c r="L99" s="2" t="s">
         <v>527</v>
       </c>
       <c r="M99" s="2" t="n">
-        <v>0.0</v>
+        <v>190.0</v>
       </c>
       <c r="N99" s="2" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
     </row>
     <row r="100">
@@ -19022,43 +19022,43 @@
         <v>99.0</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="D100" s="2" t="n">
-        <v>1146.0</v>
+        <v>837.0</v>
       </c>
       <c r="E100" s="2" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="F100" s="2" t="n">
-        <v>210.0</v>
+        <v>240.0</v>
       </c>
       <c r="G100" s="2" t="n">
-        <v>0.0</v>
+        <v>56.0</v>
       </c>
       <c r="H100" s="2" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="I100" s="2" t="n">
-        <v>1876.0</v>
+        <v>1453.0</v>
       </c>
       <c r="J100" s="2" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="K100" s="2" t="n">
-        <v>0.0</v>
+        <v>1312.0</v>
       </c>
       <c r="L100" s="2" t="s">
-        <v>530</v>
+        <v>532</v>
       </c>
       <c r="M100" s="2" t="n">
-        <v>56.0</v>
+        <v>0.0</v>
       </c>
       <c r="N100" s="2" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
     </row>
     <row r="101">
@@ -19066,43 +19066,43 @@
         <v>100.0</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>533</v>
+        <v>534</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="D101" s="2" t="n">
-        <v>830.0</v>
+        <v>1146.0</v>
       </c>
       <c r="E101" s="2" t="s">
         <v>535</v>
       </c>
       <c r="F101" s="2" t="n">
-        <v>190.0</v>
+        <v>210.0</v>
       </c>
       <c r="G101" s="2" t="n">
-        <v>1297.0</v>
+        <v>0.0</v>
       </c>
       <c r="H101" s="2" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="I101" s="2" t="n">
-        <v>1424.0</v>
+        <v>1876.0</v>
       </c>
       <c r="J101" s="2" t="s">
         <v>536</v>
       </c>
       <c r="K101" s="2" t="n">
-        <v>840.0</v>
+        <v>0.0</v>
       </c>
       <c r="L101" s="2" t="s">
+        <v>535</v>
+      </c>
+      <c r="M101" s="2" t="n">
+        <v>56.0</v>
+      </c>
+      <c r="N101" s="2" t="s">
         <v>537</v>
-      </c>
-      <c r="M101" s="2" t="n">
-        <v>381.0</v>
-      </c>
-      <c r="N101" s="2" t="s">
-        <v>538</v>
       </c>
     </row>
     <row r="102">
@@ -19110,43 +19110,43 @@
         <v>101.0</v>
       </c>
       <c r="B102" s="2" t="s">
+        <v>538</v>
+      </c>
+      <c r="C102" s="2" t="s">
         <v>539</v>
       </c>
-      <c r="C102" s="2" t="s">
+      <c r="D102" s="2" t="n">
+        <v>830.0</v>
+      </c>
+      <c r="E102" s="2" t="s">
         <v>540</v>
       </c>
-      <c r="D102" s="2" t="n">
-        <v>718.0</v>
-      </c>
-      <c r="E102" s="2" t="s">
+      <c r="F102" s="2" t="n">
+        <v>190.0</v>
+      </c>
+      <c r="G102" s="2" t="n">
+        <v>1297.0</v>
+      </c>
+      <c r="H102" s="2" t="s">
         <v>541</v>
       </c>
-      <c r="F102" s="2" t="n">
-        <v>145.0</v>
-      </c>
-      <c r="G102" s="2" t="n">
-        <v>703.0</v>
-      </c>
-      <c r="H102" s="2" t="s">
+      <c r="I102" s="2" t="n">
+        <v>1424.0</v>
+      </c>
+      <c r="J102" s="2" t="s">
+        <v>541</v>
+      </c>
+      <c r="K102" s="2" t="n">
+        <v>840.0</v>
+      </c>
+      <c r="L102" s="2" t="s">
         <v>542</v>
       </c>
-      <c r="I102" s="2" t="n">
-        <v>1370.0</v>
-      </c>
-      <c r="J102" s="2" t="s">
+      <c r="M102" s="2" t="n">
+        <v>381.0</v>
+      </c>
+      <c r="N102" s="2" t="s">
         <v>543</v>
-      </c>
-      <c r="K102" s="2" t="n">
-        <v>1115.0</v>
-      </c>
-      <c r="L102" s="2" t="s">
-        <v>544</v>
-      </c>
-      <c r="M102" s="2" t="n">
-        <v>825.0</v>
-      </c>
-      <c r="N102" s="2" t="s">
-        <v>545</v>
       </c>
     </row>
     <row r="103">
@@ -19154,40 +19154,40 @@
         <v>102.0</v>
       </c>
       <c r="B103" s="2" t="s">
+        <v>544</v>
+      </c>
+      <c r="C103" s="2" t="s">
+        <v>545</v>
+      </c>
+      <c r="D103" s="2" t="n">
+        <v>718.0</v>
+      </c>
+      <c r="E103" s="2" t="s">
         <v>546</v>
       </c>
-      <c r="C103" s="2" t="s">
+      <c r="F103" s="2" t="n">
+        <v>145.0</v>
+      </c>
+      <c r="G103" s="2" t="n">
+        <v>703.0</v>
+      </c>
+      <c r="H103" s="2" t="s">
         <v>547</v>
       </c>
-      <c r="D103" s="2" t="n">
-        <v>854.0</v>
-      </c>
-      <c r="E103" s="2" t="s">
+      <c r="I103" s="2" t="n">
+        <v>1370.0</v>
+      </c>
+      <c r="J103" s="2" t="s">
         <v>548</v>
       </c>
-      <c r="F103" s="2" t="n">
-        <v>167.0</v>
-      </c>
-      <c r="G103" s="2" t="n">
-        <v>96.0</v>
-      </c>
-      <c r="H103" s="2" t="s">
+      <c r="K103" s="2" t="n">
+        <v>1115.0</v>
+      </c>
+      <c r="L103" s="2" t="s">
         <v>549</v>
       </c>
-      <c r="I103" s="2" t="n">
-        <v>1451.0</v>
-      </c>
-      <c r="J103" s="2" t="s">
-        <v>549</v>
-      </c>
-      <c r="K103" s="2" t="n">
-        <v>1402.0</v>
-      </c>
-      <c r="L103" s="2" t="s">
-        <v>548</v>
-      </c>
       <c r="M103" s="2" t="n">
-        <v>193.0</v>
+        <v>825.0</v>
       </c>
       <c r="N103" s="2" t="s">
         <v>550</v>
@@ -19204,34 +19204,34 @@
         <v>552</v>
       </c>
       <c r="D104" s="2" t="n">
-        <v>907.0</v>
+        <v>854.0</v>
       </c>
       <c r="E104" s="2" t="s">
         <v>553</v>
       </c>
       <c r="F104" s="2" t="n">
-        <v>77.0</v>
+        <v>167.0</v>
       </c>
       <c r="G104" s="2" t="n">
-        <v>378.0</v>
+        <v>96.0</v>
       </c>
       <c r="H104" s="2" t="s">
         <v>554</v>
       </c>
       <c r="I104" s="2" t="n">
-        <v>1455.0</v>
+        <v>1451.0</v>
       </c>
       <c r="J104" s="2" t="s">
         <v>554</v>
       </c>
       <c r="K104" s="2" t="n">
-        <v>1348.0</v>
+        <v>1402.0</v>
       </c>
       <c r="L104" s="2" t="s">
-        <v>551</v>
+        <v>553</v>
       </c>
       <c r="M104" s="2" t="n">
-        <v>466.0</v>
+        <v>193.0</v>
       </c>
       <c r="N104" s="2" t="s">
         <v>555</v>
@@ -19248,34 +19248,34 @@
         <v>557</v>
       </c>
       <c r="D105" s="2" t="n">
-        <v>820.0</v>
+        <v>907.0</v>
       </c>
       <c r="E105" s="2" t="s">
         <v>558</v>
       </c>
       <c r="F105" s="2" t="n">
-        <v>186.0</v>
+        <v>77.0</v>
       </c>
       <c r="G105" s="2" t="n">
-        <v>159.0</v>
+        <v>378.0</v>
       </c>
       <c r="H105" s="2" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
       <c r="I105" s="2" t="n">
-        <v>1354.0</v>
+        <v>1455.0</v>
       </c>
       <c r="J105" s="2" t="s">
         <v>559</v>
       </c>
       <c r="K105" s="2" t="n">
-        <v>1376.0</v>
+        <v>1348.0</v>
       </c>
       <c r="L105" s="2" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="M105" s="2" t="n">
-        <v>214.0</v>
+        <v>466.0</v>
       </c>
       <c r="N105" s="2" t="s">
         <v>560</v>
@@ -19292,34 +19292,34 @@
         <v>562</v>
       </c>
       <c r="D106" s="2" t="n">
-        <v>812.0</v>
+        <v>820.0</v>
       </c>
       <c r="E106" s="2" t="s">
         <v>563</v>
       </c>
       <c r="F106" s="2" t="n">
-        <v>244.0</v>
+        <v>186.0</v>
       </c>
       <c r="G106" s="2" t="n">
-        <v>15.0</v>
+        <v>159.0</v>
       </c>
       <c r="H106" s="2" t="s">
         <v>563</v>
       </c>
       <c r="I106" s="2" t="n">
-        <v>1452.0</v>
+        <v>1354.0</v>
       </c>
       <c r="J106" s="2" t="s">
         <v>564</v>
       </c>
       <c r="K106" s="2" t="n">
-        <v>1216.0</v>
+        <v>1376.0</v>
       </c>
       <c r="L106" s="2" t="s">
         <v>563</v>
       </c>
       <c r="M106" s="2" t="n">
-        <v>25.0</v>
+        <v>214.0</v>
       </c>
       <c r="N106" s="2" t="s">
         <v>565</v>
@@ -19336,34 +19336,34 @@
         <v>567</v>
       </c>
       <c r="D107" s="2" t="n">
-        <v>770.0</v>
+        <v>812.0</v>
       </c>
       <c r="E107" s="2" t="s">
         <v>568</v>
       </c>
       <c r="F107" s="2" t="n">
-        <v>163.0</v>
+        <v>244.0</v>
       </c>
       <c r="G107" s="2" t="n">
-        <v>190.0</v>
+        <v>15.0</v>
       </c>
       <c r="H107" s="2" t="s">
         <v>568</v>
       </c>
       <c r="I107" s="2" t="n">
-        <v>1254.0</v>
+        <v>1452.0</v>
       </c>
       <c r="J107" s="2" t="s">
+        <v>569</v>
+      </c>
+      <c r="K107" s="2" t="n">
+        <v>1216.0</v>
+      </c>
+      <c r="L107" s="2" t="s">
         <v>568</v>
       </c>
-      <c r="K107" s="2" t="n">
-        <v>1262.0</v>
-      </c>
-      <c r="L107" s="2" t="s">
-        <v>569</v>
-      </c>
       <c r="M107" s="2" t="n">
-        <v>544.0</v>
+        <v>25.0</v>
       </c>
       <c r="N107" s="2" t="s">
         <v>570</v>
@@ -19380,34 +19380,34 @@
         <v>572</v>
       </c>
       <c r="D108" s="2" t="n">
-        <v>501.0</v>
+        <v>770.0</v>
       </c>
       <c r="E108" s="2" t="s">
         <v>573</v>
       </c>
       <c r="F108" s="2" t="n">
-        <v>214.0</v>
+        <v>163.0</v>
       </c>
       <c r="G108" s="2" t="n">
-        <v>849.0</v>
+        <v>190.0</v>
       </c>
       <c r="H108" s="2" t="s">
+        <v>573</v>
+      </c>
+      <c r="I108" s="2" t="n">
+        <v>1254.0</v>
+      </c>
+      <c r="J108" s="2" t="s">
+        <v>573</v>
+      </c>
+      <c r="K108" s="2" t="n">
+        <v>1262.0</v>
+      </c>
+      <c r="L108" s="2" t="s">
         <v>574</v>
       </c>
-      <c r="I108" s="2" t="n">
-        <v>1180.0</v>
-      </c>
-      <c r="J108" s="2" t="s">
-        <v>574</v>
-      </c>
-      <c r="K108" s="2" t="n">
-        <v>1145.0</v>
-      </c>
-      <c r="L108" s="2" t="s">
-        <v>571</v>
-      </c>
       <c r="M108" s="2" t="n">
-        <v>1006.0</v>
+        <v>544.0</v>
       </c>
       <c r="N108" s="2" t="s">
         <v>575</v>
@@ -19424,34 +19424,34 @@
         <v>577</v>
       </c>
       <c r="D109" s="2" t="n">
-        <v>595.0</v>
+        <v>501.0</v>
       </c>
       <c r="E109" s="2" t="s">
-        <v>576</v>
+        <v>578</v>
       </c>
       <c r="F109" s="2" t="n">
-        <v>262.0</v>
+        <v>214.0</v>
       </c>
       <c r="G109" s="2" t="n">
-        <v>135.0</v>
+        <v>849.0</v>
       </c>
       <c r="H109" s="2" t="s">
-        <v>578</v>
+        <v>579</v>
       </c>
       <c r="I109" s="2" t="n">
-        <v>1367.0</v>
+        <v>1180.0</v>
       </c>
       <c r="J109" s="2" t="s">
         <v>579</v>
       </c>
       <c r="K109" s="2" t="n">
-        <v>1002.0</v>
+        <v>1145.0</v>
       </c>
       <c r="L109" s="2" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="M109" s="2" t="n">
-        <v>644.0</v>
+        <v>1006.0</v>
       </c>
       <c r="N109" s="2" t="s">
         <v>580</v>
@@ -19468,34 +19468,34 @@
         <v>582</v>
       </c>
       <c r="D110" s="2" t="n">
-        <v>814.0</v>
+        <v>595.0</v>
       </c>
       <c r="E110" s="2" t="s">
+        <v>581</v>
+      </c>
+      <c r="F110" s="2" t="n">
+        <v>262.0</v>
+      </c>
+      <c r="G110" s="2" t="n">
+        <v>135.0</v>
+      </c>
+      <c r="H110" s="2" t="s">
         <v>583</v>
       </c>
-      <c r="F110" s="2" t="n">
-        <v>168.0</v>
-      </c>
-      <c r="G110" s="2" t="n">
-        <v>104.0</v>
-      </c>
-      <c r="H110" s="2" t="s">
-        <v>581</v>
-      </c>
       <c r="I110" s="2" t="n">
-        <v>1530.0</v>
+        <v>1367.0</v>
       </c>
       <c r="J110" s="2" t="s">
         <v>584</v>
       </c>
       <c r="K110" s="2" t="n">
-        <v>1268.0</v>
+        <v>1002.0</v>
       </c>
       <c r="L110" s="2" t="s">
         <v>583</v>
       </c>
       <c r="M110" s="2" t="n">
-        <v>186.0</v>
+        <v>644.0</v>
       </c>
       <c r="N110" s="2" t="s">
         <v>585</v>
@@ -19512,34 +19512,34 @@
         <v>587</v>
       </c>
       <c r="D111" s="2" t="n">
-        <v>913.0</v>
+        <v>814.0</v>
       </c>
       <c r="E111" s="2" t="s">
         <v>588</v>
       </c>
       <c r="F111" s="2" t="n">
-        <v>169.0</v>
+        <v>168.0</v>
       </c>
       <c r="G111" s="2" t="n">
-        <v>94.0</v>
+        <v>104.0</v>
       </c>
       <c r="H111" s="2" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="I111" s="2" t="n">
-        <v>1392.0</v>
+        <v>1530.0</v>
       </c>
       <c r="J111" s="2" t="s">
         <v>589</v>
       </c>
       <c r="K111" s="2" t="n">
-        <v>1025.0</v>
+        <v>1268.0</v>
       </c>
       <c r="L111" s="2" t="s">
-        <v>586</v>
+        <v>588</v>
       </c>
       <c r="M111" s="2" t="n">
-        <v>167.0</v>
+        <v>186.0</v>
       </c>
       <c r="N111" s="2" t="s">
         <v>590</v>
@@ -19556,37 +19556,37 @@
         <v>592</v>
       </c>
       <c r="D112" s="2" t="n">
-        <v>860.0</v>
+        <v>913.0</v>
       </c>
       <c r="E112" s="2" t="s">
         <v>593</v>
       </c>
       <c r="F112" s="2" t="n">
-        <v>139.0</v>
+        <v>169.0</v>
       </c>
       <c r="G112" s="2" t="n">
-        <v>75.0</v>
+        <v>94.0</v>
       </c>
       <c r="H112" s="2" t="s">
+        <v>593</v>
+      </c>
+      <c r="I112" s="2" t="n">
+        <v>1392.0</v>
+      </c>
+      <c r="J112" s="2" t="s">
         <v>594</v>
       </c>
-      <c r="I112" s="2" t="n">
-        <v>1398.0</v>
-      </c>
-      <c r="J112" s="2" t="s">
+      <c r="K112" s="2" t="n">
+        <v>1025.0</v>
+      </c>
+      <c r="L112" s="2" t="s">
+        <v>591</v>
+      </c>
+      <c r="M112" s="2" t="n">
+        <v>167.0</v>
+      </c>
+      <c r="N112" s="2" t="s">
         <v>595</v>
-      </c>
-      <c r="K112" s="2" t="n">
-        <v>1522.0</v>
-      </c>
-      <c r="L112" s="2" t="s">
-        <v>596</v>
-      </c>
-      <c r="M112" s="2" t="n">
-        <v>59.0</v>
-      </c>
-      <c r="N112" s="2" t="s">
-        <v>597</v>
       </c>
     </row>
     <row r="113">
@@ -19594,40 +19594,40 @@
         <v>112.0</v>
       </c>
       <c r="B113" s="2" t="s">
+        <v>596</v>
+      </c>
+      <c r="C113" s="2" t="s">
+        <v>597</v>
+      </c>
+      <c r="D113" s="2" t="n">
+        <v>860.0</v>
+      </c>
+      <c r="E113" s="2" t="s">
         <v>598</v>
       </c>
-      <c r="C113" s="2" t="s">
+      <c r="F113" s="2" t="n">
+        <v>139.0</v>
+      </c>
+      <c r="G113" s="2" t="n">
+        <v>75.0</v>
+      </c>
+      <c r="H113" s="2" t="s">
         <v>599</v>
       </c>
-      <c r="D113" s="2" t="n">
-        <v>867.0</v>
-      </c>
-      <c r="E113" s="2" t="s">
+      <c r="I113" s="2" t="n">
+        <v>1398.0</v>
+      </c>
+      <c r="J113" s="2" t="s">
         <v>600</v>
       </c>
-      <c r="F113" s="2" t="n">
-        <v>179.0</v>
-      </c>
-      <c r="G113" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="H113" s="2" t="s">
-        <v>601</v>
-      </c>
-      <c r="I113" s="2" t="n">
-        <v>1722.0</v>
-      </c>
-      <c r="J113" s="2" t="s">
-        <v>599</v>
-      </c>
       <c r="K113" s="2" t="n">
-        <v>851.0</v>
+        <v>1522.0</v>
       </c>
       <c r="L113" s="2" t="s">
         <v>601</v>
       </c>
       <c r="M113" s="2" t="n">
-        <v>159.0</v>
+        <v>59.0</v>
       </c>
       <c r="N113" s="2" t="s">
         <v>602</v>
@@ -19644,34 +19644,34 @@
         <v>604</v>
       </c>
       <c r="D114" s="2" t="n">
-        <v>643.0</v>
+        <v>867.0</v>
       </c>
       <c r="E114" s="2" t="s">
         <v>605</v>
       </c>
       <c r="F114" s="2" t="n">
-        <v>267.0</v>
+        <v>179.0</v>
       </c>
       <c r="G114" s="2" t="n">
-        <v>86.0</v>
+        <v>0.0</v>
       </c>
       <c r="H114" s="2" t="s">
-        <v>605</v>
+        <v>606</v>
       </c>
       <c r="I114" s="2" t="n">
-        <v>1243.0</v>
+        <v>1722.0</v>
       </c>
       <c r="J114" s="2" t="s">
+        <v>604</v>
+      </c>
+      <c r="K114" s="2" t="n">
+        <v>851.0</v>
+      </c>
+      <c r="L114" s="2" t="s">
         <v>606</v>
       </c>
-      <c r="K114" s="2" t="n">
-        <v>1180.0</v>
-      </c>
-      <c r="L114" s="2" t="s">
-        <v>605</v>
-      </c>
       <c r="M114" s="2" t="n">
-        <v>369.0</v>
+        <v>159.0</v>
       </c>
       <c r="N114" s="2" t="s">
         <v>607</v>
@@ -19688,34 +19688,34 @@
         <v>609</v>
       </c>
       <c r="D115" s="2" t="n">
-        <v>921.0</v>
+        <v>643.0</v>
       </c>
       <c r="E115" s="2" t="s">
         <v>610</v>
       </c>
       <c r="F115" s="2" t="n">
-        <v>120.0</v>
+        <v>267.0</v>
       </c>
       <c r="G115" s="2" t="n">
-        <v>51.0</v>
+        <v>86.0</v>
       </c>
       <c r="H115" s="2" t="s">
         <v>610</v>
       </c>
       <c r="I115" s="2" t="n">
-        <v>1330.0</v>
+        <v>1243.0</v>
       </c>
       <c r="J115" s="2" t="s">
         <v>611</v>
       </c>
       <c r="K115" s="2" t="n">
-        <v>1360.0</v>
+        <v>1180.0</v>
       </c>
       <c r="L115" s="2" t="s">
         <v>610</v>
       </c>
       <c r="M115" s="2" t="n">
-        <v>156.0</v>
+        <v>369.0</v>
       </c>
       <c r="N115" s="2" t="s">
         <v>612</v>
@@ -19732,34 +19732,34 @@
         <v>614</v>
       </c>
       <c r="D116" s="2" t="n">
-        <v>795.0</v>
+        <v>921.0</v>
       </c>
       <c r="E116" s="2" t="s">
         <v>615</v>
       </c>
       <c r="F116" s="2" t="n">
-        <v>89.0</v>
+        <v>120.0</v>
       </c>
       <c r="G116" s="2" t="n">
-        <v>198.0</v>
+        <v>51.0</v>
       </c>
       <c r="H116" s="2" t="s">
-        <v>613</v>
+        <v>615</v>
       </c>
       <c r="I116" s="2" t="n">
-        <v>1338.0</v>
+        <v>1330.0</v>
       </c>
       <c r="J116" s="2" t="s">
         <v>616</v>
       </c>
       <c r="K116" s="2" t="n">
-        <v>1286.0</v>
+        <v>1360.0</v>
       </c>
       <c r="L116" s="2" t="s">
         <v>615</v>
       </c>
       <c r="M116" s="2" t="n">
-        <v>629.0</v>
+        <v>156.0</v>
       </c>
       <c r="N116" s="2" t="s">
         <v>617</v>
@@ -19776,34 +19776,34 @@
         <v>619</v>
       </c>
       <c r="D117" s="2" t="n">
-        <v>828.0</v>
+        <v>795.0</v>
       </c>
       <c r="E117" s="2" t="s">
         <v>620</v>
       </c>
       <c r="F117" s="2" t="n">
-        <v>79.0</v>
+        <v>89.0</v>
       </c>
       <c r="G117" s="2" t="n">
-        <v>63.0</v>
+        <v>198.0</v>
       </c>
       <c r="H117" s="2" t="s">
         <v>618</v>
       </c>
       <c r="I117" s="2" t="n">
-        <v>1602.0</v>
+        <v>1338.0</v>
       </c>
       <c r="J117" s="2" t="s">
+        <v>621</v>
+      </c>
+      <c r="K117" s="2" t="n">
+        <v>1286.0</v>
+      </c>
+      <c r="L117" s="2" t="s">
         <v>620</v>
       </c>
-      <c r="K117" s="2" t="n">
-        <v>1375.0</v>
-      </c>
-      <c r="L117" s="2" t="s">
-        <v>621</v>
-      </c>
       <c r="M117" s="2" t="n">
-        <v>367.0</v>
+        <v>629.0</v>
       </c>
       <c r="N117" s="2" t="s">
         <v>622</v>
@@ -19820,34 +19820,34 @@
         <v>624</v>
       </c>
       <c r="D118" s="2" t="n">
-        <v>767.0</v>
+        <v>828.0</v>
       </c>
       <c r="E118" s="2" t="s">
         <v>625</v>
       </c>
       <c r="F118" s="2" t="n">
-        <v>208.0</v>
+        <v>79.0</v>
       </c>
       <c r="G118" s="2" t="n">
-        <v>73.0</v>
+        <v>63.0</v>
       </c>
       <c r="H118" s="2" t="s">
         <v>623</v>
       </c>
       <c r="I118" s="2" t="n">
-        <v>1321.0</v>
+        <v>1602.0</v>
       </c>
       <c r="J118" s="2" t="s">
+        <v>625</v>
+      </c>
+      <c r="K118" s="2" t="n">
+        <v>1375.0</v>
+      </c>
+      <c r="L118" s="2" t="s">
         <v>626</v>
       </c>
-      <c r="K118" s="2" t="n">
-        <v>1203.0</v>
-      </c>
-      <c r="L118" s="2" t="s">
-        <v>623</v>
-      </c>
       <c r="M118" s="2" t="n">
-        <v>218.0</v>
+        <v>367.0</v>
       </c>
       <c r="N118" s="2" t="s">
         <v>627</v>
@@ -19864,37 +19864,37 @@
         <v>629</v>
       </c>
       <c r="D119" s="2" t="n">
-        <v>693.0</v>
+        <v>767.0</v>
       </c>
       <c r="E119" s="2" t="s">
-        <v>628</v>
+        <v>630</v>
       </c>
       <c r="F119" s="2" t="n">
-        <v>170.0</v>
+        <v>208.0</v>
       </c>
       <c r="G119" s="2" t="n">
-        <v>9.0</v>
+        <v>73.0</v>
       </c>
       <c r="H119" s="2" t="s">
         <v>628</v>
       </c>
       <c r="I119" s="2" t="n">
-        <v>1503.0</v>
+        <v>1321.0</v>
       </c>
       <c r="J119" s="2" t="s">
-        <v>630</v>
+        <v>631</v>
       </c>
       <c r="K119" s="2" t="n">
-        <v>1103.0</v>
+        <v>1203.0</v>
       </c>
       <c r="L119" s="2" t="s">
         <v>628</v>
       </c>
       <c r="M119" s="2" t="n">
-        <v>562.0</v>
+        <v>218.0</v>
       </c>
       <c r="N119" s="2" t="s">
-        <v>631</v>
+        <v>632</v>
       </c>
     </row>
     <row r="120">
@@ -19902,40 +19902,40 @@
         <v>119.0</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>632</v>
+        <v>633</v>
       </c>
       <c r="C120" s="2" t="s">
+        <v>634</v>
+      </c>
+      <c r="D120" s="2" t="n">
+        <v>693.0</v>
+      </c>
+      <c r="E120" s="2" t="s">
         <v>633</v>
       </c>
-      <c r="D120" s="2" t="n">
-        <v>694.0</v>
-      </c>
-      <c r="E120" s="2" t="s">
-        <v>634</v>
-      </c>
       <c r="F120" s="2" t="n">
-        <v>238.0</v>
+        <v>170.0</v>
       </c>
       <c r="G120" s="2" t="n">
-        <v>65.0</v>
+        <v>9.0</v>
       </c>
       <c r="H120" s="2" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="I120" s="2" t="n">
-        <v>1482.0</v>
+        <v>1503.0</v>
       </c>
       <c r="J120" s="2" t="s">
         <v>635</v>
       </c>
       <c r="K120" s="2" t="n">
-        <v>1308.0</v>
+        <v>1103.0</v>
       </c>
       <c r="L120" s="2" t="s">
-        <v>632</v>
+        <v>633</v>
       </c>
       <c r="M120" s="2" t="n">
-        <v>60.0</v>
+        <v>562.0</v>
       </c>
       <c r="N120" s="2" t="s">
         <v>636</v>
@@ -19952,37 +19952,37 @@
         <v>638</v>
       </c>
       <c r="D121" s="2" t="n">
-        <v>706.0</v>
+        <v>694.0</v>
       </c>
       <c r="E121" s="2" t="s">
         <v>639</v>
       </c>
       <c r="F121" s="2" t="n">
-        <v>172.0</v>
+        <v>238.0</v>
       </c>
       <c r="G121" s="2" t="n">
-        <v>186.0</v>
+        <v>65.0</v>
       </c>
       <c r="H121" s="2" t="s">
+        <v>639</v>
+      </c>
+      <c r="I121" s="2" t="n">
+        <v>1482.0</v>
+      </c>
+      <c r="J121" s="2" t="s">
         <v>640</v>
       </c>
-      <c r="I121" s="2" t="n">
-        <v>1390.0</v>
-      </c>
-      <c r="J121" s="2" t="s">
+      <c r="K121" s="2" t="n">
+        <v>1308.0</v>
+      </c>
+      <c r="L121" s="2" t="s">
+        <v>637</v>
+      </c>
+      <c r="M121" s="2" t="n">
+        <v>60.0</v>
+      </c>
+      <c r="N121" s="2" t="s">
         <v>641</v>
-      </c>
-      <c r="K121" s="2" t="n">
-        <v>1203.0</v>
-      </c>
-      <c r="L121" s="2" t="s">
-        <v>640</v>
-      </c>
-      <c r="M121" s="2" t="n">
-        <v>436.0</v>
-      </c>
-      <c r="N121" s="2" t="s">
-        <v>642</v>
       </c>
     </row>
     <row r="122">
@@ -19990,43 +19990,43 @@
         <v>121.0</v>
       </c>
       <c r="B122" s="2" t="s">
+        <v>642</v>
+      </c>
+      <c r="C122" s="2" t="s">
         <v>643</v>
       </c>
-      <c r="C122" s="2" t="s">
+      <c r="D122" s="2" t="n">
+        <v>706.0</v>
+      </c>
+      <c r="E122" s="2" t="s">
         <v>644</v>
       </c>
-      <c r="D122" s="2" t="n">
-        <v>914.0</v>
-      </c>
-      <c r="E122" s="2" t="s">
+      <c r="F122" s="2" t="n">
+        <v>172.0</v>
+      </c>
+      <c r="G122" s="2" t="n">
+        <v>186.0</v>
+      </c>
+      <c r="H122" s="2" t="s">
         <v>645</v>
       </c>
-      <c r="F122" s="2" t="n">
-        <v>99.0</v>
-      </c>
-      <c r="G122" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="H122" s="2" t="s">
+      <c r="I122" s="2" t="n">
+        <v>1390.0</v>
+      </c>
+      <c r="J122" s="2" t="s">
         <v>646</v>
       </c>
-      <c r="I122" s="2" t="n">
-        <v>1574.0</v>
-      </c>
-      <c r="J122" s="2" t="s">
+      <c r="K122" s="2" t="n">
+        <v>1203.0</v>
+      </c>
+      <c r="L122" s="2" t="s">
+        <v>645</v>
+      </c>
+      <c r="M122" s="2" t="n">
+        <v>436.0</v>
+      </c>
+      <c r="N122" s="2" t="s">
         <v>647</v>
-      </c>
-      <c r="K122" s="2" t="n">
-        <v>1338.0</v>
-      </c>
-      <c r="L122" s="2" t="s">
-        <v>648</v>
-      </c>
-      <c r="M122" s="2" t="n">
-        <v>50.0</v>
-      </c>
-      <c r="N122" s="2" t="s">
-        <v>649</v>
       </c>
     </row>
     <row r="123">
@@ -20034,40 +20034,40 @@
         <v>122.0</v>
       </c>
       <c r="B123" s="2" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
       <c r="C123" s="2" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
       <c r="D123" s="2" t="n">
-        <v>758.0</v>
+        <v>914.0</v>
       </c>
       <c r="E123" s="2" t="s">
         <v>650</v>
       </c>
       <c r="F123" s="2" t="n">
-        <v>153.0</v>
+        <v>99.0</v>
       </c>
       <c r="G123" s="2" t="n">
-        <v>68.0</v>
+        <v>0.0</v>
       </c>
       <c r="H123" s="2" t="s">
+        <v>651</v>
+      </c>
+      <c r="I123" s="2" t="n">
+        <v>1574.0</v>
+      </c>
+      <c r="J123" s="2" t="s">
         <v>652</v>
       </c>
-      <c r="I123" s="2" t="n">
-        <v>1608.0</v>
-      </c>
-      <c r="J123" s="2" t="s">
+      <c r="K123" s="2" t="n">
+        <v>1338.0</v>
+      </c>
+      <c r="L123" s="2" t="s">
         <v>653</v>
       </c>
-      <c r="K123" s="2" t="n">
-        <v>1348.0</v>
-      </c>
-      <c r="L123" s="2" t="s">
-        <v>650</v>
-      </c>
       <c r="M123" s="2" t="n">
-        <v>148.0</v>
+        <v>50.0</v>
       </c>
       <c r="N123" s="2" t="s">
         <v>654</v>
@@ -20084,37 +20084,37 @@
         <v>656</v>
       </c>
       <c r="D124" s="2" t="n">
-        <v>656.0</v>
+        <v>758.0</v>
       </c>
       <c r="E124" s="2" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="F124" s="2" t="n">
-        <v>67.0</v>
+        <v>153.0</v>
       </c>
       <c r="G124" s="2" t="n">
-        <v>930.0</v>
+        <v>68.0</v>
       </c>
       <c r="H124" s="2" t="s">
         <v>657</v>
       </c>
       <c r="I124" s="2" t="n">
-        <v>1427.0</v>
+        <v>1608.0</v>
       </c>
       <c r="J124" s="2" t="s">
-        <v>657</v>
+        <v>658</v>
       </c>
       <c r="K124" s="2" t="n">
-        <v>1156.0</v>
+        <v>1348.0</v>
       </c>
       <c r="L124" s="2" t="s">
         <v>655</v>
       </c>
       <c r="M124" s="2" t="n">
-        <v>929.0</v>
+        <v>148.0</v>
       </c>
       <c r="N124" s="2" t="s">
-        <v>658</v>
+        <v>659</v>
       </c>
     </row>
     <row r="125">
@@ -20122,40 +20122,40 @@
         <v>124.0</v>
       </c>
       <c r="B125" s="2" t="s">
-        <v>659</v>
+        <v>660</v>
       </c>
       <c r="C125" s="2" t="s">
-        <v>660</v>
+        <v>661</v>
       </c>
       <c r="D125" s="2" t="n">
-        <v>772.0</v>
+        <v>656.0</v>
       </c>
       <c r="E125" s="2" t="s">
-        <v>661</v>
+        <v>662</v>
       </c>
       <c r="F125" s="2" t="n">
-        <v>196.0</v>
+        <v>67.0</v>
       </c>
       <c r="G125" s="2" t="n">
-        <v>40.0</v>
+        <v>930.0</v>
       </c>
       <c r="H125" s="2" t="s">
-        <v>661</v>
+        <v>662</v>
       </c>
       <c r="I125" s="2" t="n">
-        <v>1322.0</v>
+        <v>1427.0</v>
       </c>
       <c r="J125" s="2" t="s">
         <v>662</v>
       </c>
       <c r="K125" s="2" t="n">
-        <v>1236.0</v>
+        <v>1156.0</v>
       </c>
       <c r="L125" s="2" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="M125" s="2" t="n">
-        <v>179.0</v>
+        <v>929.0</v>
       </c>
       <c r="N125" s="2" t="s">
         <v>663</v>
@@ -20172,37 +20172,37 @@
         <v>665</v>
       </c>
       <c r="D126" s="2" t="n">
-        <v>778.0</v>
+        <v>772.0</v>
       </c>
       <c r="E126" s="2" t="s">
         <v>666</v>
       </c>
       <c r="F126" s="2" t="n">
-        <v>152.0</v>
+        <v>196.0</v>
       </c>
       <c r="G126" s="2" t="n">
-        <v>83.0</v>
+        <v>40.0</v>
       </c>
       <c r="H126" s="2" t="s">
-        <v>664</v>
+        <v>666</v>
       </c>
       <c r="I126" s="2" t="n">
-        <v>1352.0</v>
+        <v>1322.0</v>
       </c>
       <c r="J126" s="2" t="s">
         <v>667</v>
       </c>
       <c r="K126" s="2" t="n">
-        <v>1202.0</v>
+        <v>1236.0</v>
       </c>
       <c r="L126" s="2" t="s">
+        <v>666</v>
+      </c>
+      <c r="M126" s="2" t="n">
+        <v>179.0</v>
+      </c>
+      <c r="N126" s="2" t="s">
         <v>668</v>
-      </c>
-      <c r="M126" s="2" t="n">
-        <v>362.0</v>
-      </c>
-      <c r="N126" s="2" t="s">
-        <v>669</v>
       </c>
     </row>
     <row r="127">
@@ -20210,40 +20210,40 @@
         <v>126.0</v>
       </c>
       <c r="B127" s="2" t="s">
+        <v>669</v>
+      </c>
+      <c r="C127" s="2" t="s">
         <v>670</v>
       </c>
-      <c r="C127" s="2" t="s">
+      <c r="D127" s="2" t="n">
+        <v>778.0</v>
+      </c>
+      <c r="E127" s="2" t="s">
         <v>671</v>
       </c>
-      <c r="D127" s="2" t="n">
-        <v>935.0</v>
-      </c>
-      <c r="E127" s="2" t="s">
-        <v>672</v>
-      </c>
       <c r="F127" s="2" t="n">
-        <v>249.0</v>
+        <v>152.0</v>
       </c>
       <c r="G127" s="2" t="n">
-        <v>141.0</v>
+        <v>83.0</v>
       </c>
       <c r="H127" s="2" t="s">
-        <v>672</v>
+        <v>669</v>
       </c>
       <c r="I127" s="2" t="n">
-        <v>1490.0</v>
+        <v>1352.0</v>
       </c>
       <c r="J127" s="2" t="s">
         <v>672</v>
       </c>
       <c r="K127" s="2" t="n">
-        <v>0.0</v>
+        <v>1202.0</v>
       </c>
       <c r="L127" s="2" t="s">
         <v>673</v>
       </c>
       <c r="M127" s="2" t="n">
-        <v>284.0</v>
+        <v>362.0</v>
       </c>
       <c r="N127" s="2" t="s">
         <v>674</v>
@@ -24977,7 +24977,7 @@
         <v>59.0</v>
       </c>
       <c r="G235" s="2" t="n">
-        <v>348.0</v>
+        <v>349.0</v>
       </c>
       <c r="H235" s="2" t="s">
         <v>1233</v>
@@ -30873,7 +30873,7 @@
         <v>10.0</v>
       </c>
       <c r="G369" s="2" t="n">
-        <v>275.0</v>
+        <v>276.0</v>
       </c>
       <c r="H369" s="2" t="s">
         <v>1931</v>

</xml_diff>

<commit_message>
Add generated leaderboard data - 2024-07-02T20:12:14
</commit_message>
<xml_diff>
--- a/Leaderboards/CurrentCMRITLeaderboard2025.xlsx
+++ b/Leaderboards/CurrentCMRITLeaderboard2025.xlsx
@@ -83,7 +83,7 @@
     <t>deepak216</t>
   </si>
   <si>
-    <t>71.65</t>
+    <t>71.66</t>
   </si>
   <si>
     <t>21R01A0561</t>
@@ -506,7 +506,7 @@
     <t>22r05a0_520</t>
   </si>
   <si>
-    <t>51.7</t>
+    <t>51.71</t>
   </si>
   <si>
     <t>21R01A0557</t>
@@ -875,7 +875,7 @@
     <t>bhavani_2234</t>
   </si>
   <si>
-    <t>47.38</t>
+    <t>47.39</t>
   </si>
   <si>
     <t>21R01A0550</t>
@@ -1580,7 +1580,7 @@
     <t>vishnupriya508</t>
   </si>
   <si>
-    <t>43.36</t>
+    <t>43.37</t>
   </si>
   <si>
     <t>21R01A0441</t>
@@ -3659,6 +3659,27 @@
     <t>35.57</t>
   </si>
   <si>
+    <t>21R01A7257</t>
+  </si>
+  <si>
+    <t>Vaishnavi_017</t>
+  </si>
+  <si>
+    <t>21r01ax608</t>
+  </si>
+  <si>
+    <t>vaishnavisingireddy</t>
+  </si>
+  <si>
+    <t>vaishnavisingi</t>
+  </si>
+  <si>
+    <t>vaishnavisingir1</t>
+  </si>
+  <si>
+    <t>35.4</t>
+  </si>
+  <si>
     <t>21R01A7353</t>
   </si>
   <si>
@@ -3668,27 +3689,6 @@
     <t>hain21r01a7353</t>
   </si>
   <si>
-    <t>35.4</t>
-  </si>
-  <si>
-    <t>21R01A7257</t>
-  </si>
-  <si>
-    <t>Vaishnavi_017</t>
-  </si>
-  <si>
-    <t>21r01ax608</t>
-  </si>
-  <si>
-    <t>vaishnavisingireddy</t>
-  </si>
-  <si>
-    <t>vaishnavisingi</t>
-  </si>
-  <si>
-    <t>vaishnavisingir1</t>
-  </si>
-  <si>
     <t>21R01A66C3</t>
   </si>
   <si>
@@ -3749,6 +3749,24 @@
     <t>35.21</t>
   </si>
   <si>
+    <t>21R01A66C5</t>
+  </si>
+  <si>
+    <t>CMRIT25_21R01A66C5</t>
+  </si>
+  <si>
+    <t>21r01a66c5</t>
+  </si>
+  <si>
+    <t>T_DEVENDAR</t>
+  </si>
+  <si>
+    <t>devendar7987</t>
+  </si>
+  <si>
+    <t>35.19</t>
+  </si>
+  <si>
     <t>21R01A7307</t>
   </si>
   <si>
@@ -3764,24 +3782,6 @@
     <t>shashidhar07</t>
   </si>
   <si>
-    <t>35.19</t>
-  </si>
-  <si>
-    <t>21R01A66C5</t>
-  </si>
-  <si>
-    <t>CMRIT25_21R01A66C5</t>
-  </si>
-  <si>
-    <t>21r01a66c5</t>
-  </si>
-  <si>
-    <t>T_DEVENDAR</t>
-  </si>
-  <si>
-    <t>devendar7987</t>
-  </si>
-  <si>
     <t>21R01A05A1</t>
   </si>
   <si>
@@ -5798,6 +5798,24 @@
     <t>30.84</t>
   </si>
   <si>
+    <t>21R01A66A6</t>
+  </si>
+  <si>
+    <t>CMRIT25_21R01A66A6</t>
+  </si>
+  <si>
+    <t>21r01ac1bc</t>
+  </si>
+  <si>
+    <t>yousufansari</t>
+  </si>
+  <si>
+    <t>21r01a66a6</t>
+  </si>
+  <si>
+    <t>30.81</t>
+  </si>
+  <si>
     <t>21R01A05B2</t>
   </si>
   <si>
@@ -5810,24 +5828,6 @@
     <t>cmr_5b2</t>
   </si>
   <si>
-    <t>30.81</t>
-  </si>
-  <si>
-    <t>21R01A66A6</t>
-  </si>
-  <si>
-    <t>CMRIT25_21R01A66A6</t>
-  </si>
-  <si>
-    <t>21r01ac1bc</t>
-  </si>
-  <si>
-    <t>yousufansari</t>
-  </si>
-  <si>
-    <t>21r01a66a6</t>
-  </si>
-  <si>
     <t>21R01A6703</t>
   </si>
   <si>
@@ -7493,7 +7493,7 @@
     <t>21R01A0541cmritonline.ac.in</t>
   </si>
   <si>
-    <t>25.44</t>
+    <t>25.52</t>
   </si>
   <si>
     <t>21R01A6756</t>
@@ -14787,7 +14787,7 @@
         <v>722.0</v>
       </c>
       <c r="G3" s="2" t="n">
-        <v>608.0</v>
+        <v>614.0</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>21</v>
@@ -14963,7 +14963,7 @@
         <v>525.0</v>
       </c>
       <c r="G7" s="2" t="n">
-        <v>693.0</v>
+        <v>695.0</v>
       </c>
       <c r="H7" s="2" t="s">
         <v>41</v>
@@ -15931,7 +15931,7 @@
         <v>449.0</v>
       </c>
       <c r="G29" s="2" t="n">
-        <v>134.0</v>
+        <v>136.0</v>
       </c>
       <c r="H29" s="2" t="s">
         <v>155</v>
@@ -15975,7 +15975,7 @@
         <v>383.0</v>
       </c>
       <c r="G30" s="2" t="n">
-        <v>251.0</v>
+        <v>255.0</v>
       </c>
       <c r="H30" s="2" t="s">
         <v>159</v>
@@ -16987,7 +16987,7 @@
         <v>298.0</v>
       </c>
       <c r="G53" s="2" t="n">
-        <v>490.0</v>
+        <v>492.0</v>
       </c>
       <c r="H53" s="2" t="s">
         <v>286</v>
@@ -18659,7 +18659,7 @@
         <v>259.0</v>
       </c>
       <c r="G91" s="2" t="n">
-        <v>173.0</v>
+        <v>175.0</v>
       </c>
       <c r="H91" s="2" t="s">
         <v>487</v>
@@ -18923,7 +18923,7 @@
         <v>225.0</v>
       </c>
       <c r="G97" s="2" t="n">
-        <v>133.0</v>
+        <v>135.0</v>
       </c>
       <c r="H97" s="2" t="s">
         <v>520</v>
@@ -24810,37 +24810,37 @@
         <v>1216</v>
       </c>
       <c r="D231" s="2" t="n">
-        <v>881.0</v>
+        <v>692.0</v>
       </c>
       <c r="E231" s="2" t="s">
-        <v>1216</v>
+        <v>1217</v>
       </c>
       <c r="F231" s="2" t="n">
-        <v>0.0</v>
+        <v>10.0</v>
       </c>
       <c r="G231" s="2" t="n">
-        <v>131.0</v>
+        <v>141.0</v>
       </c>
       <c r="H231" s="2" t="s">
-        <v>1215</v>
+        <v>1218</v>
       </c>
       <c r="I231" s="2" t="n">
-        <v>1396.0</v>
+        <v>1472.0</v>
       </c>
       <c r="J231" s="2" t="s">
-        <v>1217</v>
+        <v>1219</v>
       </c>
       <c r="K231" s="2" t="n">
-        <v>1092.0</v>
+        <v>1409.0</v>
       </c>
       <c r="L231" s="2" t="s">
-        <v>1216</v>
+        <v>1220</v>
       </c>
       <c r="M231" s="2" t="n">
-        <v>280.0</v>
+        <v>434.0</v>
       </c>
       <c r="N231" s="2" t="s">
-        <v>1218</v>
+        <v>1221</v>
       </c>
     </row>
     <row r="232">
@@ -24848,43 +24848,43 @@
         <v>231.0</v>
       </c>
       <c r="B232" s="2" t="s">
-        <v>1219</v>
+        <v>1222</v>
       </c>
       <c r="C232" s="2" t="s">
-        <v>1220</v>
+        <v>1223</v>
       </c>
       <c r="D232" s="2" t="n">
-        <v>692.0</v>
+        <v>881.0</v>
       </c>
       <c r="E232" s="2" t="s">
-        <v>1221</v>
+        <v>1223</v>
       </c>
       <c r="F232" s="2" t="n">
-        <v>10.0</v>
+        <v>0.0</v>
       </c>
       <c r="G232" s="2" t="n">
-        <v>138.0</v>
+        <v>131.0</v>
       </c>
       <c r="H232" s="2" t="s">
         <v>1222</v>
       </c>
       <c r="I232" s="2" t="n">
-        <v>1472.0</v>
+        <v>1396.0</v>
       </c>
       <c r="J232" s="2" t="s">
+        <v>1224</v>
+      </c>
+      <c r="K232" s="2" t="n">
+        <v>1092.0</v>
+      </c>
+      <c r="L232" s="2" t="s">
         <v>1223</v>
       </c>
-      <c r="K232" s="2" t="n">
-        <v>1409.0</v>
-      </c>
-      <c r="L232" s="2" t="s">
-        <v>1224</v>
-      </c>
       <c r="M232" s="2" t="n">
-        <v>434.0</v>
+        <v>280.0</v>
       </c>
       <c r="N232" s="2" t="s">
-        <v>1218</v>
+        <v>1221</v>
       </c>
     </row>
     <row r="233">
@@ -24928,7 +24928,7 @@
         <v>514.0</v>
       </c>
       <c r="N233" s="2" t="s">
-        <v>1218</v>
+        <v>1221</v>
       </c>
     </row>
     <row r="234">
@@ -25039,7 +25039,7 @@
         <v>59.0</v>
       </c>
       <c r="G236" s="2" t="n">
-        <v>356.0</v>
+        <v>360.0</v>
       </c>
       <c r="H236" s="2" t="s">
         <v>1243</v>
@@ -25074,34 +25074,34 @@
         <v>1246</v>
       </c>
       <c r="D237" s="2" t="n">
-        <v>742.0</v>
+        <v>745.0</v>
       </c>
       <c r="E237" s="2" t="s">
         <v>1247</v>
       </c>
       <c r="F237" s="2" t="n">
-        <v>60.0</v>
+        <v>79.0</v>
       </c>
       <c r="G237" s="2" t="n">
-        <v>21.0</v>
+        <v>460.0</v>
       </c>
       <c r="H237" s="2" t="s">
         <v>1248</v>
       </c>
       <c r="I237" s="2" t="n">
-        <v>1552.0</v>
+        <v>1420.0</v>
       </c>
       <c r="J237" s="2" t="s">
         <v>1249</v>
       </c>
       <c r="K237" s="2" t="n">
-        <v>1361.0</v>
+        <v>895.0</v>
       </c>
       <c r="L237" s="2" t="s">
-        <v>1246</v>
+        <v>1245</v>
       </c>
       <c r="M237" s="2" t="n">
-        <v>43.0</v>
+        <v>303.0</v>
       </c>
       <c r="N237" s="2" t="s">
         <v>1250</v>
@@ -25118,34 +25118,34 @@
         <v>1252</v>
       </c>
       <c r="D238" s="2" t="n">
-        <v>745.0</v>
+        <v>742.0</v>
       </c>
       <c r="E238" s="2" t="s">
         <v>1253</v>
       </c>
       <c r="F238" s="2" t="n">
-        <v>79.0</v>
+        <v>60.0</v>
       </c>
       <c r="G238" s="2" t="n">
-        <v>454.0</v>
+        <v>21.0</v>
       </c>
       <c r="H238" s="2" t="s">
         <v>1254</v>
       </c>
       <c r="I238" s="2" t="n">
-        <v>1420.0</v>
+        <v>1552.0</v>
       </c>
       <c r="J238" s="2" t="s">
         <v>1255</v>
       </c>
       <c r="K238" s="2" t="n">
-        <v>895.0</v>
+        <v>1361.0</v>
       </c>
       <c r="L238" s="2" t="s">
-        <v>1251</v>
+        <v>1252</v>
       </c>
       <c r="M238" s="2" t="n">
-        <v>303.0</v>
+        <v>43.0</v>
       </c>
       <c r="N238" s="2" t="s">
         <v>1250</v>
@@ -30838,37 +30838,37 @@
         <v>1929</v>
       </c>
       <c r="D368" s="2" t="n">
-        <v>850.0</v>
+        <v>594.0</v>
       </c>
       <c r="E368" s="2" t="s">
         <v>1930</v>
       </c>
       <c r="F368" s="2" t="n">
-        <v>100.0</v>
+        <v>10.0</v>
       </c>
       <c r="G368" s="2" t="n">
-        <v>0.0</v>
+        <v>284.0</v>
       </c>
       <c r="H368" s="2" t="s">
         <v>1931</v>
       </c>
       <c r="I368" s="2" t="n">
-        <v>1657.0</v>
+        <v>1412.0</v>
       </c>
       <c r="J368" s="2" t="s">
         <v>1931</v>
       </c>
       <c r="K368" s="2" t="n">
-        <v>0.0</v>
+        <v>1179.0</v>
       </c>
       <c r="L368" s="2" t="s">
-        <v>1928</v>
+        <v>1932</v>
       </c>
       <c r="M368" s="2" t="n">
-        <v>0.0</v>
+        <v>313.0</v>
       </c>
       <c r="N368" s="2" t="s">
-        <v>1932</v>
+        <v>1933</v>
       </c>
     </row>
     <row r="369">
@@ -30876,43 +30876,43 @@
         <v>368.0</v>
       </c>
       <c r="B369" s="2" t="s">
+        <v>1934</v>
+      </c>
+      <c r="C369" s="2" t="s">
+        <v>1935</v>
+      </c>
+      <c r="D369" s="2" t="n">
+        <v>850.0</v>
+      </c>
+      <c r="E369" s="2" t="s">
+        <v>1936</v>
+      </c>
+      <c r="F369" s="2" t="n">
+        <v>100.0</v>
+      </c>
+      <c r="G369" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H369" s="2" t="s">
+        <v>1937</v>
+      </c>
+      <c r="I369" s="2" t="n">
+        <v>1657.0</v>
+      </c>
+      <c r="J369" s="2" t="s">
+        <v>1937</v>
+      </c>
+      <c r="K369" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L369" s="2" t="s">
+        <v>1934</v>
+      </c>
+      <c r="M369" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="N369" s="2" t="s">
         <v>1933</v>
-      </c>
-      <c r="C369" s="2" t="s">
-        <v>1934</v>
-      </c>
-      <c r="D369" s="2" t="n">
-        <v>594.0</v>
-      </c>
-      <c r="E369" s="2" t="s">
-        <v>1935</v>
-      </c>
-      <c r="F369" s="2" t="n">
-        <v>10.0</v>
-      </c>
-      <c r="G369" s="2" t="n">
-        <v>282.0</v>
-      </c>
-      <c r="H369" s="2" t="s">
-        <v>1936</v>
-      </c>
-      <c r="I369" s="2" t="n">
-        <v>1412.0</v>
-      </c>
-      <c r="J369" s="2" t="s">
-        <v>1936</v>
-      </c>
-      <c r="K369" s="2" t="n">
-        <v>1179.0</v>
-      </c>
-      <c r="L369" s="2" t="s">
-        <v>1937</v>
-      </c>
-      <c r="M369" s="2" t="n">
-        <v>313.0</v>
-      </c>
-      <c r="N369" s="2" t="s">
-        <v>1932</v>
       </c>
     </row>
     <row r="370">
@@ -34719,7 +34719,7 @@
         <v>110.0</v>
       </c>
       <c r="G456" s="2" t="n">
-        <v>58.0</v>
+        <v>60.0</v>
       </c>
       <c r="H456" s="2" t="s">
         <v>2375</v>
@@ -35687,7 +35687,7 @@
         <v>319.0</v>
       </c>
       <c r="G478" s="2" t="n">
-        <v>166.0</v>
+        <v>216.0</v>
       </c>
       <c r="H478" s="2" t="s">
         <v>2490</v>

</xml_diff>

<commit_message>
Add generated leaderboard data - 2024-07-16T20:11:30
</commit_message>
<xml_diff>
--- a/Leaderboards/CurrentCMRITLeaderboard2025.xlsx
+++ b/Leaderboards/CurrentCMRITLeaderboard2025.xlsx
@@ -149,7 +149,7 @@
     <t>prashanth50</t>
   </si>
   <si>
-    <t>61.46</t>
+    <t>61.47</t>
   </si>
   <si>
     <t>21R01A0426</t>
@@ -467,7 +467,7 @@
     <t>22r05a0_520</t>
   </si>
   <si>
-    <t>53.42</t>
+    <t>53.43</t>
   </si>
   <si>
     <t>21R01A0513</t>
@@ -524,7 +524,7 @@
     <t>meg_21r01a0531</t>
   </si>
   <si>
-    <t>52.55</t>
+    <t>52.56</t>
   </si>
   <si>
     <t>21R01A66C7</t>
@@ -803,7 +803,7 @@
     <t>k_prakashraj17</t>
   </si>
   <si>
-    <t>49.15</t>
+    <t>49.17</t>
   </si>
   <si>
     <t>22R05A0505</t>
@@ -1304,7 +1304,7 @@
     <t>cmrit_21r01a05</t>
   </si>
   <si>
-    <t>45.42</t>
+    <t>45.43</t>
   </si>
   <si>
     <t>21R01A0510</t>
@@ -2567,7 +2567,7 @@
     <t>21r01a66c41</t>
   </si>
   <si>
-    <t>38.96</t>
+    <t>38.97</t>
   </si>
   <si>
     <t>21R01A66B0</t>
@@ -3257,7 +3257,7 @@
     <t>21r01a6676</t>
   </si>
   <si>
-    <t>36.95</t>
+    <t>36.96</t>
   </si>
   <si>
     <t>21R01A66A3</t>
@@ -3716,7 +3716,7 @@
     <t>meghana_85</t>
   </si>
   <si>
-    <t>35.76</t>
+    <t>35.77</t>
   </si>
   <si>
     <t>21R01A67J1</t>
@@ -4259,6 +4259,24 @@
     <t>21r01a6657</t>
   </si>
   <si>
+    <t>21R01A6685</t>
+  </si>
+  <si>
+    <t>CMRIT25_21R01A6685</t>
+  </si>
+  <si>
+    <t>koushik_04</t>
+  </si>
+  <si>
+    <t>koushik2003</t>
+  </si>
+  <si>
+    <t>saikoushik04</t>
+  </si>
+  <si>
+    <t>34.69</t>
+  </si>
+  <si>
     <t>21R01A6795</t>
   </si>
   <si>
@@ -4286,24 +4304,6 @@
     <t>nithin421</t>
   </si>
   <si>
-    <t>21R01A6685</t>
-  </si>
-  <si>
-    <t>CMRIT25_21R01A6685</t>
-  </si>
-  <si>
-    <t>koushik_04</t>
-  </si>
-  <si>
-    <t>koushik2003</t>
-  </si>
-  <si>
-    <t>saikoushik04</t>
-  </si>
-  <si>
-    <t>34.66</t>
-  </si>
-  <si>
     <t>21R01A0421</t>
   </si>
   <si>
@@ -4478,9 +4478,6 @@
     <t>pavan138</t>
   </si>
   <si>
-    <t>34.38</t>
-  </si>
-  <si>
     <t>21R01A66D2</t>
   </si>
   <si>
@@ -4589,6 +4586,18 @@
     <t>34.19</t>
   </si>
   <si>
+    <t>21R01A6641</t>
+  </si>
+  <si>
+    <t>21r01a6641</t>
+  </si>
+  <si>
+    <t>ashritha92</t>
+  </si>
+  <si>
+    <t>34.16</t>
+  </si>
+  <si>
     <t>21R01A0574</t>
   </si>
   <si>
@@ -4895,18 +4904,6 @@
     <t>33.4</t>
   </si>
   <si>
-    <t>21R01A6641</t>
-  </si>
-  <si>
-    <t>21r01a6641</t>
-  </si>
-  <si>
-    <t>ashritha92</t>
-  </si>
-  <si>
-    <t>33.36</t>
-  </si>
-  <si>
     <t>21R01A6699</t>
   </si>
   <si>
@@ -5003,6 +5000,21 @@
     <t>33.25</t>
   </si>
   <si>
+    <t>21R01A6644</t>
+  </si>
+  <si>
+    <t>CMRIT25_21R01A6644</t>
+  </si>
+  <si>
+    <t>21r01a6644</t>
+  </si>
+  <si>
+    <t>s21r01a6644</t>
+  </si>
+  <si>
+    <t>33.18</t>
+  </si>
+  <si>
     <t>21R01A66D9</t>
   </si>
   <si>
@@ -5019,18 +5031,6 @@
   </si>
   <si>
     <t>33.17</t>
-  </si>
-  <si>
-    <t>21R01A6644</t>
-  </si>
-  <si>
-    <t>CMRIT25_21R01A6644</t>
-  </si>
-  <si>
-    <t>21r01a6644</t>
-  </si>
-  <si>
-    <t>s21r01a6644</t>
   </si>
   <si>
     <t>21R01A0485</t>
@@ -14972,7 +14972,7 @@
         <v>525.0</v>
       </c>
       <c r="G7" s="2" t="n">
-        <v>695.0</v>
+        <v>697.0</v>
       </c>
       <c r="H7" s="2" t="s">
         <v>41</v>
@@ -15852,7 +15852,7 @@
         <v>423.0</v>
       </c>
       <c r="G27" s="2" t="n">
-        <v>285.0</v>
+        <v>289.0</v>
       </c>
       <c r="H27" s="2" t="s">
         <v>146</v>
@@ -16028,7 +16028,7 @@
         <v>557.0</v>
       </c>
       <c r="G31" s="2" t="n">
-        <v>256.0</v>
+        <v>258.0</v>
       </c>
       <c r="H31" s="2" t="s">
         <v>166</v>
@@ -16776,7 +16776,7 @@
         <v>401.0</v>
       </c>
       <c r="G48" s="2" t="n">
-        <v>786.0</v>
+        <v>794.0</v>
       </c>
       <c r="H48" s="2" t="s">
         <v>261</v>
@@ -17040,7 +17040,7 @@
         <v>318.0</v>
       </c>
       <c r="G54" s="2" t="n">
-        <v>544.0</v>
+        <v>550.0</v>
       </c>
       <c r="H54" s="2" t="s">
         <v>292</v>
@@ -18140,7 +18140,7 @@
         <v>299.0</v>
       </c>
       <c r="G79" s="2" t="n">
-        <v>175.0</v>
+        <v>179.0</v>
       </c>
       <c r="H79" s="2" t="s">
         <v>426</v>
@@ -21704,7 +21704,7 @@
         <v>120.0</v>
       </c>
       <c r="G160" s="2" t="n">
-        <v>197.0</v>
+        <v>205.0</v>
       </c>
       <c r="H160" s="2" t="s">
         <v>848</v>
@@ -23640,7 +23640,7 @@
         <v>40.0</v>
       </c>
       <c r="G204" s="2" t="n">
-        <v>118.0</v>
+        <v>126.0</v>
       </c>
       <c r="H204" s="2" t="s">
         <v>1076</v>
@@ -24960,7 +24960,7 @@
         <v>39.0</v>
       </c>
       <c r="G234" s="2" t="n">
-        <v>205.0</v>
+        <v>213.0</v>
       </c>
       <c r="H234" s="2" t="s">
         <v>1232</v>
@@ -25444,7 +25444,7 @@
         <v>79.0</v>
       </c>
       <c r="G245" s="2" t="n">
-        <v>539.0</v>
+        <v>541.0</v>
       </c>
       <c r="H245" s="2" t="s">
         <v>1290</v>
@@ -25708,7 +25708,7 @@
         <v>59.0</v>
       </c>
       <c r="G251" s="2" t="n">
-        <v>384.0</v>
+        <v>386.0</v>
       </c>
       <c r="H251" s="2" t="s">
         <v>1323</v>
@@ -26491,37 +26491,37 @@
         <v>1416</v>
       </c>
       <c r="D269" s="2" t="n">
-        <v>785.0</v>
+        <v>779.0</v>
       </c>
       <c r="E269" s="2" t="s">
         <v>1417</v>
       </c>
       <c r="F269" s="2" t="n">
-        <v>69.0</v>
+        <v>50.0</v>
       </c>
       <c r="G269" s="2" t="n">
-        <v>2.0</v>
+        <v>61.0</v>
       </c>
       <c r="H269" s="2" t="s">
-        <v>1417</v>
+        <v>1418</v>
       </c>
       <c r="I269" s="2" t="n">
-        <v>1357.0</v>
+        <v>1402.0</v>
       </c>
       <c r="J269" s="2" t="s">
-        <v>1417</v>
+        <v>1419</v>
       </c>
       <c r="K269" s="2" t="n">
-        <v>1238.0</v>
+        <v>1256.0</v>
       </c>
       <c r="L269" s="2" t="s">
-        <v>1418</v>
+        <v>1415</v>
       </c>
       <c r="M269" s="2" t="n">
-        <v>50.0</v>
+        <v>103.0</v>
       </c>
       <c r="N269" s="2" t="s">
-        <v>1419</v>
+        <v>1420</v>
       </c>
     </row>
     <row r="270">
@@ -26529,43 +26529,43 @@
         <v>269.0</v>
       </c>
       <c r="B270" s="2" t="s">
-        <v>1420</v>
+        <v>1421</v>
       </c>
       <c r="C270" s="2" t="s">
-        <v>1421</v>
+        <v>1422</v>
       </c>
       <c r="D270" s="2" t="n">
-        <v>765.0</v>
+        <v>785.0</v>
       </c>
       <c r="E270" s="2" t="s">
-        <v>1422</v>
+        <v>1423</v>
       </c>
       <c r="F270" s="2" t="n">
-        <v>67.0</v>
+        <v>69.0</v>
       </c>
       <c r="G270" s="2" t="n">
-        <v>4.0</v>
+        <v>2.0</v>
       </c>
       <c r="H270" s="2" t="s">
-        <v>1420</v>
+        <v>1423</v>
       </c>
       <c r="I270" s="2" t="n">
-        <v>1452.0</v>
+        <v>1357.0</v>
       </c>
       <c r="J270" s="2" t="s">
         <v>1423</v>
       </c>
       <c r="K270" s="2" t="n">
-        <v>1218.0</v>
+        <v>1238.0</v>
       </c>
       <c r="L270" s="2" t="s">
-        <v>1422</v>
+        <v>1424</v>
       </c>
       <c r="M270" s="2" t="n">
-        <v>64.0</v>
+        <v>50.0</v>
       </c>
       <c r="N270" s="2" t="s">
-        <v>1419</v>
+        <v>1425</v>
       </c>
     </row>
     <row r="271">
@@ -26573,43 +26573,43 @@
         <v>270.0</v>
       </c>
       <c r="B271" s="2" t="s">
-        <v>1424</v>
+        <v>1426</v>
       </c>
       <c r="C271" s="2" t="s">
+        <v>1427</v>
+      </c>
+      <c r="D271" s="2" t="n">
+        <v>765.0</v>
+      </c>
+      <c r="E271" s="2" t="s">
+        <v>1428</v>
+      </c>
+      <c r="F271" s="2" t="n">
+        <v>67.0</v>
+      </c>
+      <c r="G271" s="2" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="H271" s="2" t="s">
+        <v>1426</v>
+      </c>
+      <c r="I271" s="2" t="n">
+        <v>1452.0</v>
+      </c>
+      <c r="J271" s="2" t="s">
+        <v>1429</v>
+      </c>
+      <c r="K271" s="2" t="n">
+        <v>1218.0</v>
+      </c>
+      <c r="L271" s="2" t="s">
+        <v>1428</v>
+      </c>
+      <c r="M271" s="2" t="n">
+        <v>64.0</v>
+      </c>
+      <c r="N271" s="2" t="s">
         <v>1425</v>
-      </c>
-      <c r="D271" s="2" t="n">
-        <v>779.0</v>
-      </c>
-      <c r="E271" s="2" t="s">
-        <v>1426</v>
-      </c>
-      <c r="F271" s="2" t="n">
-        <v>50.0</v>
-      </c>
-      <c r="G271" s="2" t="n">
-        <v>41.0</v>
-      </c>
-      <c r="H271" s="2" t="s">
-        <v>1427</v>
-      </c>
-      <c r="I271" s="2" t="n">
-        <v>1402.0</v>
-      </c>
-      <c r="J271" s="2" t="s">
-        <v>1428</v>
-      </c>
-      <c r="K271" s="2" t="n">
-        <v>1256.0</v>
-      </c>
-      <c r="L271" s="2" t="s">
-        <v>1424</v>
-      </c>
-      <c r="M271" s="2" t="n">
-        <v>103.0</v>
-      </c>
-      <c r="N271" s="2" t="s">
-        <v>1429</v>
       </c>
     </row>
     <row r="272">
@@ -27072,7 +27072,7 @@
         <v>49.0</v>
       </c>
       <c r="G282" s="2" t="n">
-        <v>353.0</v>
+        <v>359.0</v>
       </c>
       <c r="H282" s="2" t="s">
         <v>1484</v>
@@ -27093,7 +27093,7 @@
         <v>332.0</v>
       </c>
       <c r="N282" s="2" t="s">
-        <v>1488</v>
+        <v>1483</v>
       </c>
     </row>
     <row r="283">
@@ -27101,16 +27101,16 @@
         <v>282.0</v>
       </c>
       <c r="B283" s="2" t="s">
+        <v>1488</v>
+      </c>
+      <c r="C283" s="2" t="s">
         <v>1489</v>
-      </c>
-      <c r="C283" s="2" t="s">
-        <v>1490</v>
       </c>
       <c r="D283" s="2" t="n">
         <v>857.0</v>
       </c>
       <c r="E283" s="2" t="s">
-        <v>1491</v>
+        <v>1490</v>
       </c>
       <c r="F283" s="2" t="n">
         <v>0.0</v>
@@ -27119,25 +27119,25 @@
         <v>8.0</v>
       </c>
       <c r="H283" s="2" t="s">
-        <v>1492</v>
+        <v>1491</v>
       </c>
       <c r="I283" s="2" t="n">
         <v>1538.0</v>
       </c>
       <c r="J283" s="2" t="s">
-        <v>1492</v>
+        <v>1491</v>
       </c>
       <c r="K283" s="2" t="n">
         <v>1180.0</v>
       </c>
       <c r="L283" s="2" t="s">
-        <v>1491</v>
+        <v>1490</v>
       </c>
       <c r="M283" s="2" t="n">
         <v>75.0</v>
       </c>
       <c r="N283" s="2" t="s">
-        <v>1493</v>
+        <v>1492</v>
       </c>
     </row>
     <row r="284">
@@ -27145,16 +27145,16 @@
         <v>283.0</v>
       </c>
       <c r="B284" s="2" t="s">
+        <v>1493</v>
+      </c>
+      <c r="C284" s="2" t="s">
         <v>1494</v>
-      </c>
-      <c r="C284" s="2" t="s">
-        <v>1495</v>
       </c>
       <c r="D284" s="2" t="n">
         <v>677.0</v>
       </c>
       <c r="E284" s="2" t="s">
-        <v>1496</v>
+        <v>1495</v>
       </c>
       <c r="F284" s="2" t="n">
         <v>30.0</v>
@@ -27163,25 +27163,25 @@
         <v>108.0</v>
       </c>
       <c r="H284" s="2" t="s">
-        <v>1495</v>
+        <v>1494</v>
       </c>
       <c r="I284" s="2" t="n">
         <v>1353.0</v>
       </c>
       <c r="J284" s="2" t="s">
-        <v>1497</v>
+        <v>1496</v>
       </c>
       <c r="K284" s="2" t="n">
         <v>1016.0</v>
       </c>
       <c r="L284" s="2" t="s">
-        <v>1495</v>
+        <v>1494</v>
       </c>
       <c r="M284" s="2" t="n">
         <v>628.0</v>
       </c>
       <c r="N284" s="2" t="s">
-        <v>1498</v>
+        <v>1497</v>
       </c>
     </row>
     <row r="285">
@@ -27189,16 +27189,16 @@
         <v>284.0</v>
       </c>
       <c r="B285" s="2" t="s">
+        <v>1498</v>
+      </c>
+      <c r="C285" s="2" t="s">
         <v>1499</v>
-      </c>
-      <c r="C285" s="2" t="s">
-        <v>1500</v>
       </c>
       <c r="D285" s="2" t="n">
         <v>852.0</v>
       </c>
       <c r="E285" s="2" t="s">
-        <v>1501</v>
+        <v>1500</v>
       </c>
       <c r="F285" s="2" t="n">
         <v>0.0</v>
@@ -27207,25 +27207,25 @@
         <v>0.0</v>
       </c>
       <c r="H285" s="2" t="s">
-        <v>1499</v>
+        <v>1498</v>
       </c>
       <c r="I285" s="2" t="n">
         <v>1641.0</v>
       </c>
       <c r="J285" s="2" t="s">
-        <v>1502</v>
+        <v>1501</v>
       </c>
       <c r="K285" s="2" t="n">
         <v>1146.0</v>
       </c>
       <c r="L285" s="2" t="s">
-        <v>1499</v>
+        <v>1498</v>
       </c>
       <c r="M285" s="2" t="n">
         <v>45.0</v>
       </c>
       <c r="N285" s="2" t="s">
-        <v>1503</v>
+        <v>1502</v>
       </c>
     </row>
     <row r="286">
@@ -27233,16 +27233,16 @@
         <v>285.0</v>
       </c>
       <c r="B286" s="2" t="s">
+        <v>1503</v>
+      </c>
+      <c r="C286" s="2" t="s">
         <v>1504</v>
-      </c>
-      <c r="C286" s="2" t="s">
-        <v>1505</v>
       </c>
       <c r="D286" s="2" t="n">
         <v>758.0</v>
       </c>
       <c r="E286" s="2" t="s">
-        <v>1506</v>
+        <v>1505</v>
       </c>
       <c r="F286" s="2" t="n">
         <v>70.0</v>
@@ -27251,25 +27251,25 @@
         <v>0.0</v>
       </c>
       <c r="H286" s="2" t="s">
-        <v>1507</v>
+        <v>1506</v>
       </c>
       <c r="I286" s="2" t="n">
         <v>1419.0</v>
       </c>
       <c r="J286" s="2" t="s">
-        <v>1508</v>
+        <v>1507</v>
       </c>
       <c r="K286" s="2" t="n">
         <v>1246.0</v>
       </c>
       <c r="L286" s="2" t="s">
-        <v>1509</v>
+        <v>1508</v>
       </c>
       <c r="M286" s="2" t="n">
         <v>15.0</v>
       </c>
       <c r="N286" s="2" t="s">
-        <v>1510</v>
+        <v>1509</v>
       </c>
     </row>
     <row r="287">
@@ -27277,43 +27277,43 @@
         <v>286.0</v>
       </c>
       <c r="B287" s="2" t="s">
+        <v>1510</v>
+      </c>
+      <c r="C287" s="2" t="s">
         <v>1511</v>
-      </c>
-      <c r="C287" s="2" t="s">
-        <v>1512</v>
       </c>
       <c r="D287" s="2" t="n">
         <v>827.0</v>
       </c>
       <c r="E287" s="2" t="s">
-        <v>1513</v>
+        <v>1512</v>
       </c>
       <c r="F287" s="2" t="n">
         <v>20.0</v>
       </c>
       <c r="G287" s="2" t="n">
-        <v>21.0</v>
+        <v>23.0</v>
       </c>
       <c r="H287" s="2" t="s">
-        <v>1513</v>
+        <v>1512</v>
       </c>
       <c r="I287" s="2" t="n">
         <v>1356.0</v>
       </c>
       <c r="J287" s="2" t="s">
-        <v>1514</v>
+        <v>1513</v>
       </c>
       <c r="K287" s="2" t="n">
         <v>1197.0</v>
       </c>
       <c r="L287" s="2" t="s">
-        <v>1513</v>
+        <v>1512</v>
       </c>
       <c r="M287" s="2" t="n">
         <v>147.0</v>
       </c>
       <c r="N287" s="2" t="s">
-        <v>1515</v>
+        <v>1514</v>
       </c>
     </row>
     <row r="288">
@@ -27321,16 +27321,16 @@
         <v>287.0</v>
       </c>
       <c r="B288" s="2" t="s">
+        <v>1515</v>
+      </c>
+      <c r="C288" s="2" t="s">
         <v>1516</v>
-      </c>
-      <c r="C288" s="2" t="s">
-        <v>1517</v>
       </c>
       <c r="D288" s="2" t="n">
         <v>713.0</v>
       </c>
       <c r="E288" s="2" t="s">
-        <v>1518</v>
+        <v>1517</v>
       </c>
       <c r="F288" s="2" t="n">
         <v>30.0</v>
@@ -27339,25 +27339,25 @@
         <v>1027.0</v>
       </c>
       <c r="H288" s="2" t="s">
-        <v>1518</v>
+        <v>1517</v>
       </c>
       <c r="I288" s="2" t="n">
         <v>1573.0</v>
       </c>
       <c r="J288" s="2" t="s">
-        <v>1519</v>
+        <v>1518</v>
       </c>
       <c r="K288" s="2" t="n">
         <v>1223.0</v>
       </c>
       <c r="L288" s="2" t="s">
-        <v>1518</v>
+        <v>1517</v>
       </c>
       <c r="M288" s="2" t="n">
         <v>45.0</v>
       </c>
       <c r="N288" s="2" t="s">
-        <v>1515</v>
+        <v>1514</v>
       </c>
     </row>
     <row r="289">
@@ -27365,16 +27365,16 @@
         <v>288.0</v>
       </c>
       <c r="B289" s="2" t="s">
+        <v>1519</v>
+      </c>
+      <c r="C289" s="2" t="s">
         <v>1520</v>
-      </c>
-      <c r="C289" s="2" t="s">
-        <v>1521</v>
       </c>
       <c r="D289" s="2" t="n">
         <v>792.0</v>
       </c>
       <c r="E289" s="2" t="s">
-        <v>1522</v>
+        <v>1521</v>
       </c>
       <c r="F289" s="2" t="n">
         <v>30.0</v>
@@ -27383,25 +27383,25 @@
         <v>143.0</v>
       </c>
       <c r="H289" s="2" t="s">
-        <v>1520</v>
+        <v>1519</v>
       </c>
       <c r="I289" s="2" t="n">
         <v>1392.0</v>
       </c>
       <c r="J289" s="2" t="s">
-        <v>1523</v>
+        <v>1522</v>
       </c>
       <c r="K289" s="2" t="n">
         <v>1073.0</v>
       </c>
       <c r="L289" s="2" t="s">
-        <v>1522</v>
+        <v>1521</v>
       </c>
       <c r="M289" s="2" t="n">
         <v>235.0</v>
       </c>
       <c r="N289" s="2" t="s">
-        <v>1524</v>
+        <v>1523</v>
       </c>
     </row>
     <row r="290">
@@ -27409,43 +27409,43 @@
         <v>289.0</v>
       </c>
       <c r="B290" s="2" t="s">
+        <v>1524</v>
+      </c>
+      <c r="C290" s="2" t="s">
+        <v>1524</v>
+      </c>
+      <c r="D290" s="2" t="n">
+        <v>624.0</v>
+      </c>
+      <c r="E290" s="2" t="s">
+        <v>1524</v>
+      </c>
+      <c r="F290" s="2" t="n">
+        <v>49.0</v>
+      </c>
+      <c r="G290" s="2" t="n">
+        <v>282.0</v>
+      </c>
+      <c r="H290" s="2" t="s">
         <v>1525</v>
       </c>
-      <c r="C290" s="2" t="s">
+      <c r="I290" s="2" t="n">
+        <v>1464.0</v>
+      </c>
+      <c r="J290" s="2" t="s">
         <v>1526</v>
       </c>
-      <c r="D290" s="2" t="n">
-        <v>711.0</v>
-      </c>
-      <c r="E290" s="2" t="s">
-        <v>1525</v>
-      </c>
-      <c r="F290" s="2" t="n">
-        <v>138.0</v>
-      </c>
-      <c r="G290" s="2" t="n">
-        <v>83.0</v>
-      </c>
-      <c r="H290" s="2" t="s">
-        <v>1526</v>
-      </c>
-      <c r="I290" s="2" t="n">
-        <v>1277.0</v>
-      </c>
-      <c r="J290" s="2" t="s">
+      <c r="K290" s="2" t="n">
+        <v>1058.0</v>
+      </c>
+      <c r="L290" s="2" t="s">
+        <v>1524</v>
+      </c>
+      <c r="M290" s="2" t="n">
+        <v>518.0</v>
+      </c>
+      <c r="N290" s="2" t="s">
         <v>1527</v>
-      </c>
-      <c r="K290" s="2" t="n">
-        <v>986.0</v>
-      </c>
-      <c r="L290" s="2" t="s">
-        <v>1525</v>
-      </c>
-      <c r="M290" s="2" t="n">
-        <v>70.0</v>
-      </c>
-      <c r="N290" s="2" t="s">
-        <v>1528</v>
       </c>
     </row>
     <row r="291">
@@ -27453,43 +27453,43 @@
         <v>290.0</v>
       </c>
       <c r="B291" s="2" t="s">
+        <v>1528</v>
+      </c>
+      <c r="C291" s="2" t="s">
         <v>1529</v>
       </c>
-      <c r="C291" s="2" t="s">
+      <c r="D291" s="2" t="n">
+        <v>711.0</v>
+      </c>
+      <c r="E291" s="2" t="s">
+        <v>1528</v>
+      </c>
+      <c r="F291" s="2" t="n">
+        <v>138.0</v>
+      </c>
+      <c r="G291" s="2" t="n">
+        <v>83.0</v>
+      </c>
+      <c r="H291" s="2" t="s">
+        <v>1529</v>
+      </c>
+      <c r="I291" s="2" t="n">
+        <v>1277.0</v>
+      </c>
+      <c r="J291" s="2" t="s">
         <v>1530</v>
       </c>
-      <c r="D291" s="2" t="n">
-        <v>826.0</v>
-      </c>
-      <c r="E291" s="2" t="s">
+      <c r="K291" s="2" t="n">
+        <v>986.0</v>
+      </c>
+      <c r="L291" s="2" t="s">
+        <v>1528</v>
+      </c>
+      <c r="M291" s="2" t="n">
+        <v>70.0</v>
+      </c>
+      <c r="N291" s="2" t="s">
         <v>1531</v>
-      </c>
-      <c r="F291" s="2" t="n">
-        <v>30.0</v>
-      </c>
-      <c r="G291" s="2" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="H291" s="2" t="s">
-        <v>1532</v>
-      </c>
-      <c r="I291" s="2" t="n">
-        <v>1639.0</v>
-      </c>
-      <c r="J291" s="2" t="s">
-        <v>1531</v>
-      </c>
-      <c r="K291" s="2" t="n">
-        <v>1066.0</v>
-      </c>
-      <c r="L291" s="2" t="s">
-        <v>1532</v>
-      </c>
-      <c r="M291" s="2" t="n">
-        <v>5.0</v>
-      </c>
-      <c r="N291" s="2" t="s">
-        <v>1528</v>
       </c>
     </row>
     <row r="292">
@@ -27497,43 +27497,43 @@
         <v>291.0</v>
       </c>
       <c r="B292" s="2" t="s">
+        <v>1532</v>
+      </c>
+      <c r="C292" s="2" t="s">
         <v>1533</v>
       </c>
-      <c r="C292" s="2" t="s">
+      <c r="D292" s="2" t="n">
+        <v>826.0</v>
+      </c>
+      <c r="E292" s="2" t="s">
         <v>1534</v>
       </c>
-      <c r="D292" s="2" t="n">
-        <v>805.0</v>
-      </c>
-      <c r="E292" s="2" t="s">
+      <c r="F292" s="2" t="n">
+        <v>30.0</v>
+      </c>
+      <c r="G292" s="2" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="H292" s="2" t="s">
         <v>1535</v>
       </c>
-      <c r="F292" s="2" t="n">
-        <v>10.0</v>
-      </c>
-      <c r="G292" s="2" t="n">
-        <v>106.0</v>
-      </c>
-      <c r="H292" s="2" t="s">
-        <v>1536</v>
-      </c>
       <c r="I292" s="2" t="n">
-        <v>1375.0</v>
+        <v>1639.0</v>
       </c>
       <c r="J292" s="2" t="s">
-        <v>1537</v>
+        <v>1534</v>
       </c>
       <c r="K292" s="2" t="n">
-        <v>1053.0</v>
+        <v>1066.0</v>
       </c>
       <c r="L292" s="2" t="s">
-        <v>1536</v>
+        <v>1535</v>
       </c>
       <c r="M292" s="2" t="n">
-        <v>319.0</v>
+        <v>5.0</v>
       </c>
       <c r="N292" s="2" t="s">
-        <v>1538</v>
+        <v>1531</v>
       </c>
     </row>
     <row r="293">
@@ -27541,43 +27541,43 @@
         <v>292.0</v>
       </c>
       <c r="B293" s="2" t="s">
+        <v>1536</v>
+      </c>
+      <c r="C293" s="2" t="s">
+        <v>1537</v>
+      </c>
+      <c r="D293" s="2" t="n">
+        <v>805.0</v>
+      </c>
+      <c r="E293" s="2" t="s">
+        <v>1538</v>
+      </c>
+      <c r="F293" s="2" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="G293" s="2" t="n">
+        <v>106.0</v>
+      </c>
+      <c r="H293" s="2" t="s">
         <v>1539</v>
       </c>
-      <c r="C293" s="2" t="s">
+      <c r="I293" s="2" t="n">
+        <v>1375.0</v>
+      </c>
+      <c r="J293" s="2" t="s">
         <v>1540</v>
       </c>
-      <c r="D293" s="2" t="n">
-        <v>719.0</v>
-      </c>
-      <c r="E293" s="2" t="s">
+      <c r="K293" s="2" t="n">
+        <v>1053.0</v>
+      </c>
+      <c r="L293" s="2" t="s">
+        <v>1539</v>
+      </c>
+      <c r="M293" s="2" t="n">
+        <v>319.0</v>
+      </c>
+      <c r="N293" s="2" t="s">
         <v>1541</v>
-      </c>
-      <c r="F293" s="2" t="n">
-        <v>100.0</v>
-      </c>
-      <c r="G293" s="2" t="n">
-        <v>10.0</v>
-      </c>
-      <c r="H293" s="2" t="s">
-        <v>1541</v>
-      </c>
-      <c r="I293" s="2" t="n">
-        <v>1331.0</v>
-      </c>
-      <c r="J293" s="2" t="s">
-        <v>1542</v>
-      </c>
-      <c r="K293" s="2" t="n">
-        <v>1194.0</v>
-      </c>
-      <c r="L293" s="2" t="s">
-        <v>1541</v>
-      </c>
-      <c r="M293" s="2" t="n">
-        <v>45.0</v>
-      </c>
-      <c r="N293" s="2" t="s">
-        <v>1543</v>
       </c>
     </row>
     <row r="294">
@@ -27585,43 +27585,43 @@
         <v>293.0</v>
       </c>
       <c r="B294" s="2" t="s">
+        <v>1542</v>
+      </c>
+      <c r="C294" s="2" t="s">
+        <v>1543</v>
+      </c>
+      <c r="D294" s="2" t="n">
+        <v>719.0</v>
+      </c>
+      <c r="E294" s="2" t="s">
         <v>1544</v>
       </c>
-      <c r="C294" s="2" t="s">
+      <c r="F294" s="2" t="n">
+        <v>100.0</v>
+      </c>
+      <c r="G294" s="2" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="H294" s="2" t="s">
+        <v>1544</v>
+      </c>
+      <c r="I294" s="2" t="n">
+        <v>1331.0</v>
+      </c>
+      <c r="J294" s="2" t="s">
         <v>1545</v>
       </c>
-      <c r="D294" s="2" t="n">
-        <v>787.0</v>
-      </c>
-      <c r="E294" s="2" t="s">
+      <c r="K294" s="2" t="n">
+        <v>1194.0</v>
+      </c>
+      <c r="L294" s="2" t="s">
+        <v>1544</v>
+      </c>
+      <c r="M294" s="2" t="n">
+        <v>45.0</v>
+      </c>
+      <c r="N294" s="2" t="s">
         <v>1546</v>
-      </c>
-      <c r="F294" s="2" t="n">
-        <v>10.0</v>
-      </c>
-      <c r="G294" s="2" t="n">
-        <v>82.0</v>
-      </c>
-      <c r="H294" s="2" t="s">
-        <v>1547</v>
-      </c>
-      <c r="I294" s="2" t="n">
-        <v>1507.0</v>
-      </c>
-      <c r="J294" s="2" t="s">
-        <v>1548</v>
-      </c>
-      <c r="K294" s="2" t="n">
-        <v>1149.0</v>
-      </c>
-      <c r="L294" s="2" t="s">
-        <v>1546</v>
-      </c>
-      <c r="M294" s="2" t="n">
-        <v>201.0</v>
-      </c>
-      <c r="N294" s="2" t="s">
-        <v>1549</v>
       </c>
     </row>
     <row r="295">
@@ -27629,43 +27629,43 @@
         <v>294.0</v>
       </c>
       <c r="B295" s="2" t="s">
+        <v>1547</v>
+      </c>
+      <c r="C295" s="2" t="s">
+        <v>1548</v>
+      </c>
+      <c r="D295" s="2" t="n">
+        <v>787.0</v>
+      </c>
+      <c r="E295" s="2" t="s">
+        <v>1549</v>
+      </c>
+      <c r="F295" s="2" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="G295" s="2" t="n">
+        <v>82.0</v>
+      </c>
+      <c r="H295" s="2" t="s">
         <v>1550</v>
       </c>
-      <c r="C295" s="2" t="s">
+      <c r="I295" s="2" t="n">
+        <v>1507.0</v>
+      </c>
+      <c r="J295" s="2" t="s">
         <v>1551</v>
       </c>
-      <c r="D295" s="2" t="n">
-        <v>761.0</v>
-      </c>
-      <c r="E295" s="2" t="s">
+      <c r="K295" s="2" t="n">
+        <v>1149.0</v>
+      </c>
+      <c r="L295" s="2" t="s">
+        <v>1549</v>
+      </c>
+      <c r="M295" s="2" t="n">
+        <v>201.0</v>
+      </c>
+      <c r="N295" s="2" t="s">
         <v>1552</v>
-      </c>
-      <c r="F295" s="2" t="n">
-        <v>20.0</v>
-      </c>
-      <c r="G295" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="H295" s="2" t="s">
-        <v>1552</v>
-      </c>
-      <c r="I295" s="2" t="n">
-        <v>1492.0</v>
-      </c>
-      <c r="J295" s="2" t="s">
-        <v>1553</v>
-      </c>
-      <c r="K295" s="2" t="n">
-        <v>1270.0</v>
-      </c>
-      <c r="L295" s="2" t="s">
-        <v>1550</v>
-      </c>
-      <c r="M295" s="2" t="n">
-        <v>154.0</v>
-      </c>
-      <c r="N295" s="2" t="s">
-        <v>1549</v>
       </c>
     </row>
     <row r="296">
@@ -27673,43 +27673,43 @@
         <v>295.0</v>
       </c>
       <c r="B296" s="2" t="s">
+        <v>1553</v>
+      </c>
+      <c r="C296" s="2" t="s">
         <v>1554</v>
       </c>
-      <c r="C296" s="2" t="s">
+      <c r="D296" s="2" t="n">
+        <v>761.0</v>
+      </c>
+      <c r="E296" s="2" t="s">
         <v>1555</v>
       </c>
-      <c r="D296" s="2" t="n">
-        <v>706.0</v>
-      </c>
-      <c r="E296" s="2" t="s">
+      <c r="F296" s="2" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="G296" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H296" s="2" t="s">
+        <v>1555</v>
+      </c>
+      <c r="I296" s="2" t="n">
+        <v>1492.0</v>
+      </c>
+      <c r="J296" s="2" t="s">
         <v>1556</v>
       </c>
-      <c r="F296" s="2" t="n">
-        <v>8.0</v>
-      </c>
-      <c r="G296" s="2" t="n">
-        <v>305.0</v>
-      </c>
-      <c r="H296" s="2" t="s">
-        <v>1557</v>
-      </c>
-      <c r="I296" s="2" t="n">
-        <v>1321.0</v>
-      </c>
-      <c r="J296" s="2" t="s">
-        <v>1557</v>
-      </c>
       <c r="K296" s="2" t="n">
-        <v>1367.0</v>
+        <v>1270.0</v>
       </c>
       <c r="L296" s="2" t="s">
-        <v>1556</v>
+        <v>1553</v>
       </c>
       <c r="M296" s="2" t="n">
-        <v>326.0</v>
+        <v>154.0</v>
       </c>
       <c r="N296" s="2" t="s">
-        <v>1558</v>
+        <v>1552</v>
       </c>
     </row>
     <row r="297">
@@ -27717,43 +27717,43 @@
         <v>296.0</v>
       </c>
       <c r="B297" s="2" t="s">
+        <v>1557</v>
+      </c>
+      <c r="C297" s="2" t="s">
+        <v>1558</v>
+      </c>
+      <c r="D297" s="2" t="n">
+        <v>706.0</v>
+      </c>
+      <c r="E297" s="2" t="s">
         <v>1559</v>
       </c>
-      <c r="C297" s="2" t="s">
+      <c r="F297" s="2" t="n">
+        <v>8.0</v>
+      </c>
+      <c r="G297" s="2" t="n">
+        <v>305.0</v>
+      </c>
+      <c r="H297" s="2" t="s">
         <v>1560</v>
       </c>
-      <c r="D297" s="2" t="n">
-        <v>764.0</v>
-      </c>
-      <c r="E297" s="2" t="s">
+      <c r="I297" s="2" t="n">
+        <v>1321.0</v>
+      </c>
+      <c r="J297" s="2" t="s">
+        <v>1560</v>
+      </c>
+      <c r="K297" s="2" t="n">
+        <v>1367.0</v>
+      </c>
+      <c r="L297" s="2" t="s">
+        <v>1559</v>
+      </c>
+      <c r="M297" s="2" t="n">
+        <v>326.0</v>
+      </c>
+      <c r="N297" s="2" t="s">
         <v>1561</v>
-      </c>
-      <c r="F297" s="2" t="n">
-        <v>49.0</v>
-      </c>
-      <c r="G297" s="2" t="n">
-        <v>29.0</v>
-      </c>
-      <c r="H297" s="2" t="s">
-        <v>1562</v>
-      </c>
-      <c r="I297" s="2" t="n">
-        <v>1324.0</v>
-      </c>
-      <c r="J297" s="2" t="s">
-        <v>1563</v>
-      </c>
-      <c r="K297" s="2" t="n">
-        <v>1294.0</v>
-      </c>
-      <c r="L297" s="2" t="s">
-        <v>1562</v>
-      </c>
-      <c r="M297" s="2" t="n">
-        <v>80.0</v>
-      </c>
-      <c r="N297" s="2" t="s">
-        <v>1564</v>
       </c>
     </row>
     <row r="298">
@@ -27761,43 +27761,43 @@
         <v>297.0</v>
       </c>
       <c r="B298" s="2" t="s">
+        <v>1562</v>
+      </c>
+      <c r="C298" s="2" t="s">
+        <v>1563</v>
+      </c>
+      <c r="D298" s="2" t="n">
+        <v>764.0</v>
+      </c>
+      <c r="E298" s="2" t="s">
+        <v>1564</v>
+      </c>
+      <c r="F298" s="2" t="n">
+        <v>49.0</v>
+      </c>
+      <c r="G298" s="2" t="n">
+        <v>29.0</v>
+      </c>
+      <c r="H298" s="2" t="s">
         <v>1565</v>
       </c>
-      <c r="C298" s="2" t="s">
+      <c r="I298" s="2" t="n">
+        <v>1324.0</v>
+      </c>
+      <c r="J298" s="2" t="s">
         <v>1566</v>
       </c>
-      <c r="D298" s="2" t="n">
-        <v>695.0</v>
-      </c>
-      <c r="E298" s="2" t="s">
+      <c r="K298" s="2" t="n">
+        <v>1294.0</v>
+      </c>
+      <c r="L298" s="2" t="s">
+        <v>1565</v>
+      </c>
+      <c r="M298" s="2" t="n">
+        <v>80.0</v>
+      </c>
+      <c r="N298" s="2" t="s">
         <v>1567</v>
-      </c>
-      <c r="F298" s="2" t="n">
-        <v>38.0</v>
-      </c>
-      <c r="G298" s="2" t="n">
-        <v>108.0</v>
-      </c>
-      <c r="H298" s="2" t="s">
-        <v>1568</v>
-      </c>
-      <c r="I298" s="2" t="n">
-        <v>1508.0</v>
-      </c>
-      <c r="J298" s="2" t="s">
-        <v>1569</v>
-      </c>
-      <c r="K298" s="2" t="n">
-        <v>1145.0</v>
-      </c>
-      <c r="L298" s="2" t="s">
-        <v>1568</v>
-      </c>
-      <c r="M298" s="2" t="n">
-        <v>287.0</v>
-      </c>
-      <c r="N298" s="2" t="s">
-        <v>1570</v>
       </c>
     </row>
     <row r="299">
@@ -27805,43 +27805,43 @@
         <v>298.0</v>
       </c>
       <c r="B299" s="2" t="s">
+        <v>1568</v>
+      </c>
+      <c r="C299" s="2" t="s">
+        <v>1569</v>
+      </c>
+      <c r="D299" s="2" t="n">
+        <v>695.0</v>
+      </c>
+      <c r="E299" s="2" t="s">
+        <v>1570</v>
+      </c>
+      <c r="F299" s="2" t="n">
+        <v>38.0</v>
+      </c>
+      <c r="G299" s="2" t="n">
+        <v>108.0</v>
+      </c>
+      <c r="H299" s="2" t="s">
         <v>1571</v>
       </c>
-      <c r="C299" s="2" t="s">
+      <c r="I299" s="2" t="n">
+        <v>1508.0</v>
+      </c>
+      <c r="J299" s="2" t="s">
         <v>1572</v>
       </c>
-      <c r="D299" s="2" t="n">
-        <v>768.0</v>
-      </c>
-      <c r="E299" s="2" t="s">
+      <c r="K299" s="2" t="n">
+        <v>1145.0</v>
+      </c>
+      <c r="L299" s="2" t="s">
+        <v>1571</v>
+      </c>
+      <c r="M299" s="2" t="n">
+        <v>287.0</v>
+      </c>
+      <c r="N299" s="2" t="s">
         <v>1573</v>
-      </c>
-      <c r="F299" s="2" t="n">
-        <v>30.0</v>
-      </c>
-      <c r="G299" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="H299" s="2" t="s">
-        <v>1573</v>
-      </c>
-      <c r="I299" s="2" t="n">
-        <v>1437.0</v>
-      </c>
-      <c r="J299" s="2" t="s">
-        <v>1574</v>
-      </c>
-      <c r="K299" s="2" t="n">
-        <v>1201.0</v>
-      </c>
-      <c r="L299" s="2" t="s">
-        <v>1573</v>
-      </c>
-      <c r="M299" s="2" t="n">
-        <v>150.0</v>
-      </c>
-      <c r="N299" s="2" t="s">
-        <v>1575</v>
       </c>
     </row>
     <row r="300">
@@ -27849,43 +27849,43 @@
         <v>299.0</v>
       </c>
       <c r="B300" s="2" t="s">
+        <v>1574</v>
+      </c>
+      <c r="C300" s="2" t="s">
+        <v>1575</v>
+      </c>
+      <c r="D300" s="2" t="n">
+        <v>768.0</v>
+      </c>
+      <c r="E300" s="2" t="s">
         <v>1576</v>
       </c>
-      <c r="C300" s="2" t="s">
+      <c r="F300" s="2" t="n">
+        <v>30.0</v>
+      </c>
+      <c r="G300" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H300" s="2" t="s">
+        <v>1576</v>
+      </c>
+      <c r="I300" s="2" t="n">
+        <v>1437.0</v>
+      </c>
+      <c r="J300" s="2" t="s">
         <v>1577</v>
       </c>
-      <c r="D300" s="2" t="n">
-        <v>968.0</v>
-      </c>
-      <c r="E300" s="2" t="s">
+      <c r="K300" s="2" t="n">
+        <v>1201.0</v>
+      </c>
+      <c r="L300" s="2" t="s">
+        <v>1576</v>
+      </c>
+      <c r="M300" s="2" t="n">
+        <v>150.0</v>
+      </c>
+      <c r="N300" s="2" t="s">
         <v>1578</v>
-      </c>
-      <c r="F300" s="2" t="n">
-        <v>113.0</v>
-      </c>
-      <c r="G300" s="2" t="n">
-        <v>23.0</v>
-      </c>
-      <c r="H300" s="2" t="s">
-        <v>1578</v>
-      </c>
-      <c r="I300" s="2" t="n">
-        <v>1591.0</v>
-      </c>
-      <c r="J300" s="2" t="s">
-        <v>1579</v>
-      </c>
-      <c r="K300" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="L300" s="2" t="s">
-        <v>1578</v>
-      </c>
-      <c r="M300" s="2" t="n">
-        <v>32.0</v>
-      </c>
-      <c r="N300" s="2" t="s">
-        <v>1580</v>
       </c>
     </row>
     <row r="301">
@@ -27893,43 +27893,43 @@
         <v>300.0</v>
       </c>
       <c r="B301" s="2" t="s">
+        <v>1579</v>
+      </c>
+      <c r="C301" s="2" t="s">
+        <v>1580</v>
+      </c>
+      <c r="D301" s="2" t="n">
+        <v>968.0</v>
+      </c>
+      <c r="E301" s="2" t="s">
         <v>1581</v>
       </c>
-      <c r="C301" s="2" t="s">
+      <c r="F301" s="2" t="n">
+        <v>113.0</v>
+      </c>
+      <c r="G301" s="2" t="n">
+        <v>23.0</v>
+      </c>
+      <c r="H301" s="2" t="s">
+        <v>1581</v>
+      </c>
+      <c r="I301" s="2" t="n">
+        <v>1591.0</v>
+      </c>
+      <c r="J301" s="2" t="s">
         <v>1582</v>
       </c>
-      <c r="D301" s="2" t="n">
-        <v>757.0</v>
-      </c>
-      <c r="E301" s="2" t="s">
+      <c r="K301" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L301" s="2" t="s">
+        <v>1581</v>
+      </c>
+      <c r="M301" s="2" t="n">
+        <v>32.0</v>
+      </c>
+      <c r="N301" s="2" t="s">
         <v>1583</v>
-      </c>
-      <c r="F301" s="2" t="n">
-        <v>48.0</v>
-      </c>
-      <c r="G301" s="2" t="n">
-        <v>61.0</v>
-      </c>
-      <c r="H301" s="2" t="s">
-        <v>1582</v>
-      </c>
-      <c r="I301" s="2" t="n">
-        <v>1283.0</v>
-      </c>
-      <c r="J301" s="2" t="s">
-        <v>1584</v>
-      </c>
-      <c r="K301" s="2" t="n">
-        <v>1053.0</v>
-      </c>
-      <c r="L301" s="2" t="s">
-        <v>1582</v>
-      </c>
-      <c r="M301" s="2" t="n">
-        <v>290.0</v>
-      </c>
-      <c r="N301" s="2" t="s">
-        <v>1580</v>
       </c>
     </row>
     <row r="302">
@@ -27937,43 +27937,43 @@
         <v>301.0</v>
       </c>
       <c r="B302" s="2" t="s">
+        <v>1584</v>
+      </c>
+      <c r="C302" s="2" t="s">
         <v>1585</v>
       </c>
-      <c r="C302" s="2" t="s">
+      <c r="D302" s="2" t="n">
+        <v>757.0</v>
+      </c>
+      <c r="E302" s="2" t="s">
         <v>1586</v>
       </c>
-      <c r="D302" s="2" t="n">
-        <v>758.0</v>
-      </c>
-      <c r="E302" s="2" t="s">
+      <c r="F302" s="2" t="n">
+        <v>48.0</v>
+      </c>
+      <c r="G302" s="2" t="n">
+        <v>61.0</v>
+      </c>
+      <c r="H302" s="2" t="s">
+        <v>1585</v>
+      </c>
+      <c r="I302" s="2" t="n">
+        <v>1283.0</v>
+      </c>
+      <c r="J302" s="2" t="s">
         <v>1587</v>
       </c>
-      <c r="F302" s="2" t="n">
-        <v>40.0</v>
-      </c>
-      <c r="G302" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="H302" s="2" t="s">
-        <v>1588</v>
-      </c>
-      <c r="I302" s="2" t="n">
-        <v>1468.0</v>
-      </c>
-      <c r="J302" s="2" t="s">
-        <v>1588</v>
-      </c>
       <c r="K302" s="2" t="n">
-        <v>1256.0</v>
+        <v>1053.0</v>
       </c>
       <c r="L302" s="2" t="s">
-        <v>1589</v>
+        <v>1585</v>
       </c>
       <c r="M302" s="2" t="n">
-        <v>50.0</v>
+        <v>290.0</v>
       </c>
       <c r="N302" s="2" t="s">
-        <v>1590</v>
+        <v>1583</v>
       </c>
     </row>
     <row r="303">
@@ -27981,43 +27981,43 @@
         <v>302.0</v>
       </c>
       <c r="B303" s="2" t="s">
+        <v>1588</v>
+      </c>
+      <c r="C303" s="2" t="s">
+        <v>1589</v>
+      </c>
+      <c r="D303" s="2" t="n">
+        <v>758.0</v>
+      </c>
+      <c r="E303" s="2" t="s">
+        <v>1590</v>
+      </c>
+      <c r="F303" s="2" t="n">
+        <v>40.0</v>
+      </c>
+      <c r="G303" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H303" s="2" t="s">
         <v>1591</v>
       </c>
-      <c r="C303" s="2" t="s">
+      <c r="I303" s="2" t="n">
+        <v>1468.0</v>
+      </c>
+      <c r="J303" s="2" t="s">
+        <v>1591</v>
+      </c>
+      <c r="K303" s="2" t="n">
+        <v>1256.0</v>
+      </c>
+      <c r="L303" s="2" t="s">
         <v>1592</v>
       </c>
-      <c r="D303" s="2" t="n">
-        <v>636.0</v>
-      </c>
-      <c r="E303" s="2" t="s">
+      <c r="M303" s="2" t="n">
+        <v>50.0</v>
+      </c>
+      <c r="N303" s="2" t="s">
         <v>1593</v>
-      </c>
-      <c r="F303" s="2" t="n">
-        <v>69.0</v>
-      </c>
-      <c r="G303" s="2" t="n">
-        <v>181.0</v>
-      </c>
-      <c r="H303" s="2" t="s">
-        <v>1592</v>
-      </c>
-      <c r="I303" s="2" t="n">
-        <v>1499.0</v>
-      </c>
-      <c r="J303" s="2" t="s">
-        <v>1594</v>
-      </c>
-      <c r="K303" s="2" t="n">
-        <v>1174.0</v>
-      </c>
-      <c r="L303" s="2" t="s">
-        <v>1591</v>
-      </c>
-      <c r="M303" s="2" t="n">
-        <v>223.0</v>
-      </c>
-      <c r="N303" s="2" t="s">
-        <v>1595</v>
       </c>
     </row>
     <row r="304">
@@ -28025,43 +28025,43 @@
         <v>303.0</v>
       </c>
       <c r="B304" s="2" t="s">
+        <v>1594</v>
+      </c>
+      <c r="C304" s="2" t="s">
+        <v>1595</v>
+      </c>
+      <c r="D304" s="2" t="n">
+        <v>636.0</v>
+      </c>
+      <c r="E304" s="2" t="s">
         <v>1596</v>
       </c>
-      <c r="C304" s="2" t="s">
+      <c r="F304" s="2" t="n">
+        <v>69.0</v>
+      </c>
+      <c r="G304" s="2" t="n">
+        <v>181.0</v>
+      </c>
+      <c r="H304" s="2" t="s">
+        <v>1595</v>
+      </c>
+      <c r="I304" s="2" t="n">
+        <v>1499.0</v>
+      </c>
+      <c r="J304" s="2" t="s">
         <v>1597</v>
-      </c>
-      <c r="D304" s="2" t="n">
-        <v>756.0</v>
-      </c>
-      <c r="E304" s="2" t="s">
-        <v>1598</v>
-      </c>
-      <c r="F304" s="2" t="n">
-        <v>58.0</v>
-      </c>
-      <c r="G304" s="2" t="n">
-        <v>38.0</v>
-      </c>
-      <c r="H304" s="2" t="s">
-        <v>1598</v>
-      </c>
-      <c r="I304" s="2" t="n">
-        <v>1422.0</v>
-      </c>
-      <c r="J304" s="2" t="s">
-        <v>1598</v>
       </c>
       <c r="K304" s="2" t="n">
         <v>1174.0</v>
       </c>
       <c r="L304" s="2" t="s">
-        <v>1599</v>
+        <v>1594</v>
       </c>
       <c r="M304" s="2" t="n">
-        <v>38.0</v>
+        <v>223.0</v>
       </c>
       <c r="N304" s="2" t="s">
-        <v>1600</v>
+        <v>1598</v>
       </c>
     </row>
     <row r="305">
@@ -28069,43 +28069,43 @@
         <v>304.0</v>
       </c>
       <c r="B305" s="2" t="s">
+        <v>1599</v>
+      </c>
+      <c r="C305" s="2" t="s">
+        <v>1600</v>
+      </c>
+      <c r="D305" s="2" t="n">
+        <v>756.0</v>
+      </c>
+      <c r="E305" s="2" t="s">
         <v>1601</v>
       </c>
-      <c r="C305" s="2" t="s">
+      <c r="F305" s="2" t="n">
+        <v>58.0</v>
+      </c>
+      <c r="G305" s="2" t="n">
+        <v>38.0</v>
+      </c>
+      <c r="H305" s="2" t="s">
+        <v>1601</v>
+      </c>
+      <c r="I305" s="2" t="n">
+        <v>1422.0</v>
+      </c>
+      <c r="J305" s="2" t="s">
+        <v>1601</v>
+      </c>
+      <c r="K305" s="2" t="n">
+        <v>1174.0</v>
+      </c>
+      <c r="L305" s="2" t="s">
         <v>1602</v>
       </c>
-      <c r="D305" s="2" t="n">
-        <v>1051.0</v>
-      </c>
-      <c r="E305" s="2" t="s">
+      <c r="M305" s="2" t="n">
+        <v>38.0</v>
+      </c>
+      <c r="N305" s="2" t="s">
         <v>1603</v>
-      </c>
-      <c r="F305" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="G305" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="H305" s="2" t="s">
-        <v>1603</v>
-      </c>
-      <c r="I305" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="J305" s="2" t="s">
-        <v>1604</v>
-      </c>
-      <c r="K305" s="2" t="n">
-        <v>1510.0</v>
-      </c>
-      <c r="L305" s="2" t="s">
-        <v>1605</v>
-      </c>
-      <c r="M305" s="2" t="n">
-        <v>227.0</v>
-      </c>
-      <c r="N305" s="2" t="s">
-        <v>1606</v>
       </c>
     </row>
     <row r="306">
@@ -28113,43 +28113,43 @@
         <v>305.0</v>
       </c>
       <c r="B306" s="2" t="s">
+        <v>1604</v>
+      </c>
+      <c r="C306" s="2" t="s">
+        <v>1605</v>
+      </c>
+      <c r="D306" s="2" t="n">
+        <v>1051.0</v>
+      </c>
+      <c r="E306" s="2" t="s">
+        <v>1606</v>
+      </c>
+      <c r="F306" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G306" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H306" s="2" t="s">
+        <v>1606</v>
+      </c>
+      <c r="I306" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="J306" s="2" t="s">
         <v>1607</v>
       </c>
-      <c r="C306" s="2" t="s">
+      <c r="K306" s="2" t="n">
+        <v>1510.0</v>
+      </c>
+      <c r="L306" s="2" t="s">
         <v>1608</v>
       </c>
-      <c r="D306" s="2" t="n">
-        <v>586.0</v>
-      </c>
-      <c r="E306" s="2" t="s">
+      <c r="M306" s="2" t="n">
+        <v>227.0</v>
+      </c>
+      <c r="N306" s="2" t="s">
         <v>1609</v>
-      </c>
-      <c r="F306" s="2" t="n">
-        <v>140.0</v>
-      </c>
-      <c r="G306" s="2" t="n">
-        <v>490.0</v>
-      </c>
-      <c r="H306" s="2" t="s">
-        <v>1607</v>
-      </c>
-      <c r="I306" s="2" t="n">
-        <v>1473.0</v>
-      </c>
-      <c r="J306" s="2" t="s">
-        <v>1610</v>
-      </c>
-      <c r="K306" s="2" t="n">
-        <v>969.0</v>
-      </c>
-      <c r="L306" s="2" t="s">
-        <v>1609</v>
-      </c>
-      <c r="M306" s="2" t="n">
-        <v>119.0</v>
-      </c>
-      <c r="N306" s="2" t="s">
-        <v>1611</v>
       </c>
     </row>
     <row r="307">
@@ -28157,43 +28157,43 @@
         <v>306.0</v>
       </c>
       <c r="B307" s="2" t="s">
-        <v>1612</v>
+        <v>1610</v>
       </c>
       <c r="C307" s="2" t="s">
-        <v>1613</v>
+        <v>1611</v>
       </c>
       <c r="D307" s="2" t="n">
-        <v>734.0</v>
+        <v>586.0</v>
       </c>
       <c r="E307" s="2" t="s">
         <v>1612</v>
       </c>
       <c r="F307" s="2" t="n">
-        <v>30.0</v>
+        <v>140.0</v>
       </c>
       <c r="G307" s="2" t="n">
-        <v>113.0</v>
+        <v>490.0</v>
       </c>
       <c r="H307" s="2" t="s">
-        <v>1612</v>
+        <v>1610</v>
       </c>
       <c r="I307" s="2" t="n">
-        <v>1303.0</v>
+        <v>1473.0</v>
       </c>
       <c r="J307" s="2" t="s">
-        <v>1614</v>
+        <v>1613</v>
       </c>
       <c r="K307" s="2" t="n">
-        <v>1199.0</v>
+        <v>969.0</v>
       </c>
       <c r="L307" s="2" t="s">
         <v>1612</v>
       </c>
       <c r="M307" s="2" t="n">
-        <v>267.0</v>
+        <v>119.0</v>
       </c>
       <c r="N307" s="2" t="s">
-        <v>1615</v>
+        <v>1614</v>
       </c>
     </row>
     <row r="308">
@@ -28201,43 +28201,43 @@
         <v>307.0</v>
       </c>
       <c r="B308" s="2" t="s">
+        <v>1615</v>
+      </c>
+      <c r="C308" s="2" t="s">
         <v>1616</v>
       </c>
-      <c r="C308" s="2" t="s">
+      <c r="D308" s="2" t="n">
+        <v>734.0</v>
+      </c>
+      <c r="E308" s="2" t="s">
+        <v>1615</v>
+      </c>
+      <c r="F308" s="2" t="n">
+        <v>30.0</v>
+      </c>
+      <c r="G308" s="2" t="n">
+        <v>113.0</v>
+      </c>
+      <c r="H308" s="2" t="s">
+        <v>1615</v>
+      </c>
+      <c r="I308" s="2" t="n">
+        <v>1303.0</v>
+      </c>
+      <c r="J308" s="2" t="s">
         <v>1617</v>
       </c>
-      <c r="D308" s="2" t="n">
-        <v>823.0</v>
-      </c>
-      <c r="E308" s="2" t="s">
+      <c r="K308" s="2" t="n">
+        <v>1199.0</v>
+      </c>
+      <c r="L308" s="2" t="s">
+        <v>1615</v>
+      </c>
+      <c r="M308" s="2" t="n">
+        <v>267.0</v>
+      </c>
+      <c r="N308" s="2" t="s">
         <v>1618</v>
-      </c>
-      <c r="F308" s="2" t="n">
-        <v>10.0</v>
-      </c>
-      <c r="G308" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="H308" s="2" t="s">
-        <v>1616</v>
-      </c>
-      <c r="I308" s="2" t="n">
-        <v>1408.0</v>
-      </c>
-      <c r="J308" s="2" t="s">
-        <v>1619</v>
-      </c>
-      <c r="K308" s="2" t="n">
-        <v>1235.0</v>
-      </c>
-      <c r="L308" s="2" t="s">
-        <v>1620</v>
-      </c>
-      <c r="M308" s="2" t="n">
-        <v>52.0</v>
-      </c>
-      <c r="N308" s="2" t="s">
-        <v>1621</v>
       </c>
     </row>
     <row r="309">
@@ -28245,16 +28245,16 @@
         <v>308.0</v>
       </c>
       <c r="B309" s="2" t="s">
-        <v>1622</v>
+        <v>1619</v>
       </c>
       <c r="C309" s="2" t="s">
-        <v>1623</v>
+        <v>1620</v>
       </c>
       <c r="D309" s="2" t="n">
-        <v>807.0</v>
+        <v>823.0</v>
       </c>
       <c r="E309" s="2" t="s">
-        <v>1624</v>
+        <v>1621</v>
       </c>
       <c r="F309" s="2" t="n">
         <v>10.0</v>
@@ -28263,25 +28263,25 @@
         <v>0.0</v>
       </c>
       <c r="H309" s="2" t="s">
+        <v>1619</v>
+      </c>
+      <c r="I309" s="2" t="n">
+        <v>1408.0</v>
+      </c>
+      <c r="J309" s="2" t="s">
         <v>1622</v>
       </c>
-      <c r="I309" s="2" t="n">
-        <v>1439.0</v>
-      </c>
-      <c r="J309" s="2" t="s">
-        <v>1625</v>
-      </c>
       <c r="K309" s="2" t="n">
-        <v>1103.0</v>
+        <v>1235.0</v>
       </c>
       <c r="L309" s="2" t="s">
-        <v>1622</v>
+        <v>1623</v>
       </c>
       <c r="M309" s="2" t="n">
-        <v>167.0</v>
+        <v>52.0</v>
       </c>
       <c r="N309" s="2" t="s">
-        <v>1626</v>
+        <v>1624</v>
       </c>
     </row>
     <row r="310">
@@ -28289,43 +28289,43 @@
         <v>309.0</v>
       </c>
       <c r="B310" s="2" t="s">
-        <v>1627</v>
+        <v>1625</v>
       </c>
       <c r="C310" s="2" t="s">
-        <v>1627</v>
+        <v>1626</v>
       </c>
       <c r="D310" s="2" t="n">
-        <v>624.0</v>
+        <v>807.0</v>
       </c>
       <c r="E310" s="2" t="s">
         <v>1627</v>
       </c>
       <c r="F310" s="2" t="n">
-        <v>49.0</v>
+        <v>10.0</v>
       </c>
       <c r="G310" s="2" t="n">
-        <v>254.0</v>
+        <v>0.0</v>
       </c>
       <c r="H310" s="2" t="s">
+        <v>1625</v>
+      </c>
+      <c r="I310" s="2" t="n">
+        <v>1439.0</v>
+      </c>
+      <c r="J310" s="2" t="s">
         <v>1628</v>
       </c>
-      <c r="I310" s="2" t="n">
-        <v>1464.0</v>
-      </c>
-      <c r="J310" s="2" t="s">
+      <c r="K310" s="2" t="n">
+        <v>1103.0</v>
+      </c>
+      <c r="L310" s="2" t="s">
+        <v>1625</v>
+      </c>
+      <c r="M310" s="2" t="n">
+        <v>167.0</v>
+      </c>
+      <c r="N310" s="2" t="s">
         <v>1629</v>
-      </c>
-      <c r="K310" s="2" t="n">
-        <v>1058.0</v>
-      </c>
-      <c r="L310" s="2" t="s">
-        <v>1627</v>
-      </c>
-      <c r="M310" s="2" t="n">
-        <v>424.0</v>
-      </c>
-      <c r="N310" s="2" t="s">
-        <v>1630</v>
       </c>
     </row>
     <row r="311">
@@ -28333,16 +28333,16 @@
         <v>310.0</v>
       </c>
       <c r="B311" s="2" t="s">
+        <v>1630</v>
+      </c>
+      <c r="C311" s="2" t="s">
         <v>1631</v>
-      </c>
-      <c r="C311" s="2" t="s">
-        <v>1632</v>
       </c>
       <c r="D311" s="2" t="n">
         <v>703.0</v>
       </c>
       <c r="E311" s="2" t="s">
-        <v>1633</v>
+        <v>1632</v>
       </c>
       <c r="F311" s="2" t="n">
         <v>10.0</v>
@@ -28351,25 +28351,25 @@
         <v>140.0</v>
       </c>
       <c r="H311" s="2" t="s">
-        <v>1634</v>
+        <v>1633</v>
       </c>
       <c r="I311" s="2" t="n">
         <v>1421.0</v>
       </c>
       <c r="J311" s="2" t="s">
-        <v>1634</v>
+        <v>1633</v>
       </c>
       <c r="K311" s="2" t="n">
         <v>1090.0</v>
       </c>
       <c r="L311" s="2" t="s">
-        <v>1633</v>
+        <v>1632</v>
       </c>
       <c r="M311" s="2" t="n">
         <v>427.0</v>
       </c>
       <c r="N311" s="2" t="s">
-        <v>1635</v>
+        <v>1634</v>
       </c>
     </row>
     <row r="312">
@@ -28377,16 +28377,16 @@
         <v>311.0</v>
       </c>
       <c r="B312" s="2" t="s">
+        <v>1635</v>
+      </c>
+      <c r="C312" s="2" t="s">
         <v>1636</v>
-      </c>
-      <c r="C312" s="2" t="s">
-        <v>1637</v>
       </c>
       <c r="D312" s="2" t="n">
         <v>715.0</v>
       </c>
       <c r="E312" s="2" t="s">
-        <v>1638</v>
+        <v>1637</v>
       </c>
       <c r="F312" s="2" t="n">
         <v>10.0</v>
@@ -28395,25 +28395,25 @@
         <v>179.0</v>
       </c>
       <c r="H312" s="2" t="s">
-        <v>1639</v>
+        <v>1638</v>
       </c>
       <c r="I312" s="2" t="n">
         <v>1437.0</v>
       </c>
       <c r="J312" s="2" t="s">
-        <v>1639</v>
+        <v>1638</v>
       </c>
       <c r="K312" s="2" t="n">
         <v>1097.0</v>
       </c>
       <c r="L312" s="2" t="s">
-        <v>1638</v>
+        <v>1637</v>
       </c>
       <c r="M312" s="2" t="n">
         <v>371.0</v>
       </c>
       <c r="N312" s="2" t="s">
-        <v>1640</v>
+        <v>1639</v>
       </c>
     </row>
     <row r="313">
@@ -28421,16 +28421,16 @@
         <v>312.0</v>
       </c>
       <c r="B313" s="2" t="s">
+        <v>1640</v>
+      </c>
+      <c r="C313" s="2" t="s">
         <v>1641</v>
-      </c>
-      <c r="C313" s="2" t="s">
-        <v>1642</v>
       </c>
       <c r="D313" s="2" t="n">
         <v>833.0</v>
       </c>
       <c r="E313" s="2" t="s">
-        <v>1643</v>
+        <v>1642</v>
       </c>
       <c r="F313" s="2" t="n">
         <v>20.0</v>
@@ -28439,25 +28439,25 @@
         <v>105.0</v>
       </c>
       <c r="H313" s="2" t="s">
-        <v>1641</v>
+        <v>1640</v>
       </c>
       <c r="I313" s="2" t="n">
         <v>1472.0</v>
       </c>
       <c r="J313" s="2" t="s">
-        <v>1644</v>
+        <v>1643</v>
       </c>
       <c r="K313" s="2" t="n">
         <v>1012.0</v>
       </c>
       <c r="L313" s="2" t="s">
-        <v>1645</v>
+        <v>1644</v>
       </c>
       <c r="M313" s="2" t="n">
         <v>65.0</v>
       </c>
       <c r="N313" s="2" t="s">
-        <v>1646</v>
+        <v>1645</v>
       </c>
     </row>
     <row r="314">
@@ -28465,16 +28465,16 @@
         <v>313.0</v>
       </c>
       <c r="B314" s="2" t="s">
+        <v>1646</v>
+      </c>
+      <c r="C314" s="2" t="s">
         <v>1647</v>
-      </c>
-      <c r="C314" s="2" t="s">
-        <v>1648</v>
       </c>
       <c r="D314" s="2" t="n">
         <v>609.0</v>
       </c>
       <c r="E314" s="2" t="s">
-        <v>1649</v>
+        <v>1648</v>
       </c>
       <c r="F314" s="2" t="n">
         <v>40.0</v>
@@ -28483,25 +28483,25 @@
         <v>71.0</v>
       </c>
       <c r="H314" s="2" t="s">
-        <v>1650</v>
+        <v>1649</v>
       </c>
       <c r="I314" s="2" t="n">
         <v>1422.0</v>
       </c>
       <c r="J314" s="2" t="s">
-        <v>1651</v>
+        <v>1650</v>
       </c>
       <c r="K314" s="2" t="n">
         <v>1567.0</v>
       </c>
       <c r="L314" s="2" t="s">
-        <v>1649</v>
+        <v>1648</v>
       </c>
       <c r="M314" s="2" t="n">
         <v>170.0</v>
       </c>
       <c r="N314" s="2" t="s">
-        <v>1652</v>
+        <v>1651</v>
       </c>
     </row>
     <row r="315">
@@ -28509,16 +28509,16 @@
         <v>314.0</v>
       </c>
       <c r="B315" s="2" t="s">
+        <v>1652</v>
+      </c>
+      <c r="C315" s="2" t="s">
         <v>1653</v>
-      </c>
-      <c r="C315" s="2" t="s">
-        <v>1654</v>
       </c>
       <c r="D315" s="2" t="n">
         <v>714.0</v>
       </c>
       <c r="E315" s="2" t="s">
-        <v>1655</v>
+        <v>1654</v>
       </c>
       <c r="F315" s="2" t="n">
         <v>30.0</v>
@@ -28527,25 +28527,25 @@
         <v>36.0</v>
       </c>
       <c r="H315" s="2" t="s">
-        <v>1653</v>
+        <v>1652</v>
       </c>
       <c r="I315" s="2" t="n">
         <v>1424.0</v>
       </c>
       <c r="J315" s="2" t="s">
-        <v>1656</v>
+        <v>1655</v>
       </c>
       <c r="K315" s="2" t="n">
         <v>1232.0</v>
       </c>
       <c r="L315" s="2" t="s">
-        <v>1657</v>
+        <v>1656</v>
       </c>
       <c r="M315" s="2" t="n">
         <v>202.0</v>
       </c>
       <c r="N315" s="2" t="s">
-        <v>1658</v>
+        <v>1657</v>
       </c>
     </row>
     <row r="316">
@@ -28553,16 +28553,16 @@
         <v>315.0</v>
       </c>
       <c r="B316" s="2" t="s">
+        <v>1658</v>
+      </c>
+      <c r="C316" s="2" t="s">
         <v>1659</v>
-      </c>
-      <c r="C316" s="2" t="s">
-        <v>1660</v>
       </c>
       <c r="D316" s="2" t="n">
         <v>800.0</v>
       </c>
       <c r="E316" s="2" t="s">
-        <v>1660</v>
+        <v>1659</v>
       </c>
       <c r="F316" s="2" t="n">
         <v>60.0</v>
@@ -28571,25 +28571,25 @@
         <v>0.0</v>
       </c>
       <c r="H316" s="2" t="s">
-        <v>1660</v>
+        <v>1659</v>
       </c>
       <c r="I316" s="2" t="n">
         <v>1256.0</v>
       </c>
       <c r="J316" s="2" t="s">
-        <v>1661</v>
+        <v>1660</v>
       </c>
       <c r="K316" s="2" t="n">
         <v>1118.0</v>
       </c>
       <c r="L316" s="2" t="s">
-        <v>1660</v>
+        <v>1659</v>
       </c>
       <c r="M316" s="2" t="n">
         <v>35.0</v>
       </c>
       <c r="N316" s="2" t="s">
-        <v>1662</v>
+        <v>1661</v>
       </c>
     </row>
     <row r="317">
@@ -28597,43 +28597,43 @@
         <v>316.0</v>
       </c>
       <c r="B317" s="2" t="s">
+        <v>1662</v>
+      </c>
+      <c r="C317" s="2" t="s">
         <v>1663</v>
       </c>
-      <c r="C317" s="2" t="s">
+      <c r="D317" s="2" t="n">
+        <v>744.0</v>
+      </c>
+      <c r="E317" s="2" t="s">
         <v>1664</v>
       </c>
-      <c r="D317" s="2" t="n">
-        <v>589.0</v>
-      </c>
-      <c r="E317" s="2" t="s">
+      <c r="F317" s="2" t="n">
+        <v>40.0</v>
+      </c>
+      <c r="G317" s="2" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="H317" s="2" t="s">
         <v>1665</v>
       </c>
-      <c r="F317" s="2" t="n">
-        <v>29.0</v>
-      </c>
-      <c r="G317" s="2" t="n">
-        <v>222.0</v>
-      </c>
-      <c r="H317" s="2" t="s">
+      <c r="I317" s="2" t="n">
+        <v>1409.0</v>
+      </c>
+      <c r="J317" s="2" t="s">
+        <v>1665</v>
+      </c>
+      <c r="K317" s="2" t="n">
+        <v>1087.0</v>
+      </c>
+      <c r="L317" s="2" t="s">
+        <v>1664</v>
+      </c>
+      <c r="M317" s="2" t="n">
+        <v>192.0</v>
+      </c>
+      <c r="N317" s="2" t="s">
         <v>1666</v>
-      </c>
-      <c r="I317" s="2" t="n">
-        <v>1307.0</v>
-      </c>
-      <c r="J317" s="2" t="s">
-        <v>1667</v>
-      </c>
-      <c r="K317" s="2" t="n">
-        <v>998.0</v>
-      </c>
-      <c r="L317" s="2" t="s">
-        <v>1665</v>
-      </c>
-      <c r="M317" s="2" t="n">
-        <v>744.0</v>
-      </c>
-      <c r="N317" s="2" t="s">
-        <v>1668</v>
       </c>
     </row>
     <row r="318">
@@ -28641,43 +28641,43 @@
         <v>317.0</v>
       </c>
       <c r="B318" s="2" t="s">
+        <v>1667</v>
+      </c>
+      <c r="C318" s="2" t="s">
+        <v>1668</v>
+      </c>
+      <c r="D318" s="2" t="n">
+        <v>589.0</v>
+      </c>
+      <c r="E318" s="2" t="s">
         <v>1669</v>
       </c>
-      <c r="C318" s="2" t="s">
+      <c r="F318" s="2" t="n">
+        <v>29.0</v>
+      </c>
+      <c r="G318" s="2" t="n">
+        <v>222.0</v>
+      </c>
+      <c r="H318" s="2" t="s">
         <v>1670</v>
       </c>
-      <c r="D318" s="2" t="n">
+      <c r="I318" s="2" t="n">
+        <v>1307.0</v>
+      </c>
+      <c r="J318" s="2" t="s">
+        <v>1671</v>
+      </c>
+      <c r="K318" s="2" t="n">
+        <v>998.0</v>
+      </c>
+      <c r="L318" s="2" t="s">
+        <v>1669</v>
+      </c>
+      <c r="M318" s="2" t="n">
         <v>744.0</v>
       </c>
-      <c r="E318" s="2" t="s">
-        <v>1671</v>
-      </c>
-      <c r="F318" s="2" t="n">
-        <v>40.0</v>
-      </c>
-      <c r="G318" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="H318" s="2" t="s">
+      <c r="N318" s="2" t="s">
         <v>1672</v>
-      </c>
-      <c r="I318" s="2" t="n">
-        <v>1409.0</v>
-      </c>
-      <c r="J318" s="2" t="s">
-        <v>1672</v>
-      </c>
-      <c r="K318" s="2" t="n">
-        <v>1087.0</v>
-      </c>
-      <c r="L318" s="2" t="s">
-        <v>1671</v>
-      </c>
-      <c r="M318" s="2" t="n">
-        <v>192.0</v>
-      </c>
-      <c r="N318" s="2" t="s">
-        <v>1668</v>
       </c>
     </row>
     <row r="319">
@@ -30856,7 +30856,7 @@
         <v>30.0</v>
       </c>
       <c r="G368" s="2" t="n">
-        <v>59.0</v>
+        <v>61.0</v>
       </c>
       <c r="H368" s="2" t="s">
         <v>1931</v>
@@ -31296,7 +31296,7 @@
         <v>10.0</v>
       </c>
       <c r="G378" s="2" t="n">
-        <v>344.0</v>
+        <v>346.0</v>
       </c>
       <c r="H378" s="2" t="s">
         <v>1986</v>
@@ -38820,7 +38820,7 @@
         <v>60.0</v>
       </c>
       <c r="G549" s="2" t="n">
-        <v>21.0</v>
+        <v>23.0</v>
       </c>
       <c r="H549" s="2" t="s">
         <v>2861</v>

</xml_diff>